<commit_message>
Add functionality to insert internal comments and update Excel processing
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -719,7 +719,11 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>REDUTOR NETZSCH-SEW PARA BOMBA: NM063B/CÓDIGO NETZSCH: NS 87-AMS160/          REDUÇÃO: I=5,30/FORMA CONSTRUT: M1/CÓDIGO SEW: RF87 AMS160/                   PARA MOTOR: CARCAÇA 160/DESENHO SEW: NÃO INFORMADO/</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
@@ -748,7 +752,11 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>MOTOR SEW MODELO: DRN80MP4/FF/FORMA CONSTR: V1/POS. CAIXA LIG: R (0°/X)/      CARCAÇA: 80M/NRº DE FASES: 3/POTÊNCIA: 1,10KW/FREQUENCIA: 60HZ/               EFICIENCIA: ALTO RENDIMENTO PREMIUM (IR3)/REFRIGERAÇÃO: TFVE/                 NÚMERO DE POLOS: 4/GRAU PROTEÇÃO: IPW-55/NORMA: IEC/FLANGE: FF165/            TENSÃO: 230/460V/ISOLAMENTO: F/REGIME SERVIÇO: S1/                            CARAC. ESPECIAL: FATOR DE SERVIÇO 1,25,ENSAIO DE ROTINA SEM INSPETOR - TODO LOTE,RESISTÊNCIA DE AQUECIMENTO MONFÁSICO 200 A 240V,PLACA DE BORNES,TERMINAL DE ATERRAMENTO NA CARCAÇA/</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
@@ -777,7 +785,11 @@
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>MOTOR SEW MODELO: DRN132SP4/FF/FORMA CONSTR: V1/POS. CAIXA LIG: R (0°/X)/     CARCAÇA: 132S/NRº DE FASES: 3/POTÊNCIA: 7,50KW/FREQUENCIA: 60HZ/              EFICIENCIA: ALTO RENDIMENTO PREMIUM (IR3)/REFRIGERAÇÃO: TFVE/                 NÚMERO DE POLOS: 4/GRAU PROTEÇÃO: IPW-55/NORMA: IEC/FLANGE: FF265/            TENSÃO: 230/460V/ISOLAMENTO: F/REGIME SERVIÇO: S1/                            CARAC. ESPECIAL: FATOR DE SERVIÇO 1,25,ENSAIO DE ROTINA SEM INSPETOR - TODO LOTE,RESISTÊNCIA DE AQUECIMENTO MONFÁSICO 200 A 240V,PLACA DE BORNES,TERMINAL DE ATERRAMENTO NA CARCAÇA/</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -806,7 +818,11 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR SEW PERIPRO MODELO BOMBA: 04_0.01/MODELO: WAF10 DR2S56MP4/        REDUÇÃO: I=39,00/ROTAÇÃO: N=41RPM/                                            FORMA CONSTRUT.: M4A-L (CAIXA DE LIGAÇÃO 180°/X)/POTÊNCIA: 0,15KW/            FREQUÊNCIA: 60HZ/EFICIENCIA: STANDARD (IR1)/TENSÃO: 220/380V/                 GRAU DE PROTEÇÃO IP55/POLOS: 4/REFRIGERAÇÃO: TFVE/ISOLAMENTO: F/NORMA ABNT/   FLANGE: EF W003/06/PONTA DE EIXO: Ø16mm/                                      CARAC. ESPECIAL: COM COBERTURA DE PROTEÇÃO DO EIXO,EIXO VEIO OCO/</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -835,7 +851,11 @@
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM045B/CÓDIGO NETZSCH: NS57/              REDUÇÃO: I=17,57/ROTAÇÃO: N=100RPM/FORMA CONSTR: M2A/POTÊNCIA MOTOR: 3,70KW/  FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVF/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KF57 DRN90LP4/V/                                    CARAC. ESPECIAL: VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
@@ -864,7 +884,11 @@
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM063B/CÓDIGO NETZSCH: NS67/              REDUÇÃO: I=7,28/ROTAÇÃO: N=242RPM/FORMA CONSTR: M4A/POTÊNCIA MOTOR: 5,50KW/   FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVF/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KF67 DRN112MP4/V/                                   CARAC. ESPECIAL: VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -893,7 +917,11 @@
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR SEW PERIPRO MODELO BOMBA: 10_5.1/MODELO: RF77 DRN100L4/           REDUÇÃO: I=36,83/ROTAÇÃO: N=40RPM/POTÊNCIA: 3,00KW/FREQUÊNCIA: 50HZ/          EFICIENCIA: ALTO RENDIMENTO PREMIUM (IR3)/TENSÃO: 220/380V/                   GRAU DE PROTEÇÃO IP55/POLOS: 4/REFRIGERAÇÃO: TFVE/ISOLAMENTO: F/NORMA IEC/    FLANGE: Ø250mm/PONTA DE EIXO: 35X70MM/</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -922,7 +950,11 @@
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>MOTOR ELÉTRICO TRIFÁSICO PMM (IMÃS PERMANENTES)W22,IE4; FORMA CONSTRUTIVA V1T; TORQUE CONSTANTE 1196NM (882 ft.lb); 16 POLOS; ROTAÇÃO NOMINAL 375RPM; POTÊNCIA 47KW (63,5HP); TEFC; IP-55; FREQUÊNCIA 4 ATÉ 50 HZ; TENSÃO 380V C/ 6 TERMINAIS; CORRENTE 82A; ISOLAMENTO CLASSE F; FATOR DE SERVIÇO: 1,00; CARCAÇA 315S/M; PLANO DE PINTURA 202P; COR 091A.3145; COM PLACA DE BORNES; FLANGE FF-600; COM FURO PASSANTE NO EIXO Ø60MM; COM PONTA DE EIXO NA PARTE SUPERIOR; SAÍDA DE CABOS DA CAIXA DE LIGAÇÃO PRINCIPAL VOLTADA PARA EIXO; COM CERTIFICAÇÃO ATEX/IECEX, ZONA 2, GRUPO IIC, T3; ESPECIAL PARA APLICAÇÃO EM CABEÇOTES DE ACIONAMENTOS PCP. PLAQUETA DO MOTOR COM VALOR DE TORQUE EXPRESSA EM FT.LB E POTÊNCIA EM HP. CONFORME FOLHA DE DADOS NR...., ITEM FORNECEDOR: 17464798.</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -951,7 +983,11 @@
       <c r="P12" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1"/NORMA: ASME B16.5/                 CLASSE PRESSÃO: 600#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/                    CERTIFICADOS: CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
@@ -980,7 +1016,11 @@
       <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
@@ -1009,7 +1049,11 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 12"/NORMA: ASME B16.5/            CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL/                                             CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
@@ -1038,7 +1082,11 @@
       <c r="P15" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 10"/NORMA: ASME B16.5/            CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL/                                             CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
@@ -1067,7 +1115,11 @@
       <c r="P16" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/                    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
@@ -1096,7 +1148,11 @@
       <c r="P17" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1"/NORMA: ASME B16.5/                 CLASSE PRESSÃO: 600#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
@@ -1125,7 +1181,11 @@
       <c r="P18" t="inlineStr"/>
       <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1"/NORMA: ASME B16.5/                 CLASSE PRESSÃO: 600#/SCHEDULE: SCH40/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
@@ -1154,7 +1214,11 @@
       <c r="P19" t="inlineStr"/>
       <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1/2"/NORMA: ASME B16.5/               CLASSE PRESSÃO: 150#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A182 GR F316L/              FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
@@ -1183,7 +1247,11 @@
       <c r="P20" t="inlineStr"/>
       <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1.1/2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A182 GR F304L/              FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
@@ -1212,7 +1280,11 @@
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1/2"/NORMA: ASME B16.5/               CLASSE PRESSÃO: 150#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A182 GR F304L/              FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
@@ -1241,7 +1313,11 @@
       <c r="P22" t="inlineStr"/>
       <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
@@ -1270,7 +1346,11 @@
       <c r="P23" t="inlineStr"/>
       <c r="Q23" t="inlineStr"/>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL/                                             CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
@@ -1299,7 +1379,11 @@
       <c r="P24" t="inlineStr"/>
       <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr"/>
-      <c r="S24" t="inlineStr"/>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 3"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS,PROIBIDO OS SEGUINTES PAÍSES DE ORIGEM:,ESPANHA, PORTUGAL, TAIWAN, CHINA, LESTE EUROPEU, ÁFRICA, AMÉRICA CENTRAL E DO SUL, LAOS, C/</t>
+        </is>
+      </c>
       <c r="T24" t="inlineStr"/>
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
@@ -1328,7 +1412,11 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1/2"/NORMA: ASME B16.5/               CLASSE PRESSÃO: 300#/SCHEDULE: SCH40/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/                    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS,MATERIAL CONFORME NORMA NACE MR-0175 (REFERENCIADA NO CERTIFICADO),MATERIAIS COM CERTIFICADO DE ORIGEM DA EUROPA E/OU ESTADOS UNIDOS/</t>
+        </is>
+      </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
@@ -1357,7 +1445,11 @@
       <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1"/NORMA: ASME B16.5/                 CLASSE PRESSÃO: 300#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO NACE MR0175/ISO 15156/</t>
+        </is>
+      </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
@@ -1386,7 +1478,11 @@
       <c r="P27" t="inlineStr"/>
       <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 12"/NORMA: ASME B16.5/                CLASSE PRESSÃO: 300#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS,MATERIAL CONFORME NORMA NACE MR-0175 (REFERENCIADA NO CERTIFICADO),MATERIAIS COM CERTIFICADO DE ORIGEM DA EUROPA E/OU ESTADOS UNIDOS/</t>
+        </is>
+      </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
@@ -1415,7 +1511,11 @@
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 3"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: DUPLEX UNS S31803/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
@@ -1444,7 +1544,11 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1.1/2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: DUPLEX UNS S31803/               FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
@@ -1473,7 +1577,11 @@
       <c r="P30" t="inlineStr"/>
       <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 8"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
@@ -1502,7 +1610,11 @@
       <c r="P31" t="inlineStr"/>
       <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1.1/2"/NORMA: ASME B16.5/         CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
@@ -1531,7 +1643,11 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 3/4"/NORMA: ASME B16.5/           CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
@@ -1560,7 +1676,11 @@
       <c r="P33" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1.1/2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A182 GR F316/               FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
@@ -1589,7 +1709,11 @@
       <c r="P34" t="inlineStr"/>
       <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1.1/2"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/SCHEDULE: SCH40/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A182 GR F316/               FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS,PROIBIDO OS SEGUINTES PAÍSES DE ORIGEM: CHINA E ESTADOS UNIDOS./</t>
+        </is>
+      </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
@@ -1618,7 +1742,11 @@
       <c r="P35" t="inlineStr"/>
       <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1.1/2"/NORMA: ASME B16.5/         CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
@@ -1647,7 +1775,11 @@
       <c r="P36" t="inlineStr"/>
       <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 6"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
       <c r="V36" t="inlineStr"/>
@@ -1676,7 +1808,11 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 5"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.,CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
@@ -1705,7 +1841,11 @@
       <c r="P38" t="inlineStr"/>
       <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>MOTOR SEW MODELO: DRN132M4/FE/FORMA CONSTR: B35/POS. CAIXA LIG: T (270°/X)/   CARCAÇA: 132M/NRº DE FASES: 3/POTÊNCIA: 7,50KW/FREQUENCIA: 60HZ/              EFICIENCIA: ALTO RENDIMENTO PREMIUM (IR3)/REFRIGERAÇÃO: TFVE/                 NÚMERO DE POLOS: 4/GRAU PROTEÇÃO: IP55/NORMA: ABNT/FLANGE: FF265/             TENSÃO: 220/380V COM 06 TERMINAIS/ISOLAMENTO: F/REGIME SERVIÇO: S1/           CARAC. ESPECIAL: ENSAIO DE TIPO SEM INSPETOR - TODO LOTE,MOTOR C/ 2 FITAS DE AQUECIMENTO AC 230V, LADO A+B/</t>
+        </is>
+      </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="inlineStr"/>
@@ -1734,7 +1874,11 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1/2"/NORMA: ASME B16.5/           CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: ITEM RASTREÁVEL,COM CLASSE DE PRESSÃO SINETADO NO FLANGE/    CERTIFICADOS: CERTIFICADO DE MATERIAIS CONFORME EN 10204-3./</t>
+        </is>
+      </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
@@ -1763,7 +1907,11 @@
       <c r="P40" t="inlineStr"/>
       <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 8"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F304/FABRI. OU COMP.: COMPRADO/</t>
+        </is>
+      </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
@@ -1792,7 +1940,11 @@
       <c r="P41" t="inlineStr"/>
       <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 4"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: FF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F304/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
@@ -1821,7 +1973,11 @@
       <c r="P42" t="inlineStr"/>
       <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 3"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 150#/FACE: FF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F304/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
@@ -1850,7 +2006,11 @@
       <c r="P43" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 14"/NORMA: ASME B16.5/            CLASSE PRESSÃO: 150#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316/FABRI. OU COMP.: COMPRADO/</t>
+        </is>
+      </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
@@ -1879,7 +2039,11 @@
       <c r="P44" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 6"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316L/FABRI. OU COMP.: COMPRADO/                       CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr"/>
@@ -1908,7 +2072,11 @@
       <c r="P45" t="inlineStr"/>
       <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1.1/2"/NORMA: ASME B16.5/         CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316L/FABRI. OU COMP.: COMPRADO/</t>
+        </is>
+      </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
@@ -1937,7 +2105,11 @@
       <c r="P46" t="inlineStr"/>
       <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1/2"/NORMA: ASME B16.5/               CLASSE PRESSÃO: 150#/SCHEDULE: SCH40/FACE: RF/ACABAM. FACE: LISO/             MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/                                CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
@@ -1966,7 +2138,11 @@
       <c r="P47" t="inlineStr"/>
       <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 14"/NORMA: ASME B16.5/                CLASSE PRESSÃO: 150#/SCHEDULE: SCH40/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/                    CERTIFICADOS: CERTIFICADO COM ANÁLISE QUÍMICA E PROPRIEDADES MECÂNICAS/</t>
+        </is>
+      </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
@@ -1995,7 +2171,11 @@
       <c r="P48" t="inlineStr"/>
       <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr"/>
-      <c r="S48" t="inlineStr"/>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 1"/NORMA: ASME B16.5/             CLASSE PRESSÃO: 300#/FACE: RF/ACABAM. FACE: MSS SP-6 STD-ESPIRAL/             MATERIAL: ASTM A182 GR F316/FABRI. OU COMP.: COMPRADO/                        CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr"/>
@@ -2024,7 +2204,11 @@
       <c r="P49" t="inlineStr"/>
       <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: WN - WELDING NECK/TAMANHO: 1/2"/NORMA: ASME B16.5/               CLASSE PRESSÃO: 600#/SCHEDULE: SCH80/FACE: RF/                                ACABAM. FACE: MSS SP-6 STD-ESPIRAL/MATERIAL: ASTM A105/                       FABRI. OU COMP.: COMPRADO/                                                    CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
@@ -2053,7 +2237,11 @@
       <c r="P50" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>REDUTOR NETZSCH-SEW PARA BOMBA: NM031B/CÓDIGO NETZSCH: NS 27-AD2/             REDUÇÃO: I=9,41/FORMA CONSTRUT: M1/CÓDIGO SEW: RF27 AD2/</t>
+        </is>
+      </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
@@ -2082,7 +2270,11 @@
       <c r="P51" t="inlineStr"/>
       <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr"/>
-      <c r="S51" t="inlineStr"/>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM038B/CÓDIGO NETZSCH: NS37/              REDUÇÃO: I=10,49/ROTAÇÃO: N=167RPM/FORMA CONSTR: M4A/POTÊNCIA MOTOR: 2,20KW/  FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVF/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KAF37 DRN90LP4/V/                                   CARAC. ESPECIAL: VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+        </is>
+      </c>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr"/>
@@ -2111,7 +2303,11 @@
       <c r="P52" t="inlineStr"/>
       <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr"/>
-      <c r="S52" t="inlineStr"/>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM031B/CÓDIGO NETZSCH: NS37/              REDUÇÃO: I=8,91/ROTAÇÃO: N=197RPM/FORMA CONSTR: M4A/POTÊNCIA MOTOR: 1,50KW/   FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVF/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KF37 DRN90SP4/V/                                    CARAC. ESPECIAL: VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+        </is>
+      </c>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
@@ -2140,7 +2336,11 @@
       <c r="P53" t="inlineStr"/>
       <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>FLANGE TIPO: SOW - SLIP ON WELDING/TAMANHO: 10"/NORMA: ASME B16.5/            CLASSE PRESSÃO: 150#/FACE: FF/MATERIAL: ASTM A105/FABRI. OU COMP.: COMPRADO/  CARAC. ESPECIAL: COM CLASSE DE PRESSÃO SINETADO NO FLANGE/</t>
+        </is>
+      </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
@@ -2169,7 +2369,11 @@
       <c r="P54" t="inlineStr"/>
       <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr"/>
-      <c r="S54" t="inlineStr"/>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>ACOPLADOR CAM-LOK CI BRONZE HPF ROSCA FEMEA NPT 64 4"" - B0008- 11810017 0064</t>
+        </is>
+      </c>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr"/>
@@ -2198,7 +2402,11 @@
       <c r="P55" t="inlineStr"/>
       <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr"/>
-      <c r="S55" t="inlineStr"/>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM011B/CÓDIGO NETZSCH: NSF17/             REDUÇÃO: I=6,15/ROTAÇÃO: N=281RPM/FORMA CONSTR: M1/POTÊNCIA MOTOR: 0,37KW/    FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVE/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: R17F DRN71M4/DESENHO SEW: 415994608-800/</t>
+        </is>
+      </c>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr"/>
@@ -2227,7 +2435,11 @@
       <c r="P56" t="inlineStr"/>
       <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr"/>
-      <c r="S56" t="inlineStr"/>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR SEW PERIPRO MODELO BOMBA: 10_0.1/MODELO: R27F DRN71MS4/V/         REDUÇÃO: I=74,11/ROTAÇÃO: N=23RPM/POTÊNCIA: 0,25KW/FREQUÊNCIA: 60HZ/          EFICIENCIA: ALTO RENDIMENTO PREMIUM (IR3)/TENSÃO: 220/380/440/760V/           GRAU DE PROTEÇÃO IP55/POLOS: 4/REFRIGERAÇÃO: TFVF/ISOLAMENTO: F/NORMA ABNT/   FLANGE: Ø120mm/PONTA DE EIXO: 18X50MM/                                        CARAC. ESPECIAL: VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+        </is>
+      </c>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
@@ -2256,7 +2468,11 @@
       <c r="P57" t="inlineStr"/>
       <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr"/>
-      <c r="S57" t="inlineStr"/>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM076B/CÓDIGO NETZSCH: NS77/              REDUÇÃO: I=10,84/ROTAÇÃO: N=325RPM/FORMA CONSTR: M1A/POTÊNCIA MOTOR: 11,00KW/ FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVE/NRº PÓLOS: 2/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KF77 DRN132MEP2/</t>
+        </is>
+      </c>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr"/>
@@ -2285,7 +2501,11 @@
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr"/>
-      <c r="S58" t="inlineStr"/>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM063B/CÓDIGO NETZSCH: NS67/              REDUÇÃO: I=5,20/ROTAÇÃO: N=341RPM/FORMA CONSTR: M4A/POTÊNCIA MOTOR: 9,20KW/   FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVE/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: KF67 DRN132MP4/                                     CARAC. ESPECIAL: ÓLEO SINTÉTICO,DUPLA VEDAÇÃO NO EIXO DE SAÍDA,EIXO DE SAÍDA: 40X80mm,TANQUE DE EXPANSÃO,RESPIRO ESPECIAL/</t>
+        </is>
+      </c>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr"/>
@@ -2314,7 +2534,11 @@
       <c r="P59" t="inlineStr"/>
       <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr"/>
-      <c r="S59" t="inlineStr"/>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>BOCA DE RECALQUE  NM105-14 MATERIAL AISI 304L FLANGE CFE ANSI B16.5 150PSI 6" FF.</t>
+        </is>
+      </c>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr"/>
@@ -2343,7 +2567,11 @@
       <c r="P60" t="inlineStr"/>
       <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr"/>
-      <c r="S60" t="inlineStr"/>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>BASE MÓVEL PARA BOMBA NM031BH01L06-/02S12- MATERIAL: AISI 304; ACABAMENTO JATEADO; APTA PARA:  -MOTOREDUTOR NS 27; ESPECIAL: BASE COM 3 RODIZIOS; OBS.: FORNECER BASE SEM USINAGEM, COM FURAÇÃO E SOLDA COMPLETA.</t>
+        </is>
+      </c>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr"/>
@@ -2372,7 +2600,11 @@
       <c r="P61" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr"/>
-      <c r="S61" t="inlineStr"/>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM076/ESTÁGIOS: 06/GEOMETRIA: S/BORRACHA: NEMOLAST S459/    MATERIAL TUBO: 1020/TERMOSTATO: STP3/MEDIDA Lst: 101,50mm/MEDIDA A: M8/       MEDIDA B: 10,30mm/MEDIDA t: 40,00mm/                                          CARAC. ESPECIAL: SOLDADO,NH - NÃO HIGIÊNICO (NÃO INDICADO PARA APLICAÇÕES HIGIÊNICAS)/</t>
+        </is>
+      </c>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr"/>
@@ -2401,7 +2633,11 @@
       <c r="P62" t="inlineStr"/>
       <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr"/>
-      <c r="S62" t="inlineStr"/>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM038/ESTÁGIOS: 04/GEOMETRIA: S/BORRACHA: EP/               MATERIAL: 1020/MATERIAL TELA: TELA 1008/10/</t>
+        </is>
+      </c>
       <c r="T62" t="inlineStr"/>
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr"/>
@@ -2430,7 +2666,11 @@
       <c r="P63" t="inlineStr"/>
       <c r="Q63" t="inlineStr"/>
       <c r="R63" t="inlineStr"/>
-      <c r="S63" t="inlineStr"/>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>APERTA SELO MECANICO  NM053B-(P) MATERIAL  AISI 316    P/SELO M74-D C/ QUENCH G=1/4"NPT</t>
+        </is>
+      </c>
       <c r="T63" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr"/>
@@ -2459,7 +2699,11 @@
       <c r="P64" t="inlineStr"/>
       <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr"/>
-      <c r="S64" t="inlineStr"/>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM045/ESTÁGIOS: 12/GEOMETRIA: S/BORRACHA: NEMOLAST S61M/    MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T64" t="inlineStr"/>
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
@@ -2488,7 +2732,11 @@
       <c r="P65" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr"/>
-      <c r="S65" t="inlineStr"/>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM063/ESTÁGIOS: 01/GEOMETRIA: P/BORRACHA: NEMOLAST S41/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T65" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
@@ -2517,7 +2765,11 @@
       <c r="P66" t="inlineStr"/>
       <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr"/>
-      <c r="S66" t="inlineStr"/>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>FLANGE DIANTEIRA PRÉ-USINADO  MODELO: 3NS-/80H13-/MATERIAL: ASTM A-36/        MEDIDA A: 418,00mm/MEDIDA B: 310,00mm/MEDIDA C: 80,00mm/MEDIDA D: 371,00mm/   MEDIDA D1: D1=493,00/MEDIDA E: 367,00mm/MEDIDA F: 10,00mm/MEDIDA G: 50,00mm/  MEDIDA H: 520,00mm/                                                           MEDIDA X°: USINAR CFE DETALHE X, PARA ESPESSURA DO TUBO &gt;22mm/                MEDIDA Y°: Y°=30°/MEDIDA R: R=5,00/MEDIDA R1: R1=5,00/</t>
+        </is>
+      </c>
       <c r="T66" t="inlineStr"/>
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
@@ -2546,7 +2798,11 @@
       <c r="P67" t="inlineStr"/>
       <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr"/>
-      <c r="S67" t="inlineStr"/>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>ANEL INTERMEDIÁRIO MODELO: 3NS-/80H2-/MATERIAL: ASTM A-36/                    MEDIDA A: A=120,00mm/MEDIDA B: B=85,00/MEDIDA C: C=15,00/MEDIDA D: D=5,00/    MEDIDA X°: X°=45°/MEDIDA E: E=5,00/MEDIDA Y°: Y°=45°/</t>
+        </is>
+      </c>
       <c r="T67" t="inlineStr"/>
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
@@ -2575,7 +2831,11 @@
       <c r="P68" t="inlineStr"/>
       <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr"/>
-      <c r="S68" t="inlineStr"/>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>CORPO PCP SOLDADO PARA CABEÇOTE GH20-H  MATERIAL: A-36  *TESTES/CERTIFICADOS EXIGIDOS: *TESTE DE PARTÍCULA MAGNÉTICA E CERTIFICADOS 100% NOS OLHAIS DE IÇAMENTO</t>
+        </is>
+      </c>
       <c r="T68" t="inlineStr"/>
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr"/>
@@ -2604,7 +2864,11 @@
       <c r="P69" t="inlineStr"/>
       <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr"/>
-      <c r="S69" t="inlineStr"/>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>CORPO PCP USINADO PARA CABEÇOTE GH20-H  MATERIAL: A-36</t>
+        </is>
+      </c>
       <c r="T69" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
@@ -2633,7 +2897,11 @@
       <c r="P70" t="inlineStr"/>
       <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr"/>
-      <c r="S70" t="inlineStr"/>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM125/ESTÁGIOS: 02/GEOMETRIA: S/BORRACHA: NEMOLAST S61M/    MATERIAL: 1020/                                                               CARAC. ESPECIAL: COM CHANFRO S NAS DUAS EXTREMIDADES DO ESTATOR/</t>
+        </is>
+      </c>
       <c r="T70" t="inlineStr"/>
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
@@ -2662,7 +2930,11 @@
       <c r="P71" t="inlineStr"/>
       <c r="Q71" t="inlineStr"/>
       <c r="R71" t="inlineStr"/>
-      <c r="S71" t="inlineStr"/>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>GARGANTA DN16" - SCH40 MATERIAL: ASTM A106.</t>
+        </is>
+      </c>
       <c r="T71" t="inlineStr"/>
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr"/>
@@ -2691,7 +2963,11 @@
       <c r="P72" t="inlineStr"/>
       <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr"/>
-      <c r="S72" t="inlineStr"/>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>GARGANTA DN10" - SCH40 MATERIAL: ASTM A106.</t>
+        </is>
+      </c>
       <c r="T72" t="inlineStr"/>
       <c r="U72" t="inlineStr"/>
       <c r="V72" t="inlineStr"/>
@@ -2720,7 +2996,11 @@
       <c r="P73" t="inlineStr"/>
       <c r="Q73" t="inlineStr"/>
       <c r="R73" t="inlineStr"/>
-      <c r="S73" t="inlineStr"/>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>GARGANTA DN4" - SCH40 MATERIAL: ASTM A106.</t>
+        </is>
+      </c>
       <c r="T73" t="inlineStr"/>
       <c r="U73" t="inlineStr"/>
       <c r="V73" t="inlineStr"/>
@@ -2749,7 +3029,11 @@
       <c r="P74" t="inlineStr"/>
       <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr"/>
-      <c r="S74" t="inlineStr"/>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>GARGANTA DN8" - SCH40 MATERIAL: ASTM A106.</t>
+        </is>
+      </c>
       <c r="T74" t="inlineStr"/>
       <c r="U74" t="inlineStr"/>
       <c r="V74" t="inlineStr"/>
@@ -2778,7 +3062,11 @@
       <c r="P75" t="inlineStr"/>
       <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr"/>
-      <c r="S75" t="inlineStr"/>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM031-12. MATERIAL  AISI 316. FLANGE CFE ANSI B16.5 150PSI 2" RF. G= 3/4" NPT. ESPECIAL: ALTURA DA FACE DA FLANGE ATÉ A LINHA DE CENTRO DE 93MM.</t>
+        </is>
+      </c>
       <c r="T75" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
       <c r="V75" t="inlineStr"/>
@@ -2807,7 +3095,11 @@
       <c r="P76" t="inlineStr"/>
       <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr"/>
-      <c r="S76" t="inlineStr"/>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>GARGANTA DN12" - SCH40 MATERIAL: ASTM A106.</t>
+        </is>
+      </c>
       <c r="T76" t="inlineStr"/>
       <c r="U76" t="inlineStr"/>
       <c r="V76" t="inlineStr"/>
@@ -2836,7 +3128,11 @@
       <c r="P77" t="inlineStr"/>
       <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr"/>
-      <c r="S77" t="inlineStr"/>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>GARGANTA DN16" - SCH40 MATERIAL: ASTM A106. CARAC. ESPECIAL: ITEM RASTREÁVEL,FORNECER CERTIFICADO DE COMPOSIÇÃO QUÍMICA E PROPRIEDADES MECÂNICAS CONFORME EN 10204-3.1.</t>
+        </is>
+      </c>
       <c r="T77" t="inlineStr"/>
       <c r="U77" t="inlineStr"/>
       <c r="V77" t="inlineStr"/>
@@ -2865,7 +3161,11 @@
       <c r="P78" t="inlineStr"/>
       <c r="Q78" t="inlineStr"/>
       <c r="R78" t="inlineStr"/>
-      <c r="S78" t="inlineStr"/>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>GARGANTA DN10" - SCH80 MATERIAL: ASTM A106. CARAC. ESPECIAL: ITEM RASTREÁVEL,FORNECER CERTIFICADO DE COMPOSIÇÃO QUÍMICA E PROPRIEDADES MECÂNICAS CONFORME EN 10204-3.1.</t>
+        </is>
+      </c>
       <c r="T78" t="inlineStr"/>
       <c r="U78" t="inlineStr"/>
       <c r="V78" t="inlineStr"/>
@@ -2894,7 +3194,11 @@
       <c r="P79" t="inlineStr"/>
       <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr"/>
-      <c r="S79" t="inlineStr"/>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>ADAPTADOR HN5 MATERIAL SAE 1045</t>
+        </is>
+      </c>
       <c r="T79" t="inlineStr"/>
       <c r="U79" t="inlineStr"/>
       <c r="V79" t="inlineStr"/>
@@ -2923,7 +3227,11 @@
       <c r="P80" t="inlineStr"/>
       <c r="Q80" t="inlineStr"/>
       <c r="R80" t="inlineStr"/>
-      <c r="S80" t="inlineStr"/>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>DISPLAY/STAND COM ROTOR, PARA TRITURADOR N.MAC 50C (STAND PARA BOMBAS DE SHOW-ROOM E FEIRAS) COM PEDESTAL NO CHÃO + ROTOR + PLATAFORMA DE MADEIRA PARA O TRITURADOR  ACABAMENTO SUPERFICIAL: *BUCHA DO ROTOR/ROTOR/FLANGE DE SUSTENTAÇÃO DA PLATAFORMA - POLIDOS *DEMAIS COMPONENTES - PINTADOS: TINTA DE FUNDO - TINTA EPOXI TINTA DE ACABAMENTO - TINTA POLIÉSTER NA COR PRATA ANDINO</t>
+        </is>
+      </c>
       <c r="T80" t="inlineStr"/>
       <c r="U80" t="inlineStr"/>
       <c r="V80" t="inlineStr"/>
@@ -2952,7 +3260,11 @@
       <c r="P81" t="inlineStr"/>
       <c r="Q81" t="inlineStr"/>
       <c r="R81" t="inlineStr"/>
-      <c r="S81" t="inlineStr"/>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>GARGANTA DN 32 DIN 11851 MATERIAL: AISI 304 POLIDO INT / EXT.</t>
+        </is>
+      </c>
       <c r="T81" t="inlineStr"/>
       <c r="U81" t="inlineStr"/>
       <c r="V81" t="inlineStr"/>
@@ -2981,7 +3293,11 @@
       <c r="P82" t="inlineStr"/>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
-      <c r="S82" t="inlineStr"/>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>MODELO: 2NS-/16H3- EXECUÇÃO: PÉ P MAX PROJ SUC: 3 BAR P MAX PROJ DESC: 10 BAR ESPECIAL: ESP SENTIDO FLUXO: ESQUERDA/DIREITA FLANGE SUCÇÃO: DN 2" - ASME B16.5 - #300 - RF FLANGE DESCARGA: DN 2" - ASME B16.5 - #300 - RF CON. MAN/VACUOM: 1/2" NPT DRENO SUCÇÃO: DN 1/2" - ASME B16.5 - #300 - RF DRENO DESCARGA: DN 1/2" - ASME B16.5 - #300 - RF C/ VÁLV. ALÍVIO: EXTERNA MAT CO BOMBA: SAE 1020 CAR ES CO BOMBA: CERTIFICADO DE CONFORMIDADE|CONFORME NORMA DIN EN 10204-3.1 (CERTIFICADOS DE MATÉRIA-PRIMA CONTENDO COMPOSIÇÃO QUÍMICA E PROPRIEDADES MECÂNICAS)|COM MANUAL DE JUNTAS SOLDADAS|FORNECER DOCUMENTAÇÃO NO IDIOMA INGLÊS|INSPEÇÃO E RELATÓRIO DE LÍQUIDO PENETRANTE|INSPEÇÃO DE SOLDAGEM (IEIS/EPS/RQPS/RQS/RIS)|TODOS OS RELATÓRIOS E PROCEDIMENTOS DEVEM SER ASSINADOS POR INSPETORES QUALIFICADOS SNQC NIVEL II|ITEM RASTREÁVEL|SUPORTE PLAQUETA NÃO RASTREÁVEL|RELATÓRIO DE PARTÍCULA MAGNÉTICA ONDE APLICÁVEL|RELATÓRIO DE TESTE HIDROSTÁTICO|RELATÓRIO DE EVS (ENSAIO VISUAL DE SOLDA)|MATERIAL DO SUPORTE DA PLAQUETA: AISI 316L</t>
+        </is>
+      </c>
       <c r="T82" t="inlineStr"/>
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
@@ -3010,7 +3326,11 @@
       <c r="P83" t="inlineStr"/>
       <c r="Q83" t="inlineStr"/>
       <c r="R83" t="inlineStr"/>
-      <c r="S83" t="inlineStr"/>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>EIXO LIGAÇÃO  TIPO DE CABEÇA: F/TAMANHO: NM090/TIPO BOMBA: BH(P)/             MATERIAL: AISI 316/ACABAMENTO: POLIDO - NORMA WN0113/                         CARAC. ESPECIAL: ESPECIAL P/SELO HJ977GN,COM RESSALTO NO ENCAIXE DO SELO/</t>
+        </is>
+      </c>
       <c r="T83" t="inlineStr"/>
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr"/>
@@ -3039,7 +3359,11 @@
       <c r="P84" t="inlineStr"/>
       <c r="Q84" t="inlineStr"/>
       <c r="R84" t="inlineStr"/>
-      <c r="S84" t="inlineStr"/>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>BATENTE DO EIXO DO EXTRATOR DE LÓBULOS DE BOMBAS TORNADO MODELO DE BOMBA: TORNADO T1 XB MATERIAL: SAE 1020  PARA NOVA EXECUÇÃO FACELIFT</t>
+        </is>
+      </c>
       <c r="T84" t="inlineStr"/>
       <c r="U84" t="inlineStr"/>
       <c r="V84" t="inlineStr"/>
@@ -3068,7 +3392,11 @@
       <c r="P85" t="inlineStr"/>
       <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr"/>
-      <c r="S85" t="inlineStr"/>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>GARGANTA DN 1.1/2" - SCH80; MATERIAL: DUPLEX UNS S31803; FORNECER CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.1 ESPECIAL ITEM RASTREÁVEL.</t>
+        </is>
+      </c>
       <c r="T85" t="inlineStr"/>
       <c r="U85" t="inlineStr"/>
       <c r="V85" t="inlineStr"/>
@@ -3097,7 +3425,11 @@
       <c r="P86" t="inlineStr"/>
       <c r="Q86" t="inlineStr"/>
       <c r="R86" t="inlineStr"/>
-      <c r="S86" t="inlineStr"/>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>GARGANTA DN 1.1/2" - SCH80 MATERIAL: DUPLEX UNS S31803; FORNECER CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.1 ESPECIAL ITEM RASTREÁVEL.</t>
+        </is>
+      </c>
       <c r="T86" t="inlineStr"/>
       <c r="U86" t="inlineStr"/>
       <c r="V86" t="inlineStr"/>
@@ -3126,7 +3458,11 @@
       <c r="P87" t="inlineStr"/>
       <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr"/>
-      <c r="S87" t="inlineStr"/>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>BOCA DE RECALQUE NM063-18; FLANGE DIN EN 1092 DN 100 PN40 FF; MATERIAL: SAE 1020; COM 1 CONEXÃO P/ MANÔMETRO 3/4" NPT.</t>
+        </is>
+      </c>
       <c r="T87" t="inlineStr"/>
       <c r="U87" t="inlineStr"/>
       <c r="V87" t="inlineStr"/>
@@ -3155,7 +3491,11 @@
       <c r="P88" t="inlineStr"/>
       <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr"/>
-      <c r="S88" t="inlineStr"/>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>FUSO MOTOR TIPO: 3NS/MODELO DA BOMBA: 18/SÉRIE DA BOMBA: 16/                  FORMA CONSTR: C,H,L,S/TAMANHO MANCAL: 3/ROLAMENTOS I/                         MAT. JOGO FUSO: AÇO NITRETADO 20MNCR5/                                        SENT. ROTAÇÃO: HORÁRIO (VISTO DA PONTA DE EIXO)/FUSOS UM: 20°C PADRÃO/        TÊMPERA: 850°C-860°C/REVENIMENTO: 540°C-560°C, DUREZA 25+4 HRC/               NITRETAÇÃO: 500°C, DUREZA &gt;= 650HV, CAMADA 300+100µm/SENTIDO HÉLICE: DIREITA/ CARAC ESP PROJ: FURO DE RETORNO PARA ACL MAGNÉTICO/</t>
+        </is>
+      </c>
       <c r="T88" t="inlineStr"/>
       <c r="U88" t="inlineStr"/>
       <c r="V88" t="inlineStr"/>
@@ -3184,7 +3524,11 @@
       <c r="P89" t="inlineStr"/>
       <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr"/>
-      <c r="S89" t="inlineStr"/>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>FUSO MOTOR TIPO: 3NS/MODELO DA BOMBA: 10/SÉRIE DA BOMBA: 80/                  FORMA CONSTR: C,H,L,S/TAMANHO MANCAL: 2/ROLAMENTOS I/                         MAT. JOGO FUSO: AÇO TOOLOX 44/                                                SENT. ROTAÇÃO: HORÁRIO (VISTO DA PONTA DE EIXO)/FUSOS UM: 20°C PADRÃO/        SENTIDO HÉLICE: DIREITA/</t>
+        </is>
+      </c>
       <c r="T89" t="inlineStr"/>
       <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
@@ -3213,7 +3557,11 @@
       <c r="P90" t="inlineStr"/>
       <c r="Q90" t="inlineStr"/>
       <c r="R90" t="inlineStr"/>
-      <c r="S90" t="inlineStr"/>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>CORPO BOMBA  TAMANHO: 2NS-/16H8/EXECUÇÃO: FLANGE/MAT CORPO BOMBA: GJS500 7/   NORMA/CLASSE FL: B16.42/150FF/ESPECIAL: ESP/                                  NORMA MATERIAL: EN 1563 EN GJS 500 7/SENTIDO FLUXO: ESQUERDA P/ DIREITA/      TAMANHO FLANGE: DN 150/PRES PROJ (BAR): 16/CONEXÕES: R1/2" BSP/               CAR ES CO BOMBA: SEM USINAGEM PARA VÁLVULA,COM FURO DE DESAERAÇÃO PASSANTE,SEM UM DOS FUROS PARA RETORNO DE ÓLEO,ALOJAMENTO DOS FUSOS DESLOCADO P/ ALTA PRES. E GIRO HORÁRIO/</t>
+        </is>
+      </c>
       <c r="T90" t="inlineStr"/>
       <c r="U90" t="inlineStr"/>
       <c r="V90" t="inlineStr"/>
@@ -3242,7 +3590,11 @@
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="inlineStr"/>
       <c r="R91" t="inlineStr"/>
-      <c r="S91" t="inlineStr"/>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>EIXO MOVIDO DE BOMBA TORNADO T1  MODELO DE BOMBA: XLB-8/2R MATERIAL: SAE 4140 (1.7225)  ESPECIAL - MANCAL TRASEIRO REFORÇADO APENAS PARA O PROJETO AVARÉ - NAO USAR EM OUTRAS CPS POIS NÃO É COMPATÍVEL COM NOVOS PROJETOS</t>
+        </is>
+      </c>
       <c r="T91" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
       <c r="V91" t="inlineStr"/>
@@ -3271,7 +3623,11 @@
       <c r="P92" t="inlineStr"/>
       <c r="Q92" t="inlineStr"/>
       <c r="R92" t="inlineStr"/>
-      <c r="S92" t="inlineStr"/>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>EIXO MOTOR DE BOMBA TORNADO T1  MODELO DE BOMBA: XLB-8/2R MATERIAL: SAE 4140 (1.7225)  ESPECIAL - MANCAL TRASEIRO REFORÇADO APENAS PARA O PROJETO AVARÉ - NAO USAR EM OUTRAS CPS POIS NÃO É COMPATÍVEL COM NOVOS PROJETOS</t>
+        </is>
+      </c>
       <c r="T92" t="inlineStr"/>
       <c r="U92" t="inlineStr"/>
       <c r="V92" t="inlineStr"/>
@@ -3300,7 +3656,11 @@
       <c r="P93" t="inlineStr"/>
       <c r="Q93" t="inlineStr"/>
       <c r="R93" t="inlineStr"/>
-      <c r="S93" t="inlineStr"/>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>GARGANTA COM CONEXÇÃO SANITÁRIA MATERIAL: AISI 304  CONEXÃO SANITÁRIA 2" TC  ESPECIAL:  - INCLINADA EM 45 GRAUS  - PARA TUBO Ø88,9mm</t>
+        </is>
+      </c>
       <c r="T93" t="inlineStr"/>
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
@@ -3329,7 +3689,11 @@
       <c r="P94" t="inlineStr"/>
       <c r="Q94" t="inlineStr"/>
       <c r="R94" t="inlineStr"/>
-      <c r="S94" t="inlineStr"/>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>PORTA SELO MEC  TIPO DE BOMBA: NM105B/PLATAFORMA: (P)/TIPO: MG1-G60/          MAT CARCAÇA VED: AISI304L/EXEC VEDA EIXO: C/ DRENO,C/ FLUSHING,C/ QUENCH/     CONEX VEDA EIXO: G=1/4" NPT/CONEX. FLUSHING: G=1/4" NPT/DIÂM. DO EIXO: Ø100/  FIXAÇÃO SELAGEM: PADRÃO (PRENSADO)/                                           EXEC. ESPECIAL: COM BUCHA DE RESTRIÇÃO,PARA EXECUÇÃO SEM ANEL DE ENCOSTO,PARA PLANO API 32/</t>
+        </is>
+      </c>
       <c r="T94" t="inlineStr"/>
       <c r="U94" t="inlineStr"/>
       <c r="V94" t="inlineStr"/>
@@ -3358,7 +3722,11 @@
       <c r="P95" t="inlineStr"/>
       <c r="Q95" t="inlineStr"/>
       <c r="R95" t="inlineStr"/>
-      <c r="S95" t="inlineStr"/>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>FLANGE INTERMEDIÁRIA 3NS-/16H4I MATERIAL: FERRO FUNDIDO NODULAR - GGG50 ESPECIAL: APTA SOMENTE PARA ACOPLAMENTO MAGNÉTICO KTR MINEX 60/8; FOLGA ESPECIAL NA VEDAÇÃO DO FUSO Ø41,5 +0,18/+0,16 VAZÃO NECESSÁRIA PARA REFRIGERAÇÃO DO ACOPLAMENTO 30L/H À 2 BAR.</t>
+        </is>
+      </c>
       <c r="T95" t="inlineStr"/>
       <c r="U95" t="inlineStr"/>
       <c r="V95" t="inlineStr"/>
@@ -3387,7 +3755,11 @@
       <c r="P96" t="inlineStr"/>
       <c r="Q96" t="inlineStr"/>
       <c r="R96" t="inlineStr"/>
-      <c r="S96" t="inlineStr"/>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>SUPORTE PARA JUNCTION BOX (CAIXA DE JUNÇÃO) MATERIAL: AÇO CARBONO E AISI 316 ONDE INDICADO NO DESENHO.  MEDIDA: A= 1165,0mm / B= 280,0mm</t>
+        </is>
+      </c>
       <c r="T96" t="inlineStr"/>
       <c r="U96" t="inlineStr"/>
       <c r="V96" t="inlineStr"/>
@@ -3416,7 +3788,11 @@
       <c r="P97" t="inlineStr"/>
       <c r="Q97" t="inlineStr"/>
       <c r="R97" t="inlineStr"/>
-      <c r="S97" t="inlineStr"/>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>TAMPA DIANTEIRA 3NS-/--3I MATERIAL SAE 1045  CARACT. ESPECIAL: EXECUÇÃO PARA ACOPLAMENTO MAGNÉTICO</t>
+        </is>
+      </c>
       <c r="T97" t="inlineStr"/>
       <c r="U97" t="inlineStr"/>
       <c r="V97" t="inlineStr"/>
@@ -3445,7 +3821,11 @@
       <c r="P98" t="inlineStr"/>
       <c r="Q98" t="inlineStr"/>
       <c r="R98" t="inlineStr"/>
-      <c r="S98" t="inlineStr"/>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>EIXO DE CONEXÃO ROTOR/LÂMINA NX549/NM053 ESPECIAL P/ MOLA MATERIAL: AISI 316</t>
+        </is>
+      </c>
       <c r="T98" t="inlineStr"/>
       <c r="U98" t="inlineStr"/>
       <c r="V98" t="inlineStr"/>
@@ -3474,7 +3854,11 @@
       <c r="P99" t="inlineStr"/>
       <c r="Q99" t="inlineStr"/>
       <c r="R99" t="inlineStr"/>
-      <c r="S99" t="inlineStr"/>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>BASE DE BOMBA "E" - APTA PARA:  -BOMBA 3NS-/80H9E;  -MOTOR ELÉTRICO CARCAÇA 225SM; -ACOPLAMENTO VULKAN H128-200; -MATERIAL: A-36;  OBS.: FORNECER BASE COM USINAGEM E SOLDA COMPLETA, SUPERFÍCIES USINADAS SEM PINTURA E PROTEGIDAS SOMENTE COM INIBIDOR DE CORROSÃO.</t>
+        </is>
+      </c>
       <c r="T99" t="inlineStr"/>
       <c r="U99" t="inlineStr"/>
       <c r="V99" t="inlineStr"/>
@@ -3503,7 +3887,11 @@
       <c r="P100" t="inlineStr"/>
       <c r="Q100" t="inlineStr"/>
       <c r="R100" t="inlineStr"/>
-      <c r="S100" t="inlineStr"/>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>TUBO DE IMERSÃO (SUCÇÃO) SEM FILTRO  PARA BOMBA 3NS-/80S3E MATERIAL: AISI 316</t>
+        </is>
+      </c>
       <c r="T100" t="inlineStr"/>
       <c r="U100" t="inlineStr"/>
       <c r="V100" t="inlineStr"/>
@@ -3532,7 +3920,11 @@
       <c r="P101" t="inlineStr"/>
       <c r="Q101" t="inlineStr"/>
       <c r="R101" t="inlineStr"/>
-      <c r="S101" t="inlineStr"/>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>EIXO DE ACIONAMENTO PCP NDH020DH20-HB-SB ESPECIAL PARA ACL SUPERIOR DA VEDAÇÃO ESTÁTICA DO LIP SEAL P/HASTE 1.1/4" MATERIAL: SAE 4140</t>
+        </is>
+      </c>
       <c r="T101" t="inlineStr"/>
       <c r="U101" t="inlineStr"/>
       <c r="V101" t="inlineStr"/>
@@ -3561,7 +3953,11 @@
       <c r="P102" t="inlineStr"/>
       <c r="Q102" t="inlineStr"/>
       <c r="R102" t="inlineStr"/>
-      <c r="S102" t="inlineStr"/>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>BOMBA NETZSCH "NEMO" MOD. NM021BY01L06B  ESPECIFICAÇÕES INTERFACE: BOCAIS DE SUCÇÃO E DESCARGA COM ROSCA INTERNA 1.1/4" NPT POSIÇÃO BOCAL SUCÇÃO: 1.a.1 (VERTICAL CENTRAL) POSIÇÃO BOCAL DESCARGA: 4.a.0 (CENTRAL) BY-PASS: VÁLVULA MOD. DN15, PRESSÃO DE ABERTURA: 2 BAR  MATERIAIS CARCAÇA: AÇO INOX 316 PARTES GIRATÓRIAS: AÇO INOX 316 ROTOR: AÇO INOX 316 UM20 MACIÇO ESTATOR: ELASTÔMERO SBE SELO MECÂNICO: UNS-SEAL 100 Ø25 Q1Q1VGG (8016162) ARTICULAÇÕES/VEDAÇÃO: B/SM ELASTÔMERO NBR ACIONAMENTO: MOTOREDUTOR NM021B NS17 0,75KW 60HZ N=565RPM (NDB4345946) BY-PASS: AÇO INOX 304 VÁLVULA: AÇO INOX 316/MEMBRANA SBE  OBS.  * REGULAR PRESSÃO DE ABERTURA DA VÁLVULA EM 2 BAR.  * APÓS FINALIZAR O TESTE DE PERFORMANCE INVERTER O SENTIDO DE MONTAGEM DA    VÁLVULA.</t>
+        </is>
+      </c>
       <c r="T102" t="inlineStr"/>
       <c r="U102" t="inlineStr"/>
       <c r="V102" t="inlineStr"/>
@@ -3590,7 +3986,11 @@
       <c r="P103" t="inlineStr"/>
       <c r="Q103" t="inlineStr"/>
       <c r="R103" t="inlineStr"/>
-      <c r="S103" t="inlineStr"/>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>ACOPLAMENTO ELÁSTICO  MODELO: ROTEX/TAMANHO: 24/MEDIDA A: A=22,00mm/          MEDIDA B: B=24,50mm/MEDIDA C: C=6,00mm/CUBO FURO A: NORMAL/                   MEDIDA A1: A1=28,00mm/MEDIDA B1: B1=31,00mm/MEDIDA C1: C1=8,00mm/             CUBO FURO A1: GRANDE/FABRICANTE: KTR/                                         CARAC. ESPECIAL: CUBO 1A/1A (GRANDE/GRANDE),MEDIDA ATÉ O CENTRO DO FURO OBLONGO CONFORME DETALHE X IGUAL A 40,00/</t>
+        </is>
+      </c>
       <c r="T103" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
       <c r="V103" t="inlineStr"/>
@@ -3619,7 +4019,11 @@
       <c r="P104" t="inlineStr"/>
       <c r="Q104" t="inlineStr"/>
       <c r="R104" t="inlineStr"/>
-      <c r="S104" t="inlineStr"/>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM038/ESTÁGIOS: 02/GEOMETRIA: S/BORRACHA: NEMOLAST I459/    MATERIAL TUBO: AISI 304/</t>
+        </is>
+      </c>
       <c r="T104" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
       <c r="V104" t="inlineStr"/>
@@ -3648,7 +4052,11 @@
       <c r="P105" t="inlineStr"/>
       <c r="Q105" t="inlineStr"/>
       <c r="R105" t="inlineStr"/>
-      <c r="S105" t="inlineStr"/>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>EIXO LIGAÇÃO  TIPO DE CABEÇA: F/TAMANHO: NM076/TIPO BOMBA: BH(P)/             MATERIAL: AISI 304/ACABAMENTO: POLIDO - NORMA WN0113/                         DIÂMETRO FURO: d1=50,00mm/</t>
+        </is>
+      </c>
       <c r="T105" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
       <c r="V105" t="inlineStr"/>
@@ -3677,7 +4085,11 @@
       <c r="P106" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
       <c r="R106" t="inlineStr"/>
-      <c r="S106" t="inlineStr"/>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM090/ESTÁGIOS: 01/GEOMETRIA: L/BORRACHA: NEMOLAST S05G/    MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T106" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
       <c r="V106" t="inlineStr"/>
@@ -3706,7 +4118,11 @@
       <c r="P107" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
       <c r="R107" t="inlineStr"/>
-      <c r="S107" t="inlineStr"/>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM063/ESTÁGIOS: 04/GEOMETRIA: S/BORRACHA: NEMOLAST S63/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T107" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
       <c r="V107" t="inlineStr"/>
@@ -3735,7 +4151,11 @@
       <c r="P108" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
       <c r="R108" t="inlineStr"/>
-      <c r="S108" t="inlineStr"/>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>ESTATOR  SÉRIE: 2N/TAMANHO: 120/BORRACHA: NEMOLAST S61H/MATERIAL TUBO: 1020/  CARAC. ESPECIAL: BRUTO/</t>
+        </is>
+      </c>
       <c r="T108" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
       <c r="V108" t="inlineStr"/>
@@ -3764,7 +4184,11 @@
       <c r="P109" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
       <c r="R109" t="inlineStr"/>
-      <c r="S109" t="inlineStr"/>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM090/ESTÁGIOS: 01/GEOMETRIA: L/BORRACHA: NEMOLAST S43/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T109" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
       <c r="V109" t="inlineStr"/>
@@ -3793,7 +4217,11 @@
       <c r="P110" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
       <c r="R110" t="inlineStr"/>
-      <c r="S110" t="inlineStr"/>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>BASE P/ BOMBA NM038BY-S/L/P(WP)       ESPECIAL ALTURA 69mm MATERIAL: SAE 1020</t>
+        </is>
+      </c>
       <c r="T110" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
       <c r="V110" t="inlineStr"/>
@@ -3822,7 +4250,11 @@
       <c r="P111" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
       <c r="R111" t="inlineStr"/>
-      <c r="S111" t="inlineStr"/>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA LB07-40 NORMA ANSI B-16.1 DN 2" 250LBS TIPO FF  GG-25</t>
+        </is>
+      </c>
       <c r="T111" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
       <c r="V111" t="inlineStr"/>
@@ -3851,7 +4283,11 @@
       <c r="P112" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
       <c r="R112" t="inlineStr"/>
-      <c r="S112" t="inlineStr"/>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>ESTATOR  SÉRIE: 2N/TAMANHO: 20/BORRACHA: NEMOLAST S61H/MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T112" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
       <c r="V112" t="inlineStr"/>
@@ -3880,7 +4316,11 @@
       <c r="P113" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
       <c r="R113" t="inlineStr"/>
-      <c r="S113" t="inlineStr"/>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>FLANGE MANCAL NEL50A  304 POS 015</t>
+        </is>
+      </c>
       <c r="T113" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
       <c r="V113" t="inlineStr"/>
@@ -3909,7 +4349,11 @@
       <c r="P114" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
       <c r="R114" t="inlineStr"/>
-      <c r="S114" t="inlineStr"/>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>ANEL PARA APERTO NESP 60 A MATERIAL: AISI 304</t>
+        </is>
+      </c>
       <c r="T114" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
       <c r="V114" t="inlineStr"/>
@@ -3938,7 +4382,11 @@
       <c r="P115" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
       <c r="R115" t="inlineStr"/>
-      <c r="S115" t="inlineStr"/>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>BIELA P/ BOMBA SERA R 411.1-1100E D=25; L=149,5; MATERIAL  1.4201/ST   CÓDIGO: 90005392</t>
+        </is>
+      </c>
       <c r="T115" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
       <c r="V115" t="inlineStr"/>
@@ -3967,7 +4415,11 @@
       <c r="P116" t="inlineStr"/>
       <c r="Q116" t="inlineStr"/>
       <c r="R116" t="inlineStr"/>
-      <c r="S116" t="inlineStr"/>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>ANEL DE VEDACAO  TC 1/2" CONFORME ISO2852 TIPO A MATERIAL PERBUNAN</t>
+        </is>
+      </c>
       <c r="T116" t="inlineStr"/>
       <c r="U116" t="inlineStr"/>
       <c r="V116" t="inlineStr"/>
@@ -3996,7 +4448,11 @@
       <c r="P117" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
       <c r="R117" t="inlineStr"/>
-      <c r="S117" t="inlineStr"/>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>COLAR TRASEIRO EXTERNO PTFE P/ MDM-1516 CÓD. MDM0613</t>
+        </is>
+      </c>
       <c r="T117" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
       <c r="V117" t="inlineStr"/>
@@ -4025,7 +4481,11 @@
       <c r="P118" t="inlineStr"/>
       <c r="Q118" t="inlineStr"/>
       <c r="R118" t="inlineStr"/>
-      <c r="S118" t="inlineStr"/>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>PARAFUSO  TIPO: SEXT./BITOLA: M24 x  70,00mm/MATERIAL: A2-70 (304)/           NORMA: ISO 4014/</t>
+        </is>
+      </c>
       <c r="T118" t="inlineStr"/>
       <c r="U118" t="inlineStr"/>
       <c r="V118" t="inlineStr"/>
@@ -4054,7 +4514,11 @@
       <c r="P119" t="inlineStr"/>
       <c r="Q119" t="inlineStr"/>
       <c r="R119" t="inlineStr"/>
-      <c r="S119" t="inlineStr"/>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>FLANGE CFE. DIN EN 1092-1 TIPO 11 (WN); FACE B1; DN 25; PN 40; ESPESSURA DA PAREDE DO PESCOÇO S= 2,6 MATERIAL CFE. ASTM A 105. COM CLASSE DE PRESSÃO SINETADO NO FLANGE. FORNECER CERTIFICADO DE MATERIAIS CONFORME EN 10204-3.1 ESPECIAL ITEM RASTREÁVEL.</t>
+        </is>
+      </c>
       <c r="T119" t="inlineStr"/>
       <c r="U119" t="inlineStr"/>
       <c r="V119" t="inlineStr"/>
@@ -4083,7 +4547,11 @@
       <c r="P120" t="inlineStr"/>
       <c r="Q120" t="inlineStr"/>
       <c r="R120" t="inlineStr"/>
-      <c r="S120" t="inlineStr"/>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>FLANGE CFE. DIN EN 1092-1 TIPO 12 (SOW); FACE B1; DN 100; PN 63; MATERIAL CFE. ASTM A 105. COM CLASSE DE PRESSÃO SINETADO NO FLANGE.</t>
+        </is>
+      </c>
       <c r="T120" t="inlineStr"/>
       <c r="U120" t="inlineStr"/>
       <c r="V120" t="inlineStr"/>
@@ -4112,7 +4580,11 @@
       <c r="P121" t="inlineStr"/>
       <c r="Q121" t="inlineStr"/>
       <c r="R121" t="inlineStr"/>
-      <c r="S121" t="inlineStr"/>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>FLANGE CFE. DIN EN 1092-1 TIPO 12 (SOW); FACE B1; DN 100; PN 40; MATERIAL CFE. ASTM A 105. COM CLASSE DE PRESSÃO SINETADO NO FLANGE.</t>
+        </is>
+      </c>
       <c r="T121" t="inlineStr"/>
       <c r="U121" t="inlineStr"/>
       <c r="V121" t="inlineStr"/>
@@ -4141,7 +4613,11 @@
       <c r="P122" t="inlineStr"/>
       <c r="Q122" t="inlineStr"/>
       <c r="R122" t="inlineStr"/>
-      <c r="S122" t="inlineStr"/>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>ALÇA PARA DESLOCAMENTO P/ BOMBA TORNADO XB-4; MATERIAL SAE 1020 OBS.: FORNECER BASE COM USINAGEM, FURAÇÃO E SOLDA COMPLETA.</t>
+        </is>
+      </c>
       <c r="T122" t="inlineStr"/>
       <c r="U122" t="inlineStr"/>
       <c r="V122" t="inlineStr"/>
@@ -4170,7 +4646,11 @@
       <c r="P123" t="inlineStr"/>
       <c r="Q123" t="inlineStr"/>
       <c r="R123" t="inlineStr"/>
-      <c r="S123" t="inlineStr"/>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>ROTOR  TIPO DE CABEÇA: B/TAMANHO: NX549/NM076/ESTÁGIOS: 02/GEOMETRIA: S/      CLASSE PRESSÃO: 12/MATERIAL: AISI 316/TEMPERATURA: UM20/ESTRUTURA: MACIÇO/    CARAC. ESPECIAL: ESPECIAL PARA LÂMINA (EIXO SOLDADO)/</t>
+        </is>
+      </c>
       <c r="T123" t="inlineStr"/>
       <c r="U123" t="inlineStr"/>
       <c r="V123" t="inlineStr"/>
@@ -4199,7 +4679,11 @@
       <c r="P124" t="inlineStr"/>
       <c r="Q124" t="inlineStr"/>
       <c r="R124" t="inlineStr"/>
-      <c r="S124" t="inlineStr"/>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>MATERIAL: SAE 1020 PINTURA EXTERNA: COR VERDE EMBLEMA 2,5 G 3/4 PINTURA INTERNA: COR BRANCA</t>
+        </is>
+      </c>
       <c r="T124" t="inlineStr"/>
       <c r="U124" t="inlineStr"/>
       <c r="V124" t="inlineStr"/>
@@ -4228,7 +4712,11 @@
       <c r="P125" t="inlineStr"/>
       <c r="Q125" t="inlineStr"/>
       <c r="R125" t="inlineStr"/>
-      <c r="S125" t="inlineStr"/>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>CARTUCHO PARA BOMBA DE FUSOS ESPECIAL MODELO: 3NS-/80-7- MATERIAL: FERRO FUNDIDO DIN EN 1563 EN GJS 500 7 (GGG-50)  **ESPECIAL = POS.15 DO ANEL-O DESLOCADO**  **MEDIR RUGOSIDADE DAS PARTES INTERNAS DO CARTUCHO, ONDE SE ALOJAM OS FUSOS, ISSO PARA GARANTIR AS ESPECIFICAÇÕES  DO DESENHO.**</t>
+        </is>
+      </c>
       <c r="T125" t="inlineStr"/>
       <c r="U125" t="inlineStr"/>
       <c r="V125" t="inlineStr"/>
@@ -4257,7 +4745,11 @@
       <c r="P126" t="inlineStr"/>
       <c r="Q126" t="inlineStr"/>
       <c r="R126" t="inlineStr"/>
-      <c r="S126" t="inlineStr"/>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM076/ESTÁGIOS: 02/GEOMETRIA: S/BORRACHA: NEMOLAST S41/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T126" t="inlineStr"/>
       <c r="U126" t="inlineStr"/>
       <c r="V126" t="inlineStr"/>
@@ -4286,7 +4778,11 @@
       <c r="P127" t="inlineStr"/>
       <c r="Q127" t="inlineStr"/>
       <c r="R127" t="inlineStr"/>
-      <c r="S127" t="inlineStr"/>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM045/ESTÁGIOS: 03/GEOMETRIA: S/BORRACHA: NEMOLAST S45/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T127" t="inlineStr"/>
       <c r="U127" t="inlineStr"/>
       <c r="V127" t="inlineStr"/>
@@ -4315,7 +4811,11 @@
       <c r="P128" t="inlineStr"/>
       <c r="Q128" t="inlineStr"/>
       <c r="R128" t="inlineStr"/>
-      <c r="S128" t="inlineStr"/>
+      <c r="S128" t="inlineStr">
+        <is>
+          <t>ESTATOR  TAMANHO: NM045/ESTÁGIOS: 01/GEOMETRIA: S/BORRACHA: NEMOLAST S45/     MATERIAL TUBO: 1020/</t>
+        </is>
+      </c>
       <c r="T128" t="inlineStr"/>
       <c r="U128" t="inlineStr"/>
       <c r="V128" t="inlineStr"/>
@@ -4344,7 +4844,11 @@
       <c r="P129" t="inlineStr"/>
       <c r="Q129" t="inlineStr"/>
       <c r="R129" t="inlineStr"/>
-      <c r="S129" t="inlineStr"/>
+      <c r="S129" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: J/SÉRIE: NES/TAMANHO: 60A/MATERIAL: AISI 304/          TIPO DA ROSCA: ROSCA S/ FIM/</t>
+        </is>
+      </c>
       <c r="T129" t="inlineStr"/>
       <c r="U129" t="inlineStr"/>
       <c r="V129" t="inlineStr"/>
@@ -4373,7 +4877,11 @@
       <c r="P130" t="inlineStr"/>
       <c r="Q130" t="inlineStr"/>
       <c r="R130" t="inlineStr"/>
-      <c r="S130" t="inlineStr"/>
+      <c r="S130" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: B-SM/SÉRIE: NBS/TAMANHO: 40A/MATERIAL: AISI 316/       VEDAÇÃO SM: VED SM/TIPO DA ROSCA: ROSCA S/ FIM/</t>
+        </is>
+      </c>
       <c r="T130" t="inlineStr"/>
       <c r="U130" t="inlineStr"/>
       <c r="V130" t="inlineStr"/>
@@ -4402,7 +4910,11 @@
       <c r="P131" t="inlineStr"/>
       <c r="Q131" t="inlineStr"/>
       <c r="R131" t="inlineStr"/>
-      <c r="S131" t="inlineStr"/>
+      <c r="S131" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: V/TAMANHO: NM105/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 04/ MATERIAL: AISI 304/</t>
+        </is>
+      </c>
       <c r="T131" t="inlineStr"/>
       <c r="U131" t="inlineStr"/>
       <c r="V131" t="inlineStr"/>
@@ -4431,7 +4943,11 @@
       <c r="P132" t="inlineStr"/>
       <c r="Q132" t="inlineStr"/>
       <c r="R132" t="inlineStr"/>
-      <c r="S132" t="inlineStr"/>
+      <c r="S132" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA NES40A  MATERIAL AISI 304. COM CAMISA DE AQUECIMENTO. POLIDO INTERNAMENTE.</t>
+        </is>
+      </c>
       <c r="T132" t="inlineStr"/>
       <c r="U132" t="inlineStr"/>
       <c r="V132" t="inlineStr"/>
@@ -4460,7 +4976,11 @@
       <c r="P133" t="inlineStr"/>
       <c r="Q133" t="inlineStr"/>
       <c r="R133" t="inlineStr"/>
-      <c r="S133" t="inlineStr"/>
+      <c r="S133" t="inlineStr">
+        <is>
+          <t>GARGANTA  NE 100      MATERIAL  AISI 316</t>
+        </is>
+      </c>
       <c r="T133" t="inlineStr"/>
       <c r="U133" t="inlineStr"/>
       <c r="V133" t="inlineStr"/>
@@ -4489,7 +5009,11 @@
       <c r="P134" t="inlineStr"/>
       <c r="Q134" t="inlineStr"/>
       <c r="R134" t="inlineStr"/>
-      <c r="S134" t="inlineStr"/>
+      <c r="S134" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA NEC 60A    ESPECIAL BOCAL DE SUCÇÃO 4"SMS TANGENCIAL C/ BOCAL ADICIONAL P/ LIMPEZA CIP 2"SMS TANGENCIAL MATERIAL AISI 304 POLIDO INT/EXT.</t>
+        </is>
+      </c>
       <c r="T134" t="inlineStr"/>
       <c r="U134" t="inlineStr"/>
       <c r="V134" t="inlineStr"/>
@@ -4518,7 +5042,11 @@
       <c r="P135" t="inlineStr"/>
       <c r="Q135" t="inlineStr"/>
       <c r="R135" t="inlineStr"/>
-      <c r="S135" t="inlineStr"/>
+      <c r="S135" t="inlineStr">
+        <is>
+          <t>GARGANTA NEC 60A ESPECIAL P/CONEXÃO SANITÁRIA 4" TANGENCIAL MATERIAL: AISI 304.</t>
+        </is>
+      </c>
       <c r="T135" t="inlineStr"/>
       <c r="U135" t="inlineStr"/>
       <c r="V135" t="inlineStr"/>
@@ -4547,7 +5075,11 @@
       <c r="P136" t="inlineStr"/>
       <c r="Q136" t="inlineStr"/>
       <c r="R136" t="inlineStr"/>
-      <c r="S136" t="inlineStr"/>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: B/TAMANHO: NM053/EXECUÇÃO BOMBA: O/ESTÁGIOS: 04/       GEOMETRIA: S/CLASSE PRESSÃO: 24/MATERIAL: AISI 304/                           TIPO DA ROSCA: ROSCA S/ FIM/ACABAMENTO: ESP./DIST. ARTICUL.: GA=1100mm/       CARAC. ESPECIAL: COM ROSCA EM TODA EXTENSÃO DO FUNIL,PARA CORPO DA BOMBA COM FUNIL 602 X 224/</t>
+        </is>
+      </c>
       <c r="T136" t="inlineStr"/>
       <c r="U136" t="inlineStr"/>
       <c r="V136" t="inlineStr"/>
@@ -4576,7 +5108,11 @@
       <c r="P137" t="inlineStr"/>
       <c r="Q137" t="inlineStr"/>
       <c r="R137" t="inlineStr"/>
-      <c r="S137" t="inlineStr"/>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM031-H-12- MATERIAL  AISI 304 CONEXÃO SANITÁRIA 2.1/2"SMS POLIDO INTERNO/EXTERNAMENTE. ACABAMENTO SUPERFICIAL CFE.WN0113.</t>
+        </is>
+      </c>
       <c r="T137" t="inlineStr"/>
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr"/>
@@ -4605,7 +5141,11 @@
       <c r="P138" t="inlineStr"/>
       <c r="Q138" t="inlineStr"/>
       <c r="R138" t="inlineStr"/>
-      <c r="S138" t="inlineStr"/>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM038-12   C/ CONEXÃO SANITÁRIA 3"SMS   MATERIAL:  AISI 316 POLIDO INTERNAMENTE. C/ CAMISA DE AQUECIMENTO.</t>
+        </is>
+      </c>
       <c r="T138" t="inlineStr"/>
       <c r="U138" t="inlineStr"/>
       <c r="V138" t="inlineStr"/>
@@ -4634,7 +5174,11 @@
       <c r="P139" t="inlineStr"/>
       <c r="Q139" t="inlineStr"/>
       <c r="R139" t="inlineStr"/>
-      <c r="S139" t="inlineStr"/>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM045-F-12 MATERIAL  AISI 316 BOCA RETANGULAR 750 X 220 ACABAMENTO: POLIDO INTERNO</t>
+        </is>
+      </c>
       <c r="T139" t="inlineStr"/>
       <c r="U139" t="inlineStr"/>
       <c r="V139" t="inlineStr"/>
@@ -4663,7 +5207,11 @@
       <c r="P140" t="inlineStr"/>
       <c r="Q140" t="inlineStr"/>
       <c r="R140" t="inlineStr"/>
-      <c r="S140" t="inlineStr"/>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: V/TAMANHO: NM063/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 14/ PLATAFORMA P: (P)/MATERIAL: AISI 316L/ACABAMENTO: ESP/                        CARAC. ESPECIAL: PARA LUVA DE PROTEÇÃO/</t>
+        </is>
+      </c>
       <c r="T140" t="inlineStr"/>
       <c r="U140" t="inlineStr"/>
       <c r="V140" t="inlineStr"/>
@@ -4692,7 +5240,11 @@
       <c r="P141" t="inlineStr"/>
       <c r="Q141" t="inlineStr"/>
       <c r="R141" t="inlineStr"/>
-      <c r="S141" t="inlineStr"/>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: H/TAMANHO: NM031/EXECUÇÃO BOMBA: H/ESTÁGIOS: 02/       GEOMETRIA: S/CLASSE PRESSÃO: 12/PLATAFORMA: (P)/MATERIAL: AISI 304/           TIPO DA ROSCA: ROSCA S/ FIM/ACABAMENTO: POL./                                 TIPO ACABAMENTO: POLIDO CONFORME NORMA WN0113/</t>
+        </is>
+      </c>
       <c r="T141" t="inlineStr"/>
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr"/>
@@ -4721,7 +5273,11 @@
       <c r="P142" t="inlineStr"/>
       <c r="Q142" t="inlineStr"/>
       <c r="R142" t="inlineStr"/>
-      <c r="S142" t="inlineStr"/>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM076-14             01 DRENO COM CAMISA DE AQUECIMENTO MATERIAL  AISI 304 FLANGE CFE ANSI B16.5 150PSI 6" FF</t>
+        </is>
+      </c>
       <c r="T142" t="inlineStr"/>
       <c r="U142" t="inlineStr"/>
       <c r="V142" t="inlineStr"/>
@@ -4750,7 +5306,11 @@
       <c r="P143" t="inlineStr"/>
       <c r="Q143" t="inlineStr"/>
       <c r="R143" t="inlineStr"/>
-      <c r="S143" t="inlineStr"/>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM021-12 MATERIAL  AISI 316 CONEXAO  ROSCA NPT 1.1/4" (+01 DRENO) BOCAL DE SUCÇÃO TANGENCIAL À DIREITA (VISTA DO ACIONAMENTO)</t>
+        </is>
+      </c>
       <c r="T143" t="inlineStr"/>
       <c r="U143" t="inlineStr"/>
       <c r="V143" t="inlineStr"/>
@@ -4779,7 +5339,11 @@
       <c r="P144" t="inlineStr"/>
       <c r="Q144" t="inlineStr"/>
       <c r="R144" t="inlineStr"/>
-      <c r="S144" t="inlineStr"/>
+      <c r="S144" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: V/TAMANHO: NM031/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 48/ MATERIAL: AISI 316L/</t>
+        </is>
+      </c>
       <c r="T144" t="inlineStr"/>
       <c r="U144" t="inlineStr"/>
       <c r="V144" t="inlineStr"/>
@@ -4808,7 +5372,11 @@
       <c r="P145" t="inlineStr"/>
       <c r="Q145" t="inlineStr"/>
       <c r="R145" t="inlineStr"/>
-      <c r="S145" t="inlineStr"/>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: B/TAMANHO: NM038/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 12/ PLATAFORMA P: (P)/MATERIAL: AISI 420/ACABAMENTO: POLIDO/                      TIPO ACABAMENTO: POLIDO CONFORME NORMA WN0113/</t>
+        </is>
+      </c>
       <c r="T145" t="inlineStr"/>
       <c r="U145" t="inlineStr"/>
       <c r="V145" t="inlineStr"/>
@@ -4837,7 +5405,11 @@
       <c r="P146" t="inlineStr"/>
       <c r="Q146" t="inlineStr"/>
       <c r="R146" t="inlineStr"/>
-      <c r="S146" t="inlineStr"/>
+      <c r="S146" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM021-O-12 MATERIAL  AISI 316 BOCA RETANGULAR 104 X 204 STANDARD: COM 01 DRENO  (EXECUÇÃO C/ ROSCA SEM FIM EM TODA EXTENSÃO DO FUNIL).</t>
+        </is>
+      </c>
       <c r="T146" t="inlineStr"/>
       <c r="U146" t="inlineStr"/>
       <c r="V146" t="inlineStr"/>
@@ -4866,7 +5438,11 @@
       <c r="P147" t="inlineStr"/>
       <c r="Q147" t="inlineStr"/>
       <c r="R147" t="inlineStr"/>
-      <c r="S147" t="inlineStr"/>
+      <c r="S147" t="inlineStr">
+        <is>
+          <t>ESTATOR  NM093--02S  C/02CHANFROS(ESPECIAL) MATERIAL  NEMOLAST G91 (VI-65/Alu)</t>
+        </is>
+      </c>
       <c r="T147" t="inlineStr"/>
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr"/>
@@ -4895,7 +5471,11 @@
       <c r="P148" t="inlineStr"/>
       <c r="Q148" t="inlineStr"/>
       <c r="R148" t="inlineStr"/>
-      <c r="S148" t="inlineStr"/>
+      <c r="S148" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM105-T---12        MATERIAL  SAE 1020. FLANGE 8"ANSI B16.5 / 150PSI / FF. C/ PLACA DE SUSTENTAÇÃO RETANGULAR (1200X800). PROFUNDIDADE DE IMERSÃO: 2800mm. DIMENSÕES: A=3368mm; B=3168mm; L=2084mm;</t>
+        </is>
+      </c>
       <c r="T148" t="inlineStr"/>
       <c r="U148" t="inlineStr"/>
       <c r="V148" t="inlineStr"/>
@@ -4924,7 +5504,11 @@
       <c r="P149" t="inlineStr"/>
       <c r="Q149" t="inlineStr"/>
       <c r="R149" t="inlineStr"/>
-      <c r="S149" t="inlineStr"/>
+      <c r="S149" t="inlineStr">
+        <is>
+          <t>CORPO DE DESGASTE PARA BOMBA DE FUSOS MODELO PARA CORPO FUNDIDO: 3NS-/40H5- MATERIAL: FERRO FUNDIDO GG-30 - BRUNIMENTO NO ALOJAMENTO DOS FUSOS MOVIDOS; - MEDIR RUGOSIDADE DAS PARTES INTERNAS DO CARTUCHO, ONDE SE ALOJAM OS FUSOS, PARA GARANTIR AS ESPECIFICAÇÕES  DO DESENHO.</t>
+        </is>
+      </c>
       <c r="T149" t="inlineStr"/>
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr"/>
@@ -4953,7 +5537,11 @@
       <c r="P150" t="inlineStr"/>
       <c r="Q150" t="inlineStr"/>
       <c r="R150" t="inlineStr"/>
-      <c r="S150" t="inlineStr"/>
+      <c r="S150" t="inlineStr">
+        <is>
+          <t>BU MANCAL 2NS -/16-4-  MATERIAL: VESCONITE HILUBE</t>
+        </is>
+      </c>
       <c r="T150" t="inlineStr"/>
       <c r="U150" t="inlineStr"/>
       <c r="V150" t="inlineStr"/>
@@ -4982,7 +5570,11 @@
       <c r="P151" t="inlineStr"/>
       <c r="Q151" t="inlineStr"/>
       <c r="R151" t="inlineStr"/>
-      <c r="S151" t="inlineStr"/>
+      <c r="S151" t="inlineStr">
+        <is>
+          <t>CARTUCHO PARA BOMBA DE FUSOS NOTOS MODELO: 3NS-/25-11- MATERIAL: FERRO FUNDIDO EN-GJS-500-7</t>
+        </is>
+      </c>
       <c r="T151" t="inlineStr"/>
       <c r="U151" t="inlineStr"/>
       <c r="V151" t="inlineStr"/>
@@ -5011,7 +5603,11 @@
       <c r="P152" t="inlineStr"/>
       <c r="Q152" t="inlineStr"/>
       <c r="R152" t="inlineStr"/>
-      <c r="S152" t="inlineStr"/>
+      <c r="S152" t="inlineStr">
+        <is>
+          <t>PLACA DE ARRASTE PCP HASTE 1.1/2" 15 TON (C/SISTEMA DE CENTRALIZAÇÃO CÔNICA) MATERIAL: SAE 1045  COMPONENTES BLOCO OXICORTADO  SAE 1045  C=44,45mm A=240,00 B=145,00 - 2PÇ PARAFUSO  SEXT. M24 x 120,00mm AÇO 8.8 DIN 933 ZINC TRIV BRANCO - 6PÇ ARRUELA  PRESSÃO M24 AÇO MOLA HRC-46 DIN 127 ZINC TRIV BRANCO - 6PÇ PORCA  SEXT. M24 AÇO 8.8 DIN 934 ZINCADO TRIVALENTE BRANCO - 6PÇ 250001     CHAPA   3,04MM SAE 1008/10 - 0,02590M²  PINTURA:ALARANJADO SEGURANÇA MUNSELL 2.5YR 6/14 OBS.: PROTEGER AS PEÇAS CONTRA CORROSÃO NAS PARTES NÃO PINTADAS</t>
+        </is>
+      </c>
       <c r="T152" t="inlineStr"/>
       <c r="U152" t="inlineStr"/>
       <c r="V152" t="inlineStr"/>
@@ -5040,7 +5636,11 @@
       <c r="P153" t="inlineStr"/>
       <c r="Q153" t="inlineStr"/>
       <c r="R153" t="inlineStr"/>
-      <c r="S153" t="inlineStr"/>
+      <c r="S153" t="inlineStr">
+        <is>
+          <t>PLACA DE ARRASTE PCP HASTE 1.1/4" 15 TON (C/SISTEMA DE CENTRALIZAÇÃO CÔNICA) MATERIAL: SAE 1045  COMPONENTES BLOCO OXICORTADO  SAE 1045  C=44,45mm A=240,00 B=145,00 - 2PÇ PARAFUSO  SEXT. M24 x 120,00mm AÇO 8.8 DIN 933 ZINC TRIV BRANCO - 6PÇ ARRUELA  PRESSÃO M24 AÇO MOLA HRC-46 DIN 127 ZINC TRIV BRANCO - 6PÇ PORCA  SEXT. M24 AÇO 8.8 DIN 934 ZINCADO TRIVALENTE BRANCO - 6PÇ 250001     CHAPA   3,04MM SAE 1008/10 - 0,02590M²  PINTURA:ALARANJADO SEGURANÇA MUNSELL 2.5YR 6/14 OBS.: PROTEGER AS PEÇAS CONTRA CORROSÃO NAS PARTES NÃO PINTADAS</t>
+        </is>
+      </c>
       <c r="T153" t="inlineStr"/>
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr"/>
@@ -5069,7 +5669,11 @@
       <c r="P154" t="inlineStr"/>
       <c r="Q154" t="inlineStr"/>
       <c r="R154" t="inlineStr"/>
-      <c r="S154" t="inlineStr"/>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: F/TAMANHO: NM105/EXECUÇÃO BOMBA: H/CLASSE PRESSÃO: 02/ MATERIAL: UNS S31803/</t>
+        </is>
+      </c>
       <c r="T154" t="inlineStr"/>
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr"/>
@@ -5098,7 +5702,11 @@
       <c r="P155" t="inlineStr"/>
       <c r="Q155" t="inlineStr"/>
       <c r="R155" t="inlineStr"/>
-      <c r="S155" t="inlineStr"/>
+      <c r="S155" t="inlineStr">
+        <is>
+          <t>PÉ DA BOMBA DE FUSOS 3NS-/40H5- E 3NS-/40H6- MATERIAL FERRO FUNDIDO NODULAR DIN EN 1563 EN GJS 500 7 CONEXÕES PARA O AQUECIMENTO: 3/8"BSP PRESSÃO MÁXIMA NA CÂMARA DE AQUECIMENTO: 16,0 BAR (T_MÁX: 200°C) PRESSÃO TH MÁXIMO NA CÂMARA DE AQUECIMENTO: 24,0 BAR  MODELO NR NB4949103 (IDENT NDB4949103)</t>
+        </is>
+      </c>
       <c r="T155" t="inlineStr"/>
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr"/>
@@ -5127,7 +5735,11 @@
       <c r="P156" t="inlineStr"/>
       <c r="Q156" t="inlineStr"/>
       <c r="R156" t="inlineStr"/>
-      <c r="S156" t="inlineStr"/>
+      <c r="S156" t="inlineStr">
+        <is>
+          <t>BOCAL DE SUCÇÃO  TAMANHO: 3NS-/-L5-/NORMA: DIN EN 1563 EN GJS 500 7/          EXECUÇÃO: BOCAL ORIENTÁVEL EM TODOS OS QUADRANTES/                            MATERIAL: FERRO FUNDIDO NODULAR/MODELO: NB 4949924/                           CERTIFICADO: COMPOSIÇÃO QUÍMICA E PROPRIEDADES MECÂNICAS ESPECÍFICAS PARA O ITEM ADQUIRIDO, NORMA DE FABRICAÇÃO, NÚMERO DA CORRIDA E LOTE/PESO/PÇ (KG): 5,10/</t>
+        </is>
+      </c>
       <c r="T156" t="inlineStr"/>
       <c r="U156" t="inlineStr"/>
       <c r="V156" t="inlineStr"/>
@@ -5156,7 +5768,11 @@
       <c r="P157" t="inlineStr"/>
       <c r="Q157" t="inlineStr"/>
       <c r="R157" t="inlineStr"/>
-      <c r="S157" t="inlineStr"/>
+      <c r="S157" t="inlineStr">
+        <is>
+          <t>ESTATOR 2N 60 SBE (NBR COM 465 ACN) COM FERRAMENTA BB DIAM MENOR 59,6-0,70MM TUBO EVEN WALL</t>
+        </is>
+      </c>
       <c r="T157" t="inlineStr"/>
       <c r="U157" t="inlineStr"/>
       <c r="V157" t="inlineStr"/>
@@ -5185,7 +5801,11 @@
       <c r="P158" t="inlineStr"/>
       <c r="Q158" t="inlineStr"/>
       <c r="R158" t="inlineStr"/>
-      <c r="S158" t="inlineStr"/>
+      <c r="S158" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM038-O-12        ESPECIAL MATERIAL  AISI 316 BOCA RETANGULAR 154 X 254mm ACABAMENTO: POLIDO INTERNO</t>
+        </is>
+      </c>
       <c r="T158" t="inlineStr"/>
       <c r="U158" t="inlineStr"/>
       <c r="V158" t="inlineStr"/>
@@ -5214,7 +5834,11 @@
       <c r="P159" t="inlineStr"/>
       <c r="Q159" t="inlineStr"/>
       <c r="R159" t="inlineStr"/>
-      <c r="S159" t="inlineStr"/>
+      <c r="S159" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM090-P-18  G=1"NPT MATERIAL  SAE 1020 BOCA RETANGULAR 750 X 720MM</t>
+        </is>
+      </c>
       <c r="T159" t="inlineStr"/>
       <c r="U159" t="inlineStr"/>
       <c r="V159" t="inlineStr"/>
@@ -5243,7 +5867,11 @@
       <c r="P160" t="inlineStr"/>
       <c r="Q160" t="inlineStr"/>
       <c r="R160" t="inlineStr"/>
-      <c r="S160" t="inlineStr"/>
+      <c r="S160" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM038-H-12-              (CORPO C/ REPUXE) MATERIAL AISI 304 CONEXÃO SANITÁRIA 2"SMS POLIDO INTERNO/EXTERNAMENTE. ACABAMENTO SUPERFICIAL CFE.WN0113.</t>
+        </is>
+      </c>
       <c r="T160" t="inlineStr"/>
       <c r="U160" t="inlineStr"/>
       <c r="V160" t="inlineStr"/>
@@ -5272,7 +5900,11 @@
       <c r="P161" t="inlineStr"/>
       <c r="Q161" t="inlineStr"/>
       <c r="R161" t="inlineStr"/>
-      <c r="S161" t="inlineStr"/>
+      <c r="S161" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: V/TAMANHO: NM045/EXECUÇÃO BOMBA: BT/                   CLASSE PRESSÃO: 12/MATERIAL: AISI 304/ALTURA IMERSÃO: 2200mm/                 MEDIDA GA: GA=1692mm/MEDIDA B: B=1724mm/</t>
+        </is>
+      </c>
       <c r="T161" t="inlineStr"/>
       <c r="U161" t="inlineStr"/>
       <c r="V161" t="inlineStr"/>
@@ -5301,7 +5933,11 @@
       <c r="P162" t="inlineStr"/>
       <c r="Q162" t="inlineStr"/>
       <c r="R162" t="inlineStr"/>
-      <c r="S162" t="inlineStr"/>
+      <c r="S162" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: F/TAMANHO: NM031/EXECUÇÃO BOMBA: H/CLASSE PRESSÃO: 12/ MATERIAL: AISI 304/ACABAMENTO: ESP/                                           CARAC. ESPECIAL: APENAS PARA BOMBAS EM CORTE (EXPOSIÇÕES)/</t>
+        </is>
+      </c>
       <c r="T162" t="inlineStr"/>
       <c r="U162" t="inlineStr"/>
       <c r="V162" t="inlineStr"/>
@@ -5330,7 +5966,11 @@
       <c r="P163" t="inlineStr"/>
       <c r="Q163" t="inlineStr"/>
       <c r="R163" t="inlineStr"/>
-      <c r="S163" t="inlineStr"/>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: B/TAMANHO: NM063/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 12/ PLATAFORMA P: (P)/MATERIAL: AISI 304/ACABAMENTO: ESP/                         CARAC. ESPECIAL: PARA LUVA DE PROTEÇÃO/</t>
+        </is>
+      </c>
       <c r="T163" t="inlineStr"/>
       <c r="U163" t="inlineStr"/>
       <c r="V163" t="inlineStr"/>
@@ -5359,7 +5999,11 @@
       <c r="P164" t="inlineStr"/>
       <c r="Q164" t="inlineStr"/>
       <c r="R164" t="inlineStr"/>
-      <c r="S164" t="inlineStr"/>
+      <c r="S164" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: K/TAMANHO: NM105/EXECUÇÃO BOMBA: BT/                   CLASSE PRESSÃO: 12/MATERIAL: AISI 420/ALTURA IMERSÃO: 2891mm/                 MEDIDA GA: GA=1841mm/MEDIDA B: B=1985mm/</t>
+        </is>
+      </c>
       <c r="T164" t="inlineStr"/>
       <c r="U164" t="inlineStr"/>
       <c r="V164" t="inlineStr"/>
@@ -5388,7 +6032,11 @@
       <c r="P165" t="inlineStr"/>
       <c r="Q165" t="inlineStr"/>
       <c r="R165" t="inlineStr"/>
-      <c r="S165" t="inlineStr"/>
+      <c r="S165" t="inlineStr">
+        <is>
+          <t>CORPO DA BOMBA  NM063-14 MATERIAL AISI 316 CONEXÃO SANITÁRIA 3"TC POLIDO INTERNO</t>
+        </is>
+      </c>
       <c r="T165" t="inlineStr"/>
       <c r="U165" t="inlineStr"/>
       <c r="V165" t="inlineStr"/>
@@ -5417,7 +6065,11 @@
       <c r="P166" t="inlineStr"/>
       <c r="Q166" t="inlineStr"/>
       <c r="R166" t="inlineStr"/>
-      <c r="S166" t="inlineStr"/>
+      <c r="S166" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: J/TAMANHO: NM076/EXECUÇÃO BOMBA: Y/CLASSE PRESSÃO: 07/ PLATAFORMA P: (P)/MATERIAL: SAE 1020/ACABAMENTO: ESP/                         CARAC. ESPECIAL: MEDIDA A = 405mm/</t>
+        </is>
+      </c>
       <c r="T166" t="inlineStr"/>
       <c r="U166" t="inlineStr"/>
       <c r="V166" t="inlineStr"/>
@@ -5446,7 +6098,11 @@
       <c r="P167" t="inlineStr"/>
       <c r="Q167" t="inlineStr"/>
       <c r="R167" t="inlineStr"/>
-      <c r="S167" t="inlineStr"/>
+      <c r="S167" t="inlineStr">
+        <is>
+          <t>FLANGE DO CORPO  MODELO: 4NS-/-H1E/MATERIAL: ASTM A-36/MEDIDA B: B=280,00/    MEDIDA C: C=330,00/MEDIDA A: A=35,00/MEDIDA D: D=190,00/MEDIDA E: E=230,00/   MEDIDA F: F=10,00/MEDIDA G: G=41,28/MEDIDA H: H=140,00/MEDIDA J: J=40,00/     MEDIDA K: K=270,50/MEDIDA L: L=181,00/MEDIDA M: M=202,00/MEDIDA N: N=140,00/  MEDIDA R: R=350,00mm/MEDIDA R1: R1=180,00/</t>
+        </is>
+      </c>
       <c r="T167" t="inlineStr"/>
       <c r="U167" t="inlineStr"/>
       <c r="V167" t="inlineStr"/>
@@ -5475,7 +6131,11 @@
       <c r="P168" t="inlineStr"/>
       <c r="Q168" t="inlineStr"/>
       <c r="R168" t="inlineStr"/>
-      <c r="S168" t="inlineStr"/>
+      <c r="S168" t="inlineStr">
+        <is>
+          <t>FLANGE DO CORPO  MODELO: 4NS-/-H4E/MATERIAL: ASTM A-36/MEDIDA B: B=430,00/    MEDIDA C: C=520,00/MEDIDA A: A=65,00/MEDIDA D: D=260,00/MEDIDA E: E=380,00/   MEDIDA F: F=25,00/MEDIDA G: G=50,80/MEDIDA H: H=230,00/MEDIDA J: J=50,00/     MEDIDA K: K=269,00/MEDIDA L: L=313,00/MEDIDA M: M=344,00/MEDIDA N: N=230,00/  MEDIDA R: R=590,00mm/MEDIDA R1: R1=430,00/</t>
+        </is>
+      </c>
       <c r="T168" t="inlineStr"/>
       <c r="U168" t="inlineStr"/>
       <c r="V168" t="inlineStr"/>
@@ -5504,7 +6164,11 @@
       <c r="P169" t="inlineStr"/>
       <c r="Q169" t="inlineStr"/>
       <c r="R169" t="inlineStr"/>
-      <c r="S169" t="inlineStr"/>
+      <c r="S169" t="inlineStr">
+        <is>
+          <t>BOMBA DE FUSOS NETZSCH MOD. 3NS 07/25M2E  DIÂMETRO EXTERNO/PASSO: Ø26/38 3 = 3 FUSOS NS = NETZSCH SCREW 07 = VAZÃO (0,7m³/h @ 1000 RPM @ 0 BAR) /25 = PRESSÃO DE DESCARGA MÁX. (bar) M = EXECUÇÃO MINI 2 = MANCAL NR. 2 E = ROLAMENTO EXTERNO BLINDADO COM VÁLVULA DE ALÍVIO INTEGRADA - 10 A 25 BAR ABERTURA VÁLVULA REGULADA 20 BAR FLANGES DE CONEXÃO 1.1/2" SAE J518C 3000 PSI</t>
+        </is>
+      </c>
       <c r="T169" t="inlineStr"/>
       <c r="U169" t="inlineStr"/>
       <c r="V169" t="inlineStr"/>
@@ -5533,7 +6197,11 @@
       <c r="P170" t="inlineStr"/>
       <c r="Q170" t="inlineStr"/>
       <c r="R170" t="inlineStr"/>
-      <c r="S170" t="inlineStr"/>
+      <c r="S170" t="inlineStr">
+        <is>
+          <t>EIXO ACL  ARTICULAÇÃO: H/TAMANHO: NM038/EXECUÇÃO BOMBA: H/CLASSE PRESSÃO: 12/ PLATAFORMA P: (P)/MATERIAL: AISI 304/ACABAMENTO: ESP,POLIDO/                  TIPO ACABAMENTO: POLIDO CONFORME NORMA WN0113/                                CARAC. ESPECIAL: SEM FUROS ADICIONAIS/</t>
+        </is>
+      </c>
       <c r="T170" t="inlineStr"/>
       <c r="U170" t="inlineStr"/>
       <c r="V170" t="inlineStr"/>
@@ -5562,7 +6230,11 @@
       <c r="P171" t="inlineStr"/>
       <c r="Q171" t="inlineStr"/>
       <c r="R171" t="inlineStr"/>
-      <c r="S171" t="inlineStr"/>
+      <c r="S171" t="inlineStr">
+        <is>
+          <t>CARTUCHO PARA BOMBA DE FUSOS NOTOS MODELO: 3NS-/80-11- MATERIAL: FERRO FUNDIDO EN-GJS-500-7 SEM FURO PARA RETORNO DE ÓLEO.</t>
+        </is>
+      </c>
       <c r="T171" t="inlineStr"/>
       <c r="U171" t="inlineStr"/>
       <c r="V171" t="inlineStr"/>
@@ -5591,7 +6263,11 @@
       <c r="P172" t="inlineStr"/>
       <c r="Q172" t="inlineStr"/>
       <c r="R172" t="inlineStr"/>
-      <c r="S172" t="inlineStr"/>
+      <c r="S172" t="inlineStr">
+        <is>
+          <t>CARTUCHO PARA BOMBA DE FUSOS NOTOS MODELO: 3NS-/25-8- (MODELO ANTIGO - COMPRIMENTO MENOR) EXECUÇÃO: HOUSING; MATERIAL: FERRO FUNDIDO GGG-50;  **MEDIR RUGOSIDADE (RMAX=4) DAS PARTES INTERNAS DO CARTUCHO, ONDE SE ALOJAM OS FUSOS, ISSO PARA GARANTIR AS ESPECIFICAÇÕES  DO DESENHO.*</t>
+        </is>
+      </c>
       <c r="T172" t="inlineStr"/>
       <c r="U172" t="inlineStr"/>
       <c r="V172" t="inlineStr"/>

</xml_diff>

<commit_message>
Add Traducoes class for handling narrative translations and update app logic
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W175"/>
+  <dimension ref="A1:Z175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,6 +549,21 @@
           <t>SAP17</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>MAKTX(EN)</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>MAKTX(ES)</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>MAKTX(DE)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -666,6 +681,9 @@
           <t>NORMT (Normbezeichnung)</t>
         </is>
       </c>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -695,6 +713,9 @@
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -728,6 +749,9 @@
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -761,6 +785,9 @@
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -794,6 +821,9 @@
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -827,6 +857,9 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -860,6 +893,9 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -893,6 +929,9 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -926,6 +965,9 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -959,6 +1001,9 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -992,6 +1037,9 @@
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1025,6 +1073,9 @@
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1058,6 +1109,9 @@
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1091,6 +1145,9 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
+      <c r="Z15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1124,6 +1181,9 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1157,6 +1217,9 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
+      <c r="Z17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1190,6 +1253,9 @@
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1223,6 +1289,9 @@
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1256,6 +1325,9 @@
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
+      <c r="Z20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1289,6 +1361,9 @@
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
+      <c r="Z21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1322,6 +1397,9 @@
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
+      <c r="Z22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1355,6 +1433,9 @@
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
+      <c r="Z23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1388,6 +1469,9 @@
       <c r="U24" t="inlineStr"/>
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
+      <c r="Z24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1421,6 +1505,9 @@
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
+      <c r="Z25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1454,6 +1541,9 @@
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
       <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1487,6 +1577,9 @@
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
       <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1520,6 +1613,9 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1553,6 +1649,9 @@
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
       <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1586,6 +1685,9 @@
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
       <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1619,6 +1721,9 @@
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
       <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1652,6 +1757,9 @@
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
       <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
+      <c r="Z32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1685,6 +1793,9 @@
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1718,6 +1829,9 @@
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
       <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
+      <c r="Z34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1751,6 +1865,9 @@
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
       <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1784,6 +1901,9 @@
       <c r="U36" t="inlineStr"/>
       <c r="V36" t="inlineStr"/>
       <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
+      <c r="Z36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1817,6 +1937,9 @@
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
       <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
+      <c r="Z37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1850,6 +1973,9 @@
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="inlineStr"/>
       <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
+      <c r="Z38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1883,6 +2009,9 @@
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
       <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
+      <c r="Z39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1916,6 +2045,9 @@
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
       <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
+      <c r="Z40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1949,6 +2081,9 @@
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
       <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1982,6 +2117,9 @@
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
       <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
+      <c r="Z42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2015,6 +2153,9 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
+      <c r="Z43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2048,6 +2189,9 @@
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr"/>
       <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
+      <c r="Z44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2081,6 +2225,9 @@
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
       <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2114,6 +2261,9 @@
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
       <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr"/>
+      <c r="Z46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2147,6 +2297,9 @@
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
       <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
+      <c r="Z47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2180,6 +2333,9 @@
       <c r="U48" t="inlineStr"/>
       <c r="V48" t="inlineStr"/>
       <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
+      <c r="Z48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2213,6 +2369,9 @@
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
       <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
+      <c r="Z49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2246,6 +2405,9 @@
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
+      <c r="Z50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2279,6 +2441,9 @@
       <c r="U51" t="inlineStr"/>
       <c r="V51" t="inlineStr"/>
       <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
+      <c r="Z51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2312,6 +2477,9 @@
       <c r="U52" t="inlineStr"/>
       <c r="V52" t="inlineStr"/>
       <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
+      <c r="Z52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2345,6 +2513,9 @@
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
       <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr"/>
+      <c r="Z53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2378,6 +2549,9 @@
       <c r="U54" t="inlineStr"/>
       <c r="V54" t="inlineStr"/>
       <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
+      <c r="Z54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2411,6 +2585,9 @@
       <c r="U55" t="inlineStr"/>
       <c r="V55" t="inlineStr"/>
       <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
+      <c r="Z55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2444,6 +2621,9 @@
       <c r="U56" t="inlineStr"/>
       <c r="V56" t="inlineStr"/>
       <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
+      <c r="Z56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2477,6 +2657,9 @@
       <c r="U57" t="inlineStr"/>
       <c r="V57" t="inlineStr"/>
       <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
+      <c r="Z57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2510,6 +2693,9 @@
       <c r="U58" t="inlineStr"/>
       <c r="V58" t="inlineStr"/>
       <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
+      <c r="Z58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2543,6 +2729,9 @@
       <c r="U59" t="inlineStr"/>
       <c r="V59" t="inlineStr"/>
       <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
+      <c r="Z59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2576,6 +2765,9 @@
       <c r="U60" t="inlineStr"/>
       <c r="V60" t="inlineStr"/>
       <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
+      <c r="Z60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2609,6 +2801,9 @@
       <c r="U61" t="inlineStr"/>
       <c r="V61" t="inlineStr"/>
       <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
+      <c r="Z61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2642,6 +2837,9 @@
       <c r="U62" t="inlineStr"/>
       <c r="V62" t="inlineStr"/>
       <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
+      <c r="Z62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2675,6 +2873,9 @@
       <c r="U63" t="inlineStr"/>
       <c r="V63" t="inlineStr"/>
       <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
+      <c r="Z63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2708,6 +2909,9 @@
       <c r="U64" t="inlineStr"/>
       <c r="V64" t="inlineStr"/>
       <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
+      <c r="Z64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2741,6 +2945,9 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" t="inlineStr"/>
       <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
+      <c r="Z65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2774,6 +2981,9 @@
       <c r="U66" t="inlineStr"/>
       <c r="V66" t="inlineStr"/>
       <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr"/>
+      <c r="Y66" t="inlineStr"/>
+      <c r="Z66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2807,6 +3017,9 @@
       <c r="U67" t="inlineStr"/>
       <c r="V67" t="inlineStr"/>
       <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr"/>
+      <c r="Y67" t="inlineStr"/>
+      <c r="Z67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2840,6 +3053,9 @@
       <c r="U68" t="inlineStr"/>
       <c r="V68" t="inlineStr"/>
       <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr"/>
+      <c r="Y68" t="inlineStr"/>
+      <c r="Z68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2873,6 +3089,9 @@
       <c r="U69" t="inlineStr"/>
       <c r="V69" t="inlineStr"/>
       <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
+      <c r="Z69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2906,6 +3125,9 @@
       <c r="U70" t="inlineStr"/>
       <c r="V70" t="inlineStr"/>
       <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
+      <c r="Z70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2939,6 +3161,9 @@
       <c r="U71" t="inlineStr"/>
       <c r="V71" t="inlineStr"/>
       <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
+      <c r="Z71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2972,6 +3197,9 @@
       <c r="U72" t="inlineStr"/>
       <c r="V72" t="inlineStr"/>
       <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
+      <c r="Z72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3005,6 +3233,9 @@
       <c r="U73" t="inlineStr"/>
       <c r="V73" t="inlineStr"/>
       <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
+      <c r="Z73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3038,6 +3269,9 @@
       <c r="U74" t="inlineStr"/>
       <c r="V74" t="inlineStr"/>
       <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr"/>
+      <c r="Y74" t="inlineStr"/>
+      <c r="Z74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3071,6 +3305,9 @@
       <c r="U75" t="inlineStr"/>
       <c r="V75" t="inlineStr"/>
       <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
+      <c r="Z75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3104,6 +3341,9 @@
       <c r="U76" t="inlineStr"/>
       <c r="V76" t="inlineStr"/>
       <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
+      <c r="Z76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3137,6 +3377,9 @@
       <c r="U77" t="inlineStr"/>
       <c r="V77" t="inlineStr"/>
       <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
+      <c r="Z77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3170,6 +3413,9 @@
       <c r="U78" t="inlineStr"/>
       <c r="V78" t="inlineStr"/>
       <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr"/>
+      <c r="Y78" t="inlineStr"/>
+      <c r="Z78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3203,6 +3449,9 @@
       <c r="U79" t="inlineStr"/>
       <c r="V79" t="inlineStr"/>
       <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr"/>
+      <c r="Y79" t="inlineStr"/>
+      <c r="Z79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3236,6 +3485,9 @@
       <c r="U80" t="inlineStr"/>
       <c r="V80" t="inlineStr"/>
       <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr"/>
+      <c r="Y80" t="inlineStr"/>
+      <c r="Z80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3269,6 +3521,9 @@
       <c r="U81" t="inlineStr"/>
       <c r="V81" t="inlineStr"/>
       <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
+      <c r="Z81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3302,6 +3557,9 @@
       <c r="U82" t="inlineStr"/>
       <c r="V82" t="inlineStr"/>
       <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
+      <c r="Z82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3335,6 +3593,9 @@
       <c r="U83" t="inlineStr"/>
       <c r="V83" t="inlineStr"/>
       <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
+      <c r="Z83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3368,6 +3629,9 @@
       <c r="U84" t="inlineStr"/>
       <c r="V84" t="inlineStr"/>
       <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
+      <c r="Z84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3401,6 +3665,9 @@
       <c r="U85" t="inlineStr"/>
       <c r="V85" t="inlineStr"/>
       <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
+      <c r="Z85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3434,6 +3701,9 @@
       <c r="U86" t="inlineStr"/>
       <c r="V86" t="inlineStr"/>
       <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr"/>
+      <c r="Y86" t="inlineStr"/>
+      <c r="Z86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3467,6 +3737,9 @@
       <c r="U87" t="inlineStr"/>
       <c r="V87" t="inlineStr"/>
       <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr"/>
+      <c r="Y87" t="inlineStr"/>
+      <c r="Z87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3500,6 +3773,9 @@
       <c r="U88" t="inlineStr"/>
       <c r="V88" t="inlineStr"/>
       <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr"/>
+      <c r="Y88" t="inlineStr"/>
+      <c r="Z88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3533,6 +3809,9 @@
       <c r="U89" t="inlineStr"/>
       <c r="V89" t="inlineStr"/>
       <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
+      <c r="Z89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3566,6 +3845,9 @@
       <c r="U90" t="inlineStr"/>
       <c r="V90" t="inlineStr"/>
       <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
+      <c r="Z90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3599,6 +3881,9 @@
       <c r="U91" t="inlineStr"/>
       <c r="V91" t="inlineStr"/>
       <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
+      <c r="Z91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3632,6 +3917,9 @@
       <c r="U92" t="inlineStr"/>
       <c r="V92" t="inlineStr"/>
       <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
+      <c r="Z92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3665,6 +3953,9 @@
       <c r="U93" t="inlineStr"/>
       <c r="V93" t="inlineStr"/>
       <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
+      <c r="Z93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3698,6 +3989,9 @@
       <c r="U94" t="inlineStr"/>
       <c r="V94" t="inlineStr"/>
       <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr"/>
+      <c r="Y94" t="inlineStr"/>
+      <c r="Z94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3731,6 +4025,9 @@
       <c r="U95" t="inlineStr"/>
       <c r="V95" t="inlineStr"/>
       <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
+      <c r="Z95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3764,6 +4061,9 @@
       <c r="U96" t="inlineStr"/>
       <c r="V96" t="inlineStr"/>
       <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
+      <c r="Z96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3797,6 +4097,9 @@
       <c r="U97" t="inlineStr"/>
       <c r="V97" t="inlineStr"/>
       <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr"/>
+      <c r="Y97" t="inlineStr"/>
+      <c r="Z97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3830,6 +4133,9 @@
       <c r="U98" t="inlineStr"/>
       <c r="V98" t="inlineStr"/>
       <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr"/>
+      <c r="Y98" t="inlineStr"/>
+      <c r="Z98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3863,6 +4169,9 @@
       <c r="U99" t="inlineStr"/>
       <c r="V99" t="inlineStr"/>
       <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
+      <c r="Z99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3896,6 +4205,9 @@
       <c r="U100" t="inlineStr"/>
       <c r="V100" t="inlineStr"/>
       <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
+      <c r="Z100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3929,6 +4241,9 @@
       <c r="U101" t="inlineStr"/>
       <c r="V101" t="inlineStr"/>
       <c r="W101" t="inlineStr"/>
+      <c r="X101" t="inlineStr"/>
+      <c r="Y101" t="inlineStr"/>
+      <c r="Z101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3962,6 +4277,9 @@
       <c r="U102" t="inlineStr"/>
       <c r="V102" t="inlineStr"/>
       <c r="W102" t="inlineStr"/>
+      <c r="X102" t="inlineStr"/>
+      <c r="Y102" t="inlineStr"/>
+      <c r="Z102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3995,6 +4313,9 @@
       <c r="U103" t="inlineStr"/>
       <c r="V103" t="inlineStr"/>
       <c r="W103" t="inlineStr"/>
+      <c r="X103" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
+      <c r="Z103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4028,6 +4349,9 @@
       <c r="U104" t="inlineStr"/>
       <c r="V104" t="inlineStr"/>
       <c r="W104" t="inlineStr"/>
+      <c r="X104" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
+      <c r="Z104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4061,6 +4385,9 @@
       <c r="U105" t="inlineStr"/>
       <c r="V105" t="inlineStr"/>
       <c r="W105" t="inlineStr"/>
+      <c r="X105" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
+      <c r="Z105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4094,6 +4421,9 @@
       <c r="U106" t="inlineStr"/>
       <c r="V106" t="inlineStr"/>
       <c r="W106" t="inlineStr"/>
+      <c r="X106" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
+      <c r="Z106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4127,6 +4457,9 @@
       <c r="U107" t="inlineStr"/>
       <c r="V107" t="inlineStr"/>
       <c r="W107" t="inlineStr"/>
+      <c r="X107" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
+      <c r="Z107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4160,6 +4493,9 @@
       <c r="U108" t="inlineStr"/>
       <c r="V108" t="inlineStr"/>
       <c r="W108" t="inlineStr"/>
+      <c r="X108" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
+      <c r="Z108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4193,6 +4529,9 @@
       <c r="U109" t="inlineStr"/>
       <c r="V109" t="inlineStr"/>
       <c r="W109" t="inlineStr"/>
+      <c r="X109" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
+      <c r="Z109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4226,6 +4565,9 @@
       <c r="U110" t="inlineStr"/>
       <c r="V110" t="inlineStr"/>
       <c r="W110" t="inlineStr"/>
+      <c r="X110" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
+      <c r="Z110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4259,6 +4601,9 @@
       <c r="U111" t="inlineStr"/>
       <c r="V111" t="inlineStr"/>
       <c r="W111" t="inlineStr"/>
+      <c r="X111" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
+      <c r="Z111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4292,6 +4637,9 @@
       <c r="U112" t="inlineStr"/>
       <c r="V112" t="inlineStr"/>
       <c r="W112" t="inlineStr"/>
+      <c r="X112" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
+      <c r="Z112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4325,6 +4673,9 @@
       <c r="U113" t="inlineStr"/>
       <c r="V113" t="inlineStr"/>
       <c r="W113" t="inlineStr"/>
+      <c r="X113" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
+      <c r="Z113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4358,6 +4709,9 @@
       <c r="U114" t="inlineStr"/>
       <c r="V114" t="inlineStr"/>
       <c r="W114" t="inlineStr"/>
+      <c r="X114" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
+      <c r="Z114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4391,6 +4745,9 @@
       <c r="U115" t="inlineStr"/>
       <c r="V115" t="inlineStr"/>
       <c r="W115" t="inlineStr"/>
+      <c r="X115" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
+      <c r="Z115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4424,6 +4781,9 @@
       <c r="U116" t="inlineStr"/>
       <c r="V116" t="inlineStr"/>
       <c r="W116" t="inlineStr"/>
+      <c r="X116" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
+      <c r="Z116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4457,6 +4817,9 @@
       <c r="U117" t="inlineStr"/>
       <c r="V117" t="inlineStr"/>
       <c r="W117" t="inlineStr"/>
+      <c r="X117" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
+      <c r="Z117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4490,6 +4853,9 @@
       <c r="U118" t="inlineStr"/>
       <c r="V118" t="inlineStr"/>
       <c r="W118" t="inlineStr"/>
+      <c r="X118" t="inlineStr"/>
+      <c r="Y118" t="inlineStr"/>
+      <c r="Z118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4523,6 +4889,9 @@
       <c r="U119" t="inlineStr"/>
       <c r="V119" t="inlineStr"/>
       <c r="W119" t="inlineStr"/>
+      <c r="X119" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
+      <c r="Z119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4556,6 +4925,9 @@
       <c r="U120" t="inlineStr"/>
       <c r="V120" t="inlineStr"/>
       <c r="W120" t="inlineStr"/>
+      <c r="X120" t="inlineStr"/>
+      <c r="Y120" t="inlineStr"/>
+      <c r="Z120" t="inlineStr"/>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4589,6 +4961,9 @@
       <c r="U121" t="inlineStr"/>
       <c r="V121" t="inlineStr"/>
       <c r="W121" t="inlineStr"/>
+      <c r="X121" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
+      <c r="Z121" t="inlineStr"/>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4622,6 +4997,9 @@
       <c r="U122" t="inlineStr"/>
       <c r="V122" t="inlineStr"/>
       <c r="W122" t="inlineStr"/>
+      <c r="X122" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+      <c r="Z122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4655,6 +5033,9 @@
       <c r="U123" t="inlineStr"/>
       <c r="V123" t="inlineStr"/>
       <c r="W123" t="inlineStr"/>
+      <c r="X123" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+      <c r="Z123" t="inlineStr"/>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4688,6 +5069,9 @@
       <c r="U124" t="inlineStr"/>
       <c r="V124" t="inlineStr"/>
       <c r="W124" t="inlineStr"/>
+      <c r="X124" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+      <c r="Z124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4721,6 +5105,9 @@
       <c r="U125" t="inlineStr"/>
       <c r="V125" t="inlineStr"/>
       <c r="W125" t="inlineStr"/>
+      <c r="X125" t="inlineStr"/>
+      <c r="Y125" t="inlineStr"/>
+      <c r="Z125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4754,6 +5141,9 @@
       <c r="U126" t="inlineStr"/>
       <c r="V126" t="inlineStr"/>
       <c r="W126" t="inlineStr"/>
+      <c r="X126" t="inlineStr"/>
+      <c r="Y126" t="inlineStr"/>
+      <c r="Z126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4787,6 +5177,9 @@
       <c r="U127" t="inlineStr"/>
       <c r="V127" t="inlineStr"/>
       <c r="W127" t="inlineStr"/>
+      <c r="X127" t="inlineStr"/>
+      <c r="Y127" t="inlineStr"/>
+      <c r="Z127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4820,6 +5213,9 @@
       <c r="U128" t="inlineStr"/>
       <c r="V128" t="inlineStr"/>
       <c r="W128" t="inlineStr"/>
+      <c r="X128" t="inlineStr"/>
+      <c r="Y128" t="inlineStr"/>
+      <c r="Z128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4853,6 +5249,9 @@
       <c r="U129" t="inlineStr"/>
       <c r="V129" t="inlineStr"/>
       <c r="W129" t="inlineStr"/>
+      <c r="X129" t="inlineStr"/>
+      <c r="Y129" t="inlineStr"/>
+      <c r="Z129" t="inlineStr"/>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4886,6 +5285,9 @@
       <c r="U130" t="inlineStr"/>
       <c r="V130" t="inlineStr"/>
       <c r="W130" t="inlineStr"/>
+      <c r="X130" t="inlineStr"/>
+      <c r="Y130" t="inlineStr"/>
+      <c r="Z130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4919,6 +5321,9 @@
       <c r="U131" t="inlineStr"/>
       <c r="V131" t="inlineStr"/>
       <c r="W131" t="inlineStr"/>
+      <c r="X131" t="inlineStr"/>
+      <c r="Y131" t="inlineStr"/>
+      <c r="Z131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4952,6 +5357,9 @@
       <c r="U132" t="inlineStr"/>
       <c r="V132" t="inlineStr"/>
       <c r="W132" t="inlineStr"/>
+      <c r="X132" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
+      <c r="Z132" t="inlineStr"/>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4985,6 +5393,9 @@
       <c r="U133" t="inlineStr"/>
       <c r="V133" t="inlineStr"/>
       <c r="W133" t="inlineStr"/>
+      <c r="X133" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
+      <c r="Z133" t="inlineStr"/>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5018,6 +5429,9 @@
       <c r="U134" t="inlineStr"/>
       <c r="V134" t="inlineStr"/>
       <c r="W134" t="inlineStr"/>
+      <c r="X134" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
+      <c r="Z134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5051,6 +5465,9 @@
       <c r="U135" t="inlineStr"/>
       <c r="V135" t="inlineStr"/>
       <c r="W135" t="inlineStr"/>
+      <c r="X135" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
+      <c r="Z135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -5084,6 +5501,9 @@
       <c r="U136" t="inlineStr"/>
       <c r="V136" t="inlineStr"/>
       <c r="W136" t="inlineStr"/>
+      <c r="X136" t="inlineStr"/>
+      <c r="Y136" t="inlineStr"/>
+      <c r="Z136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -5117,6 +5537,9 @@
       <c r="U137" t="inlineStr"/>
       <c r="V137" t="inlineStr"/>
       <c r="W137" t="inlineStr"/>
+      <c r="X137" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
+      <c r="Z137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -5150,6 +5573,9 @@
       <c r="U138" t="inlineStr"/>
       <c r="V138" t="inlineStr"/>
       <c r="W138" t="inlineStr"/>
+      <c r="X138" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
+      <c r="Z138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -5183,6 +5609,9 @@
       <c r="U139" t="inlineStr"/>
       <c r="V139" t="inlineStr"/>
       <c r="W139" t="inlineStr"/>
+      <c r="X139" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
+      <c r="Z139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -5216,6 +5645,9 @@
       <c r="U140" t="inlineStr"/>
       <c r="V140" t="inlineStr"/>
       <c r="W140" t="inlineStr"/>
+      <c r="X140" t="inlineStr"/>
+      <c r="Y140" t="inlineStr"/>
+      <c r="Z140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -5249,6 +5681,9 @@
       <c r="U141" t="inlineStr"/>
       <c r="V141" t="inlineStr"/>
       <c r="W141" t="inlineStr"/>
+      <c r="X141" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
+      <c r="Z141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -5282,6 +5717,9 @@
       <c r="U142" t="inlineStr"/>
       <c r="V142" t="inlineStr"/>
       <c r="W142" t="inlineStr"/>
+      <c r="X142" t="inlineStr"/>
+      <c r="Y142" t="inlineStr"/>
+      <c r="Z142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -5315,6 +5753,9 @@
       <c r="U143" t="inlineStr"/>
       <c r="V143" t="inlineStr"/>
       <c r="W143" t="inlineStr"/>
+      <c r="X143" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
+      <c r="Z143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -5348,6 +5789,9 @@
       <c r="U144" t="inlineStr"/>
       <c r="V144" t="inlineStr"/>
       <c r="W144" t="inlineStr"/>
+      <c r="X144" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
+      <c r="Z144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -5381,6 +5825,9 @@
       <c r="U145" t="inlineStr"/>
       <c r="V145" t="inlineStr"/>
       <c r="W145" t="inlineStr"/>
+      <c r="X145" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
+      <c r="Z145" t="inlineStr"/>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -5414,6 +5861,9 @@
       <c r="U146" t="inlineStr"/>
       <c r="V146" t="inlineStr"/>
       <c r="W146" t="inlineStr"/>
+      <c r="X146" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
+      <c r="Z146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5447,6 +5897,9 @@
       <c r="U147" t="inlineStr"/>
       <c r="V147" t="inlineStr"/>
       <c r="W147" t="inlineStr"/>
+      <c r="X147" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
+      <c r="Z147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5480,6 +5933,9 @@
       <c r="U148" t="inlineStr"/>
       <c r="V148" t="inlineStr"/>
       <c r="W148" t="inlineStr"/>
+      <c r="X148" t="inlineStr"/>
+      <c r="Y148" t="inlineStr"/>
+      <c r="Z148" t="inlineStr"/>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5513,6 +5969,9 @@
       <c r="U149" t="inlineStr"/>
       <c r="V149" t="inlineStr"/>
       <c r="W149" t="inlineStr"/>
+      <c r="X149" t="inlineStr"/>
+      <c r="Y149" t="inlineStr"/>
+      <c r="Z149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5546,6 +6005,9 @@
       <c r="U150" t="inlineStr"/>
       <c r="V150" t="inlineStr"/>
       <c r="W150" t="inlineStr"/>
+      <c r="X150" t="inlineStr"/>
+      <c r="Y150" t="inlineStr"/>
+      <c r="Z150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5579,6 +6041,9 @@
       <c r="U151" t="inlineStr"/>
       <c r="V151" t="inlineStr"/>
       <c r="W151" t="inlineStr"/>
+      <c r="X151" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+      <c r="Z151" t="inlineStr"/>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5612,6 +6077,9 @@
       <c r="U152" t="inlineStr"/>
       <c r="V152" t="inlineStr"/>
       <c r="W152" t="inlineStr"/>
+      <c r="X152" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+      <c r="Z152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5645,6 +6113,9 @@
       <c r="U153" t="inlineStr"/>
       <c r="V153" t="inlineStr"/>
       <c r="W153" t="inlineStr"/>
+      <c r="X153" t="inlineStr"/>
+      <c r="Y153" t="inlineStr"/>
+      <c r="Z153" t="inlineStr"/>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5678,6 +6149,9 @@
       <c r="U154" t="inlineStr"/>
       <c r="V154" t="inlineStr"/>
       <c r="W154" t="inlineStr"/>
+      <c r="X154" t="inlineStr"/>
+      <c r="Y154" t="inlineStr"/>
+      <c r="Z154" t="inlineStr"/>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5711,6 +6185,9 @@
       <c r="U155" t="inlineStr"/>
       <c r="V155" t="inlineStr"/>
       <c r="W155" t="inlineStr"/>
+      <c r="X155" t="inlineStr"/>
+      <c r="Y155" t="inlineStr"/>
+      <c r="Z155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5744,6 +6221,9 @@
       <c r="U156" t="inlineStr"/>
       <c r="V156" t="inlineStr"/>
       <c r="W156" t="inlineStr"/>
+      <c r="X156" t="inlineStr"/>
+      <c r="Y156" t="inlineStr"/>
+      <c r="Z156" t="inlineStr"/>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5777,6 +6257,9 @@
       <c r="U157" t="inlineStr"/>
       <c r="V157" t="inlineStr"/>
       <c r="W157" t="inlineStr"/>
+      <c r="X157" t="inlineStr"/>
+      <c r="Y157" t="inlineStr"/>
+      <c r="Z157" t="inlineStr"/>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5810,6 +6293,9 @@
       <c r="U158" t="inlineStr"/>
       <c r="V158" t="inlineStr"/>
       <c r="W158" t="inlineStr"/>
+      <c r="X158" t="inlineStr"/>
+      <c r="Y158" t="inlineStr"/>
+      <c r="Z158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5843,6 +6329,9 @@
       <c r="U159" t="inlineStr"/>
       <c r="V159" t="inlineStr"/>
       <c r="W159" t="inlineStr"/>
+      <c r="X159" t="inlineStr"/>
+      <c r="Y159" t="inlineStr"/>
+      <c r="Z159" t="inlineStr"/>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5876,6 +6365,9 @@
       <c r="U160" t="inlineStr"/>
       <c r="V160" t="inlineStr"/>
       <c r="W160" t="inlineStr"/>
+      <c r="X160" t="inlineStr"/>
+      <c r="Y160" t="inlineStr"/>
+      <c r="Z160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5909,6 +6401,9 @@
       <c r="U161" t="inlineStr"/>
       <c r="V161" t="inlineStr"/>
       <c r="W161" t="inlineStr"/>
+      <c r="X161" t="inlineStr"/>
+      <c r="Y161" t="inlineStr"/>
+      <c r="Z161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5942,6 +6437,9 @@
       <c r="U162" t="inlineStr"/>
       <c r="V162" t="inlineStr"/>
       <c r="W162" t="inlineStr"/>
+      <c r="X162" t="inlineStr"/>
+      <c r="Y162" t="inlineStr"/>
+      <c r="Z162" t="inlineStr"/>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5975,6 +6473,9 @@
       <c r="U163" t="inlineStr"/>
       <c r="V163" t="inlineStr"/>
       <c r="W163" t="inlineStr"/>
+      <c r="X163" t="inlineStr"/>
+      <c r="Y163" t="inlineStr"/>
+      <c r="Z163" t="inlineStr"/>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -6008,6 +6509,9 @@
       <c r="U164" t="inlineStr"/>
       <c r="V164" t="inlineStr"/>
       <c r="W164" t="inlineStr"/>
+      <c r="X164" t="inlineStr"/>
+      <c r="Y164" t="inlineStr"/>
+      <c r="Z164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -6041,6 +6545,9 @@
       <c r="U165" t="inlineStr"/>
       <c r="V165" t="inlineStr"/>
       <c r="W165" t="inlineStr"/>
+      <c r="X165" t="inlineStr"/>
+      <c r="Y165" t="inlineStr"/>
+      <c r="Z165" t="inlineStr"/>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -6074,6 +6581,9 @@
       <c r="U166" t="inlineStr"/>
       <c r="V166" t="inlineStr"/>
       <c r="W166" t="inlineStr"/>
+      <c r="X166" t="inlineStr"/>
+      <c r="Y166" t="inlineStr"/>
+      <c r="Z166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -6107,6 +6617,9 @@
       <c r="U167" t="inlineStr"/>
       <c r="V167" t="inlineStr"/>
       <c r="W167" t="inlineStr"/>
+      <c r="X167" t="inlineStr"/>
+      <c r="Y167" t="inlineStr"/>
+      <c r="Z167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -6140,6 +6653,9 @@
       <c r="U168" t="inlineStr"/>
       <c r="V168" t="inlineStr"/>
       <c r="W168" t="inlineStr"/>
+      <c r="X168" t="inlineStr"/>
+      <c r="Y168" t="inlineStr"/>
+      <c r="Z168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -6173,6 +6689,9 @@
       <c r="U169" t="inlineStr"/>
       <c r="V169" t="inlineStr"/>
       <c r="W169" t="inlineStr"/>
+      <c r="X169" t="inlineStr"/>
+      <c r="Y169" t="inlineStr"/>
+      <c r="Z169" t="inlineStr"/>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -6206,6 +6725,9 @@
       <c r="U170" t="inlineStr"/>
       <c r="V170" t="inlineStr"/>
       <c r="W170" t="inlineStr"/>
+      <c r="X170" t="inlineStr"/>
+      <c r="Y170" t="inlineStr"/>
+      <c r="Z170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -6239,6 +6761,9 @@
       <c r="U171" t="inlineStr"/>
       <c r="V171" t="inlineStr"/>
       <c r="W171" t="inlineStr"/>
+      <c r="X171" t="inlineStr"/>
+      <c r="Y171" t="inlineStr"/>
+      <c r="Z171" t="inlineStr"/>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -6272,6 +6797,9 @@
       <c r="U172" t="inlineStr"/>
       <c r="V172" t="inlineStr"/>
       <c r="W172" t="inlineStr"/>
+      <c r="X172" t="inlineStr"/>
+      <c r="Y172" t="inlineStr"/>
+      <c r="Z172" t="inlineStr"/>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -6301,6 +6829,9 @@
       <c r="U173" t="inlineStr"/>
       <c r="V173" t="inlineStr"/>
       <c r="W173" t="inlineStr"/>
+      <c r="X173" t="inlineStr"/>
+      <c r="Y173" t="inlineStr"/>
+      <c r="Z173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -6330,6 +6861,9 @@
       <c r="U174" t="inlineStr"/>
       <c r="V174" t="inlineStr"/>
       <c r="W174" t="inlineStr"/>
+      <c r="X174" t="inlineStr"/>
+      <c r="Y174" t="inlineStr"/>
+      <c r="Z174" t="inlineStr"/>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -6359,6 +6893,9 @@
       <c r="U175" t="inlineStr"/>
       <c r="V175" t="inlineStr"/>
       <c r="W175" t="inlineStr"/>
+      <c r="X175" t="inlineStr"/>
+      <c r="Y175" t="inlineStr"/>
+      <c r="Z175" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Refactor material and norms insertion functions; update SAP6 and SAP17 processing logic
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -601,9 +601,19 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>SPECIAL</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>FAF37-DRN90LP4</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -636,6 +646,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>MG-SG</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -676,9 +691,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>MG-M</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>SIC</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -716,9 +736,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>MG-M</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>SIC</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -756,6 +781,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -796,9 +826,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>MG-KGM</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -836,14 +871,19 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NETZSCH</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -876,6 +916,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -916,6 +961,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>MG-M</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>PRINCIPAL</t>
@@ -956,6 +1006,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -996,6 +1051,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1036,6 +1096,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1076,6 +1141,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1116,6 +1186,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1156,6 +1231,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1196,6 +1276,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1236,6 +1321,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -1276,6 +1366,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1316,6 +1411,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1356,6 +1456,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1396,6 +1501,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1436,6 +1546,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1476,6 +1591,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1516,6 +1636,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1556,6 +1681,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1596,6 +1726,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -1636,6 +1771,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -1676,6 +1816,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1716,6 +1861,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1756,6 +1906,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1796,6 +1951,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1836,6 +1996,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1876,6 +2041,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1916,6 +2086,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1956,6 +2131,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1996,6 +2176,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>MG-M</t>
+        </is>
+      </c>
       <c r="K38" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -2036,6 +2221,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K39" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2076,6 +2266,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K40" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2116,6 +2311,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2156,6 +2356,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2196,6 +2401,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2236,6 +2446,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K44" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -2276,6 +2491,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K45" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -2316,6 +2536,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2356,6 +2581,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2396,6 +2626,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K48" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2436,6 +2671,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K49" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2476,6 +2716,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>MG-SG</t>
+        </is>
+      </c>
       <c r="K50" t="inlineStr">
         <is>
           <t>St</t>
@@ -2516,9 +2761,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>MG-KGM</t>
+        </is>
+      </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -2556,9 +2806,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>MG-KGM</t>
+        </is>
+      </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -2596,6 +2851,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K53" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2636,6 +2896,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>A-ZUB</t>
+        </is>
+      </c>
       <c r="K54" t="inlineStr">
         <is>
           <t>BRONZE</t>
@@ -2676,6 +2941,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K55" t="inlineStr">
         <is>
           <t>281</t>
@@ -2716,6 +2986,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K56" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -2723,7 +2998,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>PERIPRO</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -2756,9 +3031,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>MG-SGM</t>
+        </is>
+      </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>EL</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -2796,6 +3076,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>MG-KGM</t>
+        </is>
+      </c>
       <c r="K58" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -2836,6 +3121,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K59" t="inlineStr">
         <is>
           <t>AISI 304L FLANGE CFE</t>
@@ -2876,6 +3166,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
       <c r="K60" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -2883,7 +3178,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NM031BH</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -2916,6 +3211,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K61" t="inlineStr">
         <is>
           <t>NEMOLAST S459</t>
@@ -2956,6 +3256,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K62" t="inlineStr">
         <is>
           <t>TELA: TELA 1008</t>
@@ -2996,6 +3301,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K63" t="inlineStr">
         <is>
           <t>AISI 316    P</t>
@@ -3036,6 +3346,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K64" t="inlineStr">
         <is>
           <t>NEMOLAST S61M</t>
@@ -3076,6 +3391,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K65" t="inlineStr">
         <is>
           <t>NEMOLAST S41</t>
@@ -3116,6 +3436,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K66" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -3156,6 +3481,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K67" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -3196,6 +3526,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>PCP-NDHP</t>
+        </is>
+      </c>
       <c r="K68" t="inlineStr">
         <is>
           <t>A-36</t>
@@ -3236,6 +3571,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>PCP-NDHP</t>
+        </is>
+      </c>
       <c r="K69" t="inlineStr">
         <is>
           <t>A-36</t>
@@ -3276,6 +3616,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K70" t="inlineStr">
         <is>
           <t>NEMOLAST S61M</t>
@@ -3316,6 +3661,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K71" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3356,6 +3706,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K72" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3396,6 +3751,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K73" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3436,6 +3796,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K74" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3476,6 +3841,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K75" t="inlineStr">
         <is>
           <t>AISI 316.</t>
@@ -3516,6 +3886,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K76" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3556,6 +3931,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K77" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3596,6 +3976,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K78" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3636,6 +4021,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>HMSP-P</t>
+        </is>
+      </c>
       <c r="K79" t="inlineStr">
         <is>
           <t>SAE 1045</t>
@@ -3676,6 +4066,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>PM-BT</t>
+        </is>
+      </c>
       <c r="K80" t="inlineStr">
         <is>
           <t>ROTOR</t>
@@ -3716,6 +4111,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>HMSP-P</t>
+        </is>
+      </c>
       <c r="K81" t="inlineStr">
         <is>
           <t>AISI 304 P</t>
@@ -3756,6 +4156,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K82" t="inlineStr">
         <is>
           <t>SAE 1020 C</t>
@@ -3763,7 +4168,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>ASME B16.5</t>
+          <t>2NS-/16H3-</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
@@ -3796,6 +4201,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K83" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -3803,7 +4213,7 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>HJ977GN</t>
         </is>
       </c>
       <c r="M83" t="inlineStr">
@@ -3836,6 +4246,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>TXB-ET</t>
+        </is>
+      </c>
       <c r="K84" t="inlineStr">
         <is>
           <t>SAE 1020  P</t>
@@ -3876,6 +4291,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K85" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -3916,6 +4336,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K86" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -3956,6 +4381,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K87" t="inlineStr">
         <is>
           <t>SAE 1020;</t>
@@ -3996,6 +4426,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K88" t="inlineStr">
         <is>
           <t>20MNCR5</t>
@@ -4036,6 +4471,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K89" t="inlineStr">
         <is>
           <t>TOOLOX 44</t>
@@ -4076,6 +4516,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K90" t="inlineStr">
         <is>
           <t>EN 1563 EN GJS 500 7</t>
@@ -4116,6 +4561,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>TXLB-ET</t>
+        </is>
+      </c>
       <c r="K91" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -4156,6 +4606,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>TXLB-ET</t>
+        </is>
+      </c>
       <c r="K92" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -4196,6 +4651,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K93" t="inlineStr">
         <is>
           <t>AISI 304  C</t>
@@ -4236,6 +4696,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K94" t="inlineStr">
         <is>
           <t>AISI304L</t>
@@ -4243,7 +4708,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>MG1-G60</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
@@ -4276,6 +4741,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K95" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -4316,6 +4786,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>A-ZUB</t>
+        </is>
+      </c>
       <c r="K96" t="inlineStr">
         <is>
           <t>Aço Carbono</t>
@@ -4356,6 +4831,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K97" t="inlineStr">
         <is>
           <t>SAE 1045</t>
@@ -4396,6 +4876,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K98" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -4436,6 +4921,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
       <c r="K99" t="inlineStr">
         <is>
           <t>A-36;</t>
@@ -4476,6 +4966,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K100" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -4516,6 +5011,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>PCP-NDHP</t>
+        </is>
+      </c>
       <c r="K101" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -4556,6 +5056,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>NMBY</t>
+        </is>
+      </c>
       <c r="K102" t="inlineStr">
         <is>
           <t>INOX 316 P</t>
@@ -4596,9 +5101,14 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>ACO</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -4636,6 +5146,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K104" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -4676,6 +5191,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K105" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -4716,6 +5236,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K106" t="inlineStr">
         <is>
           <t>NEMOLAST S05G</t>
@@ -4756,6 +5281,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K107" t="inlineStr">
         <is>
           <t>NEMOLAST S63</t>
@@ -4796,6 +5326,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>NE-STA</t>
+        </is>
+      </c>
       <c r="K108" t="inlineStr">
         <is>
           <t>NEMOLAST S61H</t>
@@ -4836,6 +5371,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K109" t="inlineStr">
         <is>
           <t>1020</t>
@@ -4876,6 +5416,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
       <c r="K110" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -4916,6 +5461,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K111" t="inlineStr">
         <is>
           <t>GG-25</t>
@@ -4956,6 +5506,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>NE-STA</t>
+        </is>
+      </c>
       <c r="K112" t="inlineStr">
         <is>
           <t>NEMOLAST S61H</t>
@@ -5076,6 +5631,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>PBDD-ET</t>
+        </is>
+      </c>
       <c r="K115" t="inlineStr">
         <is>
           <t>1.4201</t>
@@ -5116,6 +5676,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>A-DIC</t>
+        </is>
+      </c>
       <c r="K116" t="inlineStr">
         <is>
           <t>PERBUNAN</t>
@@ -5156,6 +5721,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>PBCM-ET</t>
+        </is>
+      </c>
       <c r="K117" t="inlineStr">
         <is>
           <t>PTFE</t>
@@ -5196,6 +5766,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>A-VT</t>
+        </is>
+      </c>
       <c r="K118" t="inlineStr">
         <is>
           <t>A2-70 (304)</t>
@@ -5236,6 +5811,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K119" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5276,6 +5856,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K120" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5316,6 +5901,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>HT-FL</t>
+        </is>
+      </c>
       <c r="K121" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5356,6 +5946,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>AUB</t>
+        </is>
+      </c>
       <c r="K122" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -5396,6 +5991,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>NM-ROT</t>
+        </is>
+      </c>
       <c r="K123" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -5436,6 +6036,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>HB</t>
+        </is>
+      </c>
       <c r="K124" t="inlineStr">
         <is>
           <t>SAE 1020 P</t>
@@ -5476,6 +6081,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K125" t="inlineStr">
         <is>
           <t>DIN EN 1563 EN GJS 500 7</t>
@@ -5651,6 +6261,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>NE-RT</t>
+        </is>
+      </c>
       <c r="K129" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5658,7 +6273,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -5691,6 +6306,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>NE-RT</t>
+        </is>
+      </c>
       <c r="K130" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -5731,6 +6351,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K131" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5851,6 +6476,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>NE-GH</t>
+        </is>
+      </c>
       <c r="K134" t="inlineStr">
         <is>
           <t>AISI 304 P</t>
@@ -5858,7 +6488,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NEC 60A</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
@@ -5898,7 +6528,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NEC 60A</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
@@ -5931,6 +6561,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I136" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K136" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5971,6 +6606,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I137" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K137" t="inlineStr">
         <is>
           <t>AISI 304 C</t>
@@ -6011,6 +6651,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I138" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K138" t="inlineStr">
         <is>
           <t>AISI 316 P</t>
@@ -6091,6 +6736,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I140" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K140" t="inlineStr">
         <is>
           <t>AISI 316L</t>
@@ -6131,6 +6781,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I141" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K141" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6211,6 +6866,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I143" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K143" t="inlineStr">
         <is>
           <t>AISI 316 C</t>
@@ -6251,6 +6911,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I144" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K144" t="inlineStr">
         <is>
           <t>AISI 316L</t>
@@ -6291,6 +6956,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I145" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K145" t="inlineStr">
         <is>
           <t>AISI 420</t>
@@ -6331,6 +7001,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I146" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K146" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6371,6 +7046,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I147" t="inlineStr">
+        <is>
+          <t>NM-STA</t>
+        </is>
+      </c>
       <c r="K147" t="inlineStr">
         <is>
           <t>VI-65/Alu</t>
@@ -6418,7 +7098,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>NM105-T---</t>
+          <t>ANSI B16.5</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
@@ -6451,6 +7131,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K149" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO GG-30</t>
@@ -6491,6 +7176,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I150" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K150" t="inlineStr">
         <is>
           <t>vesconite hilube</t>
@@ -6531,6 +7221,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I151" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K151" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -6571,6 +7266,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I152" t="inlineStr">
+        <is>
+          <t>PCP-NDHP</t>
+        </is>
+      </c>
       <c r="K152" t="inlineStr">
         <is>
           <t>AÇO MOLA HRC-46</t>
@@ -6611,6 +7311,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I153" t="inlineStr">
+        <is>
+          <t>PCP-NDHP</t>
+        </is>
+      </c>
       <c r="K153" t="inlineStr">
         <is>
           <t>AÇO MOLA HRC-46</t>
@@ -6651,6 +7356,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I154" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K154" t="inlineStr">
         <is>
           <t>UNS S31803</t>
@@ -6691,6 +7401,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I155" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K155" t="inlineStr">
         <is>
           <t>DIN EN 1563 EN GJS 500 7</t>
@@ -6778,7 +7493,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>2</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -6811,6 +7526,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I158" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K158" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6891,6 +7611,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>NM-GH</t>
+        </is>
+      </c>
       <c r="K160" t="inlineStr">
         <is>
           <t>AISI 304 C</t>
@@ -6931,6 +7656,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I161" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K161" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6971,6 +7701,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I162" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K162" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7011,6 +7746,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I163" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K163" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7051,6 +7791,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I164" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K164" t="inlineStr">
         <is>
           <t>AISI 420</t>
@@ -7131,6 +7876,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I166" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K166" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -7171,6 +7921,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I167" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K167" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -7211,6 +7966,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I168" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K168" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -7251,6 +8011,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I169" t="inlineStr">
+        <is>
+          <t>MSP3S25</t>
+        </is>
+      </c>
       <c r="K169" t="inlineStr">
         <is>
           <t>SCREW</t>
@@ -7291,6 +8056,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I170" t="inlineStr">
+        <is>
+          <t>NM-RT</t>
+        </is>
+      </c>
       <c r="K170" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7331,6 +8101,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="I171" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
+        </is>
+      </c>
       <c r="K171" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -7369,6 +8144,11 @@
       <c r="D172" t="inlineStr">
         <is>
           <t>NDB</t>
+        </is>
+      </c>
+      <c r="I172" t="inlineStr">
+        <is>
+          <t>MSP-P</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">

</xml_diff>

<commit_message>
Add alias for inserir_size_dimension in inserir_narrativas.py for compatibility
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -606,6 +606,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K3" t="inlineStr">
         <is>
           <t>SPECIAL</t>
@@ -651,6 +656,11 @@
           <t>MG-SG</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>NM063</t>
+        </is>
+      </c>
       <c r="K4" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -696,6 +706,11 @@
           <t>MG-M</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K5" t="inlineStr">
         <is>
           <t>SIC</t>
@@ -741,6 +756,11 @@
           <t>MG-M</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K6" t="inlineStr">
         <is>
           <t>SIC</t>
@@ -786,6 +806,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K7" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -831,9 +856,14 @@
           <t>MG-KGM</t>
         </is>
       </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>332</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -876,14 +906,19 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>332</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -921,6 +956,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>250MM</t>
+        </is>
+      </c>
       <c r="K10" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -966,6 +1006,11 @@
           <t>MG-M</t>
         </is>
       </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K11" t="inlineStr">
         <is>
           <t>PRINCIPAL</t>
@@ -1011,6 +1056,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K12" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1056,6 +1106,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K13" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1101,6 +1156,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1146,6 +1206,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K15" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1191,6 +1256,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K16" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1236,6 +1306,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K17" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1281,6 +1356,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K18" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1326,6 +1406,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K19" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -1371,6 +1456,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1416,6 +1506,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K21" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1461,6 +1556,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K22" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1506,6 +1606,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K23" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1551,6 +1656,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K24" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1596,6 +1706,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K25" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1641,6 +1756,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K26" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1686,6 +1806,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K27" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1731,6 +1856,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K28" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -1776,6 +1906,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K29" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -1821,6 +1956,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K30" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -1866,6 +2006,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K31" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1911,6 +2056,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K32" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -1956,6 +2106,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K33" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2001,6 +2156,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K34" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2046,6 +2206,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K35" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2091,6 +2256,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K36" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2136,6 +2306,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K37" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2181,6 +2356,11 @@
           <t>MG-M</t>
         </is>
       </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K38" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -2226,6 +2406,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K39" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2271,6 +2456,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
       <c r="K40" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2316,6 +2506,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K41" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2361,6 +2556,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K42" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2406,6 +2606,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
       <c r="K43" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2451,6 +2656,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K44" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -2496,6 +2706,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1.1/2"</t>
+        </is>
+      </c>
       <c r="K45" t="inlineStr">
         <is>
           <t>ASTM A182 GR F316L</t>
@@ -2541,6 +2756,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K46" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2586,6 +2806,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K47" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2631,6 +2856,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K48" t="inlineStr">
         <is>
           <t>ASTM A182</t>
@@ -2676,6 +2906,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K49" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2721,6 +2956,11 @@
           <t>MG-SG</t>
         </is>
       </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>NM031</t>
+        </is>
+      </c>
       <c r="K50" t="inlineStr">
         <is>
           <t>St</t>
@@ -2766,9 +3006,14 @@
           <t>MG-KGM</t>
         </is>
       </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>332</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -2811,9 +3056,14 @@
           <t>MG-KGM</t>
         </is>
       </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>332</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -2856,6 +3106,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K53" t="inlineStr">
         <is>
           <t>ASTM A105</t>
@@ -2901,6 +3156,11 @@
           <t>A-ZUB</t>
         </is>
       </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>NPT</t>
+        </is>
+      </c>
       <c r="K54" t="inlineStr">
         <is>
           <t>BRONZE</t>
@@ -2946,6 +3206,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>NM011</t>
+        </is>
+      </c>
       <c r="K55" t="inlineStr">
         <is>
           <t>281</t>
@@ -2991,6 +3256,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K56" t="inlineStr">
         <is>
           <t>Grau D</t>
@@ -2998,7 +3268,7 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>PERIPRO</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M56" t="inlineStr">
@@ -3036,6 +3306,11 @@
           <t>MG-SGM</t>
         </is>
       </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>NM076</t>
+        </is>
+      </c>
       <c r="K57" t="inlineStr">
         <is>
           <t>St</t>
@@ -3081,6 +3356,11 @@
           <t>MG-KGM</t>
         </is>
       </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K58" t="inlineStr">
         <is>
           <t>CAR</t>
@@ -3126,6 +3406,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>NM105</t>
+        </is>
+      </c>
       <c r="K59" t="inlineStr">
         <is>
           <t>AISI 304L FLANGE CFE</t>
@@ -3171,6 +3456,11 @@
           <t>AUB</t>
         </is>
       </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K60" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -3178,7 +3468,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>NM031BH</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -3216,6 +3506,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K61" t="inlineStr">
         <is>
           <t>NEMOLAST S459</t>
@@ -3261,6 +3556,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>NM038</t>
+        </is>
+      </c>
       <c r="K62" t="inlineStr">
         <is>
           <t>TELA: TELA 1008</t>
@@ -3306,6 +3606,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>G=1/4"NPT</t>
+        </is>
+      </c>
       <c r="K63" t="inlineStr">
         <is>
           <t>AISI 316    P</t>
@@ -3351,6 +3656,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>NM045</t>
+        </is>
+      </c>
       <c r="K64" t="inlineStr">
         <is>
           <t>NEMOLAST S61M</t>
@@ -3396,6 +3706,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>NM063</t>
+        </is>
+      </c>
       <c r="K65" t="inlineStr">
         <is>
           <t>NEMOLAST S41</t>
@@ -3441,6 +3756,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K66" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -3486,6 +3806,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K67" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -3531,6 +3856,11 @@
           <t>PCP-NDHP</t>
         </is>
       </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
       <c r="K68" t="inlineStr">
         <is>
           <t>A-36</t>
@@ -3576,6 +3906,11 @@
           <t>PCP-NDHP</t>
         </is>
       </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
       <c r="K69" t="inlineStr">
         <is>
           <t>A-36</t>
@@ -3621,6 +3956,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K70" t="inlineStr">
         <is>
           <t>NEMOLAST S61M</t>
@@ -3666,6 +4006,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>DN1</t>
+        </is>
+      </c>
       <c r="K71" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3711,6 +4056,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>DN10</t>
+        </is>
+      </c>
       <c r="K72" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3756,6 +4106,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>DN4</t>
+        </is>
+      </c>
       <c r="K73" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3801,6 +4156,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>DN8</t>
+        </is>
+      </c>
       <c r="K74" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3846,6 +4206,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>3/4" NPT</t>
+        </is>
+      </c>
       <c r="K75" t="inlineStr">
         <is>
           <t>AISI 316.</t>
@@ -3891,6 +4256,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>DN12</t>
+        </is>
+      </c>
       <c r="K76" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3936,6 +4306,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K77" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -3981,6 +4356,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K78" t="inlineStr">
         <is>
           <t>ASTM A106.</t>
@@ -4026,6 +4406,11 @@
           <t>HMSP-P</t>
         </is>
       </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
       <c r="K79" t="inlineStr">
         <is>
           <t>SAE 1045</t>
@@ -4071,6 +4456,11 @@
           <t>PM-BT</t>
         </is>
       </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Show-room</t>
+        </is>
+      </c>
       <c r="K80" t="inlineStr">
         <is>
           <t>ROTOR</t>
@@ -4116,6 +4506,11 @@
           <t>HMSP-P</t>
         </is>
       </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>DN 32</t>
+        </is>
+      </c>
       <c r="K81" t="inlineStr">
         <is>
           <t>AISI 304 P</t>
@@ -4161,6 +4556,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>1/2" NPT</t>
+        </is>
+      </c>
       <c r="K82" t="inlineStr">
         <is>
           <t>SAE 1020 C</t>
@@ -4206,6 +4606,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K83" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -4251,6 +4656,11 @@
           <t>TXB-ET</t>
         </is>
       </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>facelift</t>
+        </is>
+      </c>
       <c r="K84" t="inlineStr">
         <is>
           <t>SAE 1020  P</t>
@@ -4296,6 +4706,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K85" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -4341,6 +4756,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K86" t="inlineStr">
         <is>
           <t>DUPLEX UNS S31803</t>
@@ -4386,6 +4806,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>3/4" NPT</t>
+        </is>
+      </c>
       <c r="K87" t="inlineStr">
         <is>
           <t>SAE 1020;</t>
@@ -4431,6 +4856,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>MANCAL: 3</t>
+        </is>
+      </c>
       <c r="K88" t="inlineStr">
         <is>
           <t>20MNCR5</t>
@@ -4476,6 +4906,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>MANCAL: 2</t>
+        </is>
+      </c>
       <c r="K89" t="inlineStr">
         <is>
           <t>TOOLOX 44</t>
@@ -4521,6 +4956,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>1/2" BSP</t>
+        </is>
+      </c>
       <c r="K90" t="inlineStr">
         <is>
           <t>EN 1563 EN GJS 500 7</t>
@@ -4566,6 +5006,11 @@
           <t>TXLB-ET</t>
         </is>
       </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K91" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -4611,6 +5056,11 @@
           <t>TXLB-ET</t>
         </is>
       </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K92" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -4656,6 +5106,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K93" t="inlineStr">
         <is>
           <t>AISI 304  C</t>
@@ -4701,6 +5156,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>G=1/4" NPT</t>
+        </is>
+      </c>
       <c r="K94" t="inlineStr">
         <is>
           <t>AISI304L</t>
@@ -4746,6 +5206,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K95" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -4791,6 +5256,11 @@
           <t>A-ZUB</t>
         </is>
       </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
       <c r="K96" t="inlineStr">
         <is>
           <t>Aço Carbono</t>
@@ -4836,6 +5306,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K97" t="inlineStr">
         <is>
           <t>SAE 1045</t>
@@ -4881,6 +5356,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K98" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -4926,6 +5406,11 @@
           <t>AUB</t>
         </is>
       </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K99" t="inlineStr">
         <is>
           <t>A-36;</t>
@@ -4971,6 +5456,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K100" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -5016,6 +5506,11 @@
           <t>PCP-NDHP</t>
         </is>
       </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K101" t="inlineStr">
         <is>
           <t>SAE 4140</t>
@@ -5061,6 +5556,11 @@
           <t>NMBY</t>
         </is>
       </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>UNS-SEAL 100</t>
+        </is>
+      </c>
       <c r="K102" t="inlineStr">
         <is>
           <t>INOX 316 P</t>
@@ -5106,9 +5606,14 @@
           <t>AUB</t>
         </is>
       </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>CAR</t>
+          <t>ACO</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -5151,6 +5656,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>NM038</t>
+        </is>
+      </c>
       <c r="K104" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5196,6 +5706,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>NM076</t>
+        </is>
+      </c>
       <c r="K105" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5241,6 +5756,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>NM090</t>
+        </is>
+      </c>
       <c r="K106" t="inlineStr">
         <is>
           <t>NEMOLAST S05G</t>
@@ -5286,6 +5806,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>NM063</t>
+        </is>
+      </c>
       <c r="K107" t="inlineStr">
         <is>
           <t>NEMOLAST S63</t>
@@ -5331,6 +5856,11 @@
           <t>NE-STA</t>
         </is>
       </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K108" t="inlineStr">
         <is>
           <t>NEMOLAST S61H</t>
@@ -5376,6 +5906,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>NM090</t>
+        </is>
+      </c>
       <c r="K109" t="inlineStr">
         <is>
           <t>1020</t>
@@ -5421,6 +5956,11 @@
           <t>AUB</t>
         </is>
       </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>S/L/P(WP)</t>
+        </is>
+      </c>
       <c r="K110" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -5466,6 +6006,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>DN 2</t>
+        </is>
+      </c>
       <c r="K111" t="inlineStr">
         <is>
           <t>GG-25</t>
@@ -5511,6 +6056,11 @@
           <t>NE-STA</t>
         </is>
       </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
       <c r="K112" t="inlineStr">
         <is>
           <t>NEMOLAST S61H</t>
@@ -5551,6 +6101,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>50A</t>
+        </is>
+      </c>
       <c r="K113" t="inlineStr">
         <is>
           <t>304</t>
@@ -5591,6 +6146,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
       <c r="K114" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -5636,6 +6196,11 @@
           <t>PBDD-ET</t>
         </is>
       </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>D=25</t>
+        </is>
+      </c>
       <c r="K115" t="inlineStr">
         <is>
           <t>1.4201</t>
@@ -5681,6 +6246,11 @@
           <t>A-DIC</t>
         </is>
       </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>1/2"</t>
+        </is>
+      </c>
       <c r="K116" t="inlineStr">
         <is>
           <t>PERBUNAN</t>
@@ -5726,6 +6296,11 @@
           <t>PBCM-ET</t>
         </is>
       </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
       <c r="K117" t="inlineStr">
         <is>
           <t>PTFE</t>
@@ -5771,6 +6346,11 @@
           <t>A-VT</t>
         </is>
       </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>M24</t>
+        </is>
+      </c>
       <c r="K118" t="inlineStr">
         <is>
           <t>A2-70 (304)</t>
@@ -5816,6 +6396,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K119" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5861,6 +6446,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>DN 100</t>
+        </is>
+      </c>
       <c r="K120" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5906,6 +6496,11 @@
           <t>HT-FL</t>
         </is>
       </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>DN 100</t>
+        </is>
+      </c>
       <c r="K121" t="inlineStr">
         <is>
           <t>CFE. ASTM A 105.</t>
@@ -5951,6 +6546,11 @@
           <t>AUB</t>
         </is>
       </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
       <c r="K122" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -5996,6 +6596,11 @@
           <t>NM-ROT</t>
         </is>
       </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K123" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6041,6 +6646,11 @@
           <t>HB</t>
         </is>
       </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
       <c r="K124" t="inlineStr">
         <is>
           <t>SAE 1020 P</t>
@@ -6086,6 +6696,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K125" t="inlineStr">
         <is>
           <t>DIN EN 1563 EN GJS 500 7</t>
@@ -6131,6 +6746,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>NM076</t>
+        </is>
+      </c>
       <c r="K126" t="inlineStr">
         <is>
           <t>NEMOLAST S41</t>
@@ -6176,6 +6796,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>NM045</t>
+        </is>
+      </c>
       <c r="K127" t="inlineStr">
         <is>
           <t>NEMOLAST S45</t>
@@ -6221,6 +6846,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>NM045</t>
+        </is>
+      </c>
       <c r="K128" t="inlineStr">
         <is>
           <t>NEMOLAST S45</t>
@@ -6266,6 +6896,11 @@
           <t>NE-RT</t>
         </is>
       </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>60A</t>
+        </is>
+      </c>
       <c r="K129" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6273,7 +6908,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -6311,6 +6946,11 @@
           <t>NE-RT</t>
         </is>
       </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>40A</t>
+        </is>
+      </c>
       <c r="K130" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6356,6 +6996,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>NM105</t>
+        </is>
+      </c>
       <c r="K131" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6396,6 +7041,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>40A</t>
+        </is>
+      </c>
       <c r="K132" t="inlineStr">
         <is>
           <t>AISI 304.</t>
@@ -6436,6 +7086,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
       <c r="K133" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6481,6 +7136,11 @@
           <t>NE-GH</t>
         </is>
       </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K134" t="inlineStr">
         <is>
           <t>AISI 304 P</t>
@@ -6521,6 +7181,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K135" t="inlineStr">
         <is>
           <t>AISI 304.</t>
@@ -6566,6 +7231,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K136" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6611,6 +7281,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>2.1/2"SMS</t>
+        </is>
+      </c>
       <c r="K137" t="inlineStr">
         <is>
           <t>AISI 304 C</t>
@@ -6656,6 +7331,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>NM038</t>
+        </is>
+      </c>
       <c r="K138" t="inlineStr">
         <is>
           <t>AISI 316 P</t>
@@ -6696,6 +7376,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>750 X 220</t>
+        </is>
+      </c>
       <c r="K139" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -6741,6 +7426,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K140" t="inlineStr">
         <is>
           <t>AISI 316L</t>
@@ -6786,6 +7476,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>NM031</t>
+        </is>
+      </c>
       <c r="K141" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6826,6 +7521,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>NM076</t>
+        </is>
+      </c>
       <c r="K142" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -6871,6 +7571,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>1.1/4"</t>
+        </is>
+      </c>
       <c r="K143" t="inlineStr">
         <is>
           <t>AISI 316 C</t>
@@ -6916,6 +7621,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>NM031</t>
+        </is>
+      </c>
       <c r="K144" t="inlineStr">
         <is>
           <t>AISI 316L</t>
@@ -6961,6 +7671,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>NM038</t>
+        </is>
+      </c>
       <c r="K145" t="inlineStr">
         <is>
           <t>AISI 420</t>
@@ -7006,6 +7721,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>104 X 204</t>
+        </is>
+      </c>
       <c r="K146" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -7051,6 +7771,11 @@
           <t>NM-STA</t>
         </is>
       </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K147" t="inlineStr">
         <is>
           <t>VI-65/Alu</t>
@@ -7091,6 +7816,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>800mm</t>
+        </is>
+      </c>
       <c r="K148" t="inlineStr">
         <is>
           <t>SAE 1020.</t>
@@ -7098,7 +7828,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>ANSI B16.5</t>
+          <t>NM105-T---</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
@@ -7136,6 +7866,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K149" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO GG-30</t>
@@ -7181,6 +7916,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>2NS -</t>
+        </is>
+      </c>
       <c r="K150" t="inlineStr">
         <is>
           <t>vesconite hilube</t>
@@ -7226,6 +7966,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K151" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -7271,6 +8016,11 @@
           <t>PCP-NDHP</t>
         </is>
       </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>M24 x 120,00mm</t>
+        </is>
+      </c>
       <c r="K152" t="inlineStr">
         <is>
           <t>AÇO MOLA HRC-46</t>
@@ -7316,6 +8066,11 @@
           <t>PCP-NDHP</t>
         </is>
       </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>M24 x 120,00mm</t>
+        </is>
+      </c>
       <c r="K153" t="inlineStr">
         <is>
           <t>AÇO MOLA HRC-46</t>
@@ -7361,6 +8116,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>NM105</t>
+        </is>
+      </c>
       <c r="K154" t="inlineStr">
         <is>
           <t>UNS S31803</t>
@@ -7406,6 +8166,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K155" t="inlineStr">
         <is>
           <t>DIN EN 1563 EN GJS 500 7</t>
@@ -7446,6 +8211,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K156" t="inlineStr">
         <is>
           <t>DIN EN 1563 EN GJS 500 7</t>
@@ -7486,6 +8256,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>70mm</t>
+        </is>
+      </c>
       <c r="K157" t="inlineStr">
         <is>
           <t>NBR C</t>
@@ -7493,7 +8268,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>D</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -7531,6 +8306,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>154 X 254</t>
+        </is>
+      </c>
       <c r="K158" t="inlineStr">
         <is>
           <t>AISI 316</t>
@@ -7571,6 +8351,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>G=1"NPT</t>
+        </is>
+      </c>
       <c r="K159" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -7616,6 +8401,11 @@
           <t>NM-GH</t>
         </is>
       </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>NM038</t>
+        </is>
+      </c>
       <c r="K160" t="inlineStr">
         <is>
           <t>AISI 304 C</t>
@@ -7661,6 +8451,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>200MM</t>
+        </is>
+      </c>
       <c r="K161" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7706,6 +8501,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K162" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7751,6 +8551,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K163" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -7796,6 +8601,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>NM105</t>
+        </is>
+      </c>
       <c r="K164" t="inlineStr">
         <is>
           <t>AISI 420</t>
@@ -7836,6 +8646,11 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>NM063</t>
+        </is>
+      </c>
       <c r="K165" t="inlineStr">
         <is>
           <t>AISI 316 C</t>
@@ -7881,6 +8696,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>A = 405mm</t>
+        </is>
+      </c>
       <c r="K166" t="inlineStr">
         <is>
           <t>SAE 1020</t>
@@ -7926,6 +8746,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>180</t>
+        </is>
+      </c>
       <c r="K167" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -7971,6 +8796,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
       <c r="K168" t="inlineStr">
         <is>
           <t>ASTM A-36</t>
@@ -8016,6 +8846,11 @@
           <t>MSP3S25</t>
         </is>
       </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>3000 PSI</t>
+        </is>
+      </c>
       <c r="K169" t="inlineStr">
         <is>
           <t>SCREW</t>
@@ -8061,6 +8896,11 @@
           <t>NM-RT</t>
         </is>
       </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>special</t>
+        </is>
+      </c>
       <c r="K170" t="inlineStr">
         <is>
           <t>AISI 304</t>
@@ -8106,6 +8946,11 @@
           <t>MSP-P</t>
         </is>
       </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>3NS-</t>
+        </is>
+      </c>
       <c r="K171" t="inlineStr">
         <is>
           <t>FERRO FUNDIDO</t>
@@ -8149,6 +8994,11 @@
       <c r="I172" t="inlineStr">
         <is>
           <t>MSP-P</t>
+        </is>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>Housing</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">

</xml_diff>

<commit_message>
Remove debug print statement for product group mapping in inserir_internal_coments function
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -713,7 +713,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -958,7 +958,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>250MM</t>
+          <t>35X70</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>332</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -3313,7 +3313,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>St</t>
+          <t>NR</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -3468,7 +3468,7 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NM031BH</t>
         </is>
       </c>
       <c r="M60" t="inlineStr">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>3NS-</t>
+          <t>22mm</t>
         </is>
       </c>
       <c r="K66" t="inlineStr">
@@ -4418,7 +4418,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
@@ -4458,7 +4458,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Show-room</t>
+          <t>N.MAC 50C</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -4568,7 +4568,7 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>2NS-/16H3-</t>
+          <t>ASME B16.5</t>
         </is>
       </c>
       <c r="M82" t="inlineStr">
@@ -5168,7 +5168,7 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>MG1-G60</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M94" t="inlineStr">
@@ -5258,7 +5258,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>80</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -6148,7 +6148,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>30</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -6208,7 +6208,7 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>MB</t>
+          <t>25</t>
         </is>
       </c>
       <c r="M115" t="inlineStr">
@@ -6298,7 +6298,7 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
@@ -7333,7 +7333,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>NM038</t>
+          <t>3"SMS</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -8168,7 +8168,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>3NS-</t>
+          <t>3/8"</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -8268,7 +8268,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>C</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -8403,7 +8403,7 @@
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>NM038</t>
+          <t>2"SMS</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -8798,7 +8798,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>50</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">

</xml_diff>

<commit_message>
Refactor SAP narrative processing and add unit insertion functionality
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -596,6 +596,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -646,6 +651,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -696,6 +706,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -713,7 +728,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -746,6 +761,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -763,7 +783,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>CAR</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -796,6 +816,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -846,6 +871,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D8" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -896,6 +926,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -946,6 +981,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D10" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -996,6 +1036,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D11" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1046,6 +1091,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D12" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1096,6 +1146,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D13" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1146,6 +1201,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D14" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1196,6 +1256,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1246,6 +1311,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D16" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1296,6 +1366,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D17" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1346,6 +1421,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D18" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1396,6 +1476,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D19" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1446,6 +1531,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D20" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1496,6 +1586,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1546,6 +1641,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D22" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1596,6 +1696,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D23" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1646,6 +1751,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D24" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1696,6 +1806,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D25" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1746,6 +1861,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D26" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1796,6 +1916,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1846,6 +1971,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D28" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1896,6 +2026,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D29" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1946,6 +2081,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D30" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -1996,6 +2136,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2046,6 +2191,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D32" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2096,6 +2246,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D33" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2146,6 +2301,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D34" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2196,6 +2356,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D35" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2246,6 +2411,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2296,6 +2466,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2346,6 +2521,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2396,6 +2576,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2446,6 +2631,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2496,6 +2686,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2546,6 +2741,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2596,6 +2796,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2646,6 +2851,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2696,6 +2906,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2746,6 +2961,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2796,6 +3016,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2846,6 +3071,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2896,6 +3126,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2946,6 +3181,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -2963,7 +3203,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>St</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -2996,6 +3236,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3046,6 +3291,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3096,6 +3346,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3146,6 +3401,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>PÇ</t>
+        </is>
+      </c>
       <c r="D54" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3196,6 +3456,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D55" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3246,6 +3511,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3296,6 +3566,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3313,7 +3588,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>St</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="L57" t="inlineStr">
@@ -3346,6 +3621,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3396,6 +3676,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3446,6 +3731,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D60" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3496,6 +3786,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3546,6 +3841,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3596,6 +3896,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D63" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3646,6 +3951,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3696,6 +4006,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3746,6 +4061,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3796,6 +4116,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3846,6 +4171,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3896,6 +4226,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D69" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3946,6 +4281,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D70" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -3996,6 +4336,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4046,6 +4391,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4096,6 +4446,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D73" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4146,6 +4501,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D74" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4196,6 +4556,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4246,6 +4611,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4296,6 +4666,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4346,6 +4721,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4396,6 +4776,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D79" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4408,7 +4793,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -4418,7 +4803,7 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="M79" t="inlineStr">
@@ -4446,6 +4831,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D80" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4458,7 +4848,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Show-room</t>
+          <t>N.MAC 50C</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -4496,6 +4886,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D81" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4546,6 +4941,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4596,6 +4996,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D83" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4646,6 +5051,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D84" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4696,6 +5106,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4746,6 +5161,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4796,6 +5216,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D87" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4846,6 +5271,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D88" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4896,6 +5326,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D89" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4946,6 +5381,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -4996,6 +5436,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5046,6 +5491,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5096,6 +5546,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D93" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5146,6 +5601,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>PÇ</t>
+        </is>
+      </c>
       <c r="D94" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5196,6 +5656,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5246,6 +5711,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5296,6 +5766,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D97" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5346,6 +5821,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D98" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5396,6 +5876,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5446,6 +5931,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D100" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5496,6 +5986,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D101" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5546,6 +6041,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D102" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5596,6 +6096,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D103" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5646,6 +6151,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D104" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5696,6 +6206,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D105" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5746,6 +6261,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D106" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5796,6 +6316,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D107" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5846,6 +6371,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D108" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5896,6 +6426,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D109" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5946,6 +6481,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D110" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -5996,6 +6536,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D111" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6018,7 +6563,7 @@
       </c>
       <c r="L111" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>MB</t>
         </is>
       </c>
       <c r="M111" t="inlineStr">
@@ -6046,6 +6591,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D112" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6058,7 +6608,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -6096,6 +6646,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D113" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6141,6 +6696,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D114" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6186,6 +6746,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D115" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6236,6 +6801,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D116" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6286,6 +6856,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D117" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6336,6 +6911,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D118" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6386,6 +6966,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D119" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6436,6 +7021,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D120" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6486,6 +7076,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D121" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6536,6 +7131,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D122" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6548,7 +7148,7 @@
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
@@ -6586,6 +7186,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D123" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6636,6 +7241,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D124" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6648,7 +7258,7 @@
       </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>02</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K124" t="inlineStr">
@@ -6686,6 +7296,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D125" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6736,6 +7351,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D126" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6786,6 +7406,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D127" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6836,6 +7461,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D128" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6886,6 +7516,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D129" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6936,6 +7571,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D130" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -6986,6 +7626,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D131" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7036,6 +7681,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D132" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7081,6 +7731,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D133" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7126,6 +7781,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D134" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7148,7 +7808,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>NEC 60A</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
@@ -7176,6 +7836,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D135" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7193,7 +7858,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>NEC 60A</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
@@ -7221,6 +7886,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D136" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7271,6 +7941,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D137" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7321,6 +7996,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D138" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7333,7 +8013,7 @@
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>NM038</t>
+          <t>3"SMS</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
@@ -7371,6 +8051,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D139" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7416,6 +8101,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D140" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7466,6 +8156,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D141" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7516,6 +8211,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D142" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7561,6 +8261,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D143" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7611,6 +8316,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D144" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7661,6 +8371,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D145" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7711,6 +8426,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D146" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7761,6 +8481,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D147" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7811,6 +8536,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D148" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7818,7 +8548,7 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>800mm</t>
+          <t>200x8</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
@@ -7828,7 +8558,7 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>NM105-T---</t>
+          <t>ANSI B16.5</t>
         </is>
       </c>
       <c r="M148" t="inlineStr">
@@ -7856,6 +8586,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D149" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7906,6 +8641,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D150" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -7956,6 +8696,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D151" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8006,6 +8751,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D152" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8056,6 +8806,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D153" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8106,6 +8861,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D154" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8156,6 +8916,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D155" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8206,6 +8971,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D156" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8251,6 +9021,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D157" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8268,7 +9043,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>A</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -8296,6 +9071,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D158" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8346,6 +9126,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D159" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8391,6 +9176,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D160" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8441,6 +9231,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D161" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8491,6 +9286,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D162" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8541,6 +9341,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D163" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8591,6 +9396,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D164" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8641,6 +9451,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D165" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8686,6 +9501,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D166" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8736,6 +9556,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D167" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8786,6 +9611,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D168" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8798,7 +9628,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
@@ -8836,6 +9666,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D169" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8886,6 +9721,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D170" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8936,6 +9776,11 @@
           <t>10</t>
         </is>
       </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
       <c r="D171" t="inlineStr">
         <is>
           <t>NDB</t>
@@ -8984,6 +9829,11 @@
       <c r="B172" t="inlineStr">
         <is>
           <t>10</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>PC</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">

</xml_diff>

<commit_message>
Refactor file paths and update data processing logic in planilha handling
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -496,12 +496,13 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Narrativa</t>
+          <t>SAP123</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>SAP123</t>
+          <t xml:space="preserve">Narrativa
+</t>
         </is>
       </c>
     </row>
@@ -513,7 +514,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MSTAE (X-Plant Mat.Status)_x000d_</t>
+          <t>MSTAE (X-Plant Mat.Status)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -528,7 +529,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>MAKTX (PT)_x000d_</t>
+          <t>MAKTX (PT)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -567,11 +568,6 @@
         </is>
       </c>
       <c r="M2" t="inlineStr">
-        <is>
-          <t>Narrativa</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
         <is>
           <t>Internal comment (narrative)</t>
         </is>
@@ -598,21 +594,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -620,27 +601,27 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>special</t>
+          <t>100</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>INOX</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>FAF37-DRN90LP4</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>verificar internal comment</t>
+          <t>TUBO: NTZ DIAM. NOMINAL: 238 PRESSÃO: 100 GEOMETRIA: ST VAZÃO 1.6 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO BORRACHA EST: 286 ANEL INOX SOLDA: NÃO</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>MOTOREDUTOR NETZSCH-SEW PARA BOMBA: NM038B/CÓDIGO NETZSCH: NS37/              REDUÇÃO: I=4,22/ROTAÇÃO: N=416RPM/FORMA CONSTR: M1/POTÊNCIA MOTOR: 2,20KW/    FREQUENCIA: 60HZ/EFICIÊNCIA: ALTO RENDIMENTO PREMIUM (IR3)/                   REFRIGERAÇÃO: TFVF/NRº PÓLOS: 4/GRAU PROTEÇÃO: IP55/TENSÃO: 220/380/440/760V/ ISOLAMENTO: F/MODELO SEW: FAF37-DRN90LP4/V/TF/                                CARAC. ESPECIAL: COM TERMISTOR TIPO PTC - TF,VENT FORÇ"V" MONOF 50/60HZ: 220~277VAC; 50HZ: TRIÂNG,200~303VAC; ESTR,346~525VAC; 60HZ: TRIÂNG,220~332VAC; ESTR,380~575VAC/</t>
+          <t>TUBO: NTZ DIAM. NOMINAL: 238 PRESSÃO: 100 GEOMETRIA: ST VAZÃO 1.6 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO BORRACHA EST: 286 ANEL INOX SOLDA: NÃO</t>
         </is>
       </c>
     </row>
@@ -665,21 +646,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Redutor</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Reducer</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Reductor</t>
-        </is>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -821,21 +787,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -858,21 +809,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -920,21 +856,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -982,21 +903,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1004,7 +910,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>286</t>
+          <t>PIN</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1014,12 +920,12 @@
       </c>
       <c r="M10" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*120DT50-SH - DIAM. EXTERNO MÁX. 104 MM  ESTATOR 4" 286  TUBO DE EXTENSÃO 4"  CROSS OVER 2.7/8" EU BOX STOP PIN - 2.7/8" EU PIN TODAS AS PEÇAS DEVERÃO SER SOLDADAS</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*120DT50-SH - DIAM. EXTERNO MÁX. 104 MM  ESTATOR 4" 286  TUBO DE EXTENSÃO 4"  CROSS OVER 2.7/8" EU BOX STOP PIN - 2.7/8" EU PIN TODAS AS PEÇAS DEVERÃO SER SOLDADAS</t>
         </is>
       </c>
     </row>
@@ -1091,21 +997,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1153,21 +1044,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J13" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1215,21 +1091,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1277,21 +1138,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J15" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1339,21 +1185,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J16" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1401,21 +1232,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>2.3/8"</t>
@@ -1433,12 +1249,12 @@
       </c>
       <c r="M17" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ166*120ST0.8   ROTOR Z2 1045 HCP25 COUPLING 1/2" X 5/8"  ESTATOR 286 NU CROSS OVER - 1.66" X 2.3/8" EU BOX STOP PIN - 1.66" X 2.3/8" EU PIN</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ166*120ST0.8   ROTOR Z2 1045 HCP25 COUPLING 1/2" X 5/8"  ESTATOR 286 NU CROSS OVER - 1.66" X 2.3/8" EU BOX STOP PIN - 1.66" X 2.3/8" EU PIN</t>
         </is>
       </c>
     </row>
@@ -1463,21 +1279,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J18" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -1495,12 +1296,12 @@
       </c>
       <c r="M18" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ450*090DT150-SH ESTATOR 286 NUE - SOLDADO C/TUBO DE EXTENSÃO 4.1/2" NUE - SOLDADO C/LUVA SUPERIOR 4.1/2" NU X 3.1/2" EUE BOX - SOLDADA NO TUBO DE EXTENSÃO ROTOR P5 1045 HCP25 C/STOP PIN SOLDADO -  4.1/2" NU X 2.7/8" EU PIN</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N18" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ450*090DT150-SH ESTATOR 286 NUE - SOLDADO C/TUBO DE EXTENSÃO 4.1/2" NUE - SOLDADO C/LUVA SUPERIOR 4.1/2" NU X 3.1/2" EUE BOX - SOLDADA NO TUBO DE EXTENSÃO ROTOR P5 1045 HCP25 C/STOP PIN SOLDADO -  4.1/2" NU X 2.7/8" EU PIN</t>
         </is>
       </c>
     </row>
@@ -1525,21 +1326,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J19" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -1557,12 +1343,12 @@
       </c>
       <c r="M19" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ450*120DT150-SH ESTATOR 286 NUE - SOLDADO C/TUBO DE EXTENSÃO 4.1/2" NUE - SOLDADO C/LUVA SUPERIOR 4.1/2" NU X 3.1/2" EUE BOX - SOLDADA NO TUBO DE EXTENSÃO ROTOR P5 1045 HCP25 C/STOP PIN SOLDADO -  4.1/2" NU X 2.7/8" EU PIN</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N19" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ450*120DT150-SH ESTATOR 286 NUE - SOLDADO C/TUBO DE EXTENSÃO 4.1/2" NUE - SOLDADO C/LUVA SUPERIOR 4.1/2" NU X 3.1/2" EUE BOX - SOLDADA NO TUBO DE EXTENSÃO ROTOR P5 1045 HCP25 C/STOP PIN SOLDADO -  4.1/2" NU X 2.7/8" EU PIN</t>
         </is>
       </c>
     </row>
@@ -1587,21 +1373,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1649,21 +1420,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J21" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1711,21 +1467,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J22" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1773,21 +1514,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1835,21 +1561,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1897,21 +1608,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1959,21 +1655,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2021,21 +1702,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2083,21 +1749,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J28" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2145,21 +1796,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J29" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2207,21 +1843,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J30" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2239,12 +1860,12 @@
       </c>
       <c r="M30" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*200DT50 ROTOR P6 1045 HCP12 ESTATOR 286 NU TUBO DE EXTENSÃO 4" NU  LUVA ESTATOR 4" NU BOX X 4" NU BOX CROSS OVER 4" NU BOX  X 2.7/8" EU BOX STOP PIN - 4" NU X 2.7/8" EU PIN</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N30" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*200DT50 ROTOR P6 1045 HCP12 ESTATOR 286 NU TUBO DE EXTENSÃO 4" NU  LUVA ESTATOR 4" NU BOX X 4" NU BOX CROSS OVER 4" NU BOX  X 2.7/8" EU BOX STOP PIN - 4" NU X 2.7/8" EU PIN</t>
         </is>
       </c>
     </row>
@@ -2269,21 +1890,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J31" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -2331,21 +1937,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J32" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2393,21 +1984,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J33" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2455,21 +2031,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J34" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -2487,12 +2048,12 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ450*120DT150-SH ROTOR P7 1045 HCP25 ESTATOR 286 NU TUBO DE EXTENSAO 4.1/2" - 6PÉS (CLIENTE IRÁ SOLDAR POR CONTA) STOP PIN - 4.1/2" NU X 2.7/8" EU PIN SOLDADO CONEXÃO SUPERIOR 3.1/2" EU</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ450*120DT150-SH ROTOR P7 1045 HCP25 ESTATOR 286 NU TUBO DE EXTENSAO 4.1/2" - 6PÉS (CLIENTE IRÁ SOLDAR POR CONTA) STOP PIN - 4.1/2" NU X 2.7/8" EU PIN SOLDADO CONEXÃO SUPERIOR 3.1/2" EU</t>
         </is>
       </c>
     </row>
@@ -2517,21 +2078,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J35" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -2539,7 +2085,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>ROTOR</t>
+          <t>V-630</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2549,12 +2095,12 @@
       </c>
       <c r="M35" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ450*162DT150 ROTOR P4 V-630 WITHOUT CHROME (OBS.: TO FORESSE DIMENSIONS  WITH LAYER OF 0,15 MM IN THE CREST POINT AND 0,18MM IN VALLEY POINT OF ROTOR.)  THE ROTOR CONEXION AND FLEXI ROD CONEXION WILL BE LEFT THREADS. ESTATOR 237 4.1/2 x 8 NU WITH REDUCED DIAMETER. THE CASING IS 7". O.D. FOR THE STATOR SHALL NOT OVER 132MM.  FLEXI ROD V-630 STOP PIN - 4.1/2" EU PIN</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ450*162DT150 ROTOR P4 V-630 WITHOUT CHROME (OBS.: TO FORESSE DIMENSIONS  WITH LAYER OF 0,15 MM IN THE CREST POINT AND 0,18MM IN VALLEY POINT OF ROTOR.)  THE ROTOR CONEXION AND FLEXI ROD CONEXION WILL BE LEFT THREADS. ESTATOR 237 4.1/2 x 8 NU WITH REDUCED DIAMETER. THE CASING IS 7". O.D. FOR THE STATOR SHALL NOT OVER 132MM.  FLEXI ROD V-630 STOP PIN - 4.1/2" EU PIN</t>
         </is>
       </c>
     </row>
@@ -2579,21 +2125,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J36" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -2611,12 +2142,12 @@
       </c>
       <c r="M36" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ450*240DT74  ROTOR P8 1045 HCP25 ESTATOR 286-R EU ADAPTER COUPLING 1.1/8" X 1" STOP PIN - 3.1/2" EU PIN CROSS OVER  4.1/2" EU X 3.1/2" EU EXTENSION TUBE 4.1/2" EU - 6 PÉS</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ450*240DT74  ROTOR P8 1045 HCP25 ESTATOR 286-R EU ADAPTER COUPLING 1.1/8" X 1" STOP PIN - 3.1/2" EU PIN CROSS OVER  4.1/2" EU X 3.1/2" EU EXTENSION TUBE 4.1/2" EU - 6 PÉS</t>
         </is>
       </c>
     </row>
@@ -2641,21 +2172,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J37" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2750,21 +2266,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J39" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2812,21 +2313,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J40" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -2874,21 +2360,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2911,21 +2382,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2948,21 +2404,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2985,21 +2426,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J44" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3047,21 +2473,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J45" t="inlineStr">
         <is>
           <t>120</t>
@@ -3109,21 +2520,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -3176,21 +2572,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J47" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3208,12 +2589,12 @@
       </c>
       <c r="M47" t="inlineStr">
         <is>
+          <t>BOMBA PCP MOD. NTZ400*120ST25   ROTOR P6 1045 HCP25 ESTATOR 286-R NU LUVA ESTATOR 4" NU BOX  X  4" NU BOX TUBO DE EXTENSÃO 4" NU - 6 PÉS CROSS OVER 4" NU BOX  X 3-1/2" NU BOX STOP PIN - 3-1/2" NU PIN</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>BOMBA PCP MOD. NTZ400*120ST25   ROTOR P6 1045 HCP25 ESTATOR 286-R NU LUVA ESTATOR 4" NU BOX  X  4" NU BOX TUBO DE EXTENSÃO 4" NU - 6 PÉS CROSS OVER 4" NU BOX  X 3-1/2" NU BOX STOP PIN - 3-1/2" NU PIN</t>
         </is>
       </c>
     </row>
@@ -3238,21 +2619,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J48" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3270,12 +2636,12 @@
       </c>
       <c r="M48" t="inlineStr">
         <is>
+          <t>BOMBA PCP MOD. NTZ400*120ST25   ROTOR P5 1045 HCP25 ESTATOR 286-R NU LUVA ESTATOR 4" NU BOX  X  4" NU BOX TUBO DE EXTENSÃO 4" NU - 6 PÉS CROSS OVER 4" NU BOX  X 3-1/2" NU BOX STOP PIN - 3-1/2" NU PIN</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>BOMBA PCP MOD. NTZ400*120ST25   ROTOR P5 1045 HCP25 ESTATOR 286-R NU LUVA ESTATOR 4" NU BOX  X  4" NU BOX TUBO DE EXTENSÃO 4" NU - 6 PÉS CROSS OVER 4" NU BOX  X 3-1/2" NU BOX STOP PIN - 3-1/2" NU PIN</t>
         </is>
       </c>
     </row>
@@ -3300,21 +2666,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J49" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3362,21 +2713,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Redutor</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Reducer</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Reductor</t>
-        </is>
-      </c>
       <c r="I50" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -3394,17 +2730,17 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
+          <t>BOMBA PCP  TUBO: NTZ/DIAM. NOMINAL: 278/PRESSÃO: 120/GEOMETRIA: ST/VAZÃO 14/  SH: NÃO/PADDLE: NÃO/THT: NÃO/H: NÃO/LUVA ROT SH: NÃO/ANEL INOX SOLDA: NÃO/</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>BOMBA PCP  TUBO: NTZ/DIAM. NOMINAL: 278/PRESSÃO: 120/GEOMETRIA: ST/VAZÃO 14/  SH: NÃO/PADDLE: NÃO/THT: NÃO/H: NÃO/LUVA ROT SH: NÃO/ANEL INOX SOLDA: NÃO/</t>
         </is>
       </c>
     </row>
@@ -3429,21 +2765,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J51" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3491,21 +2812,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J52" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3553,21 +2859,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J53" t="inlineStr">
         <is>
           <t>2.3/8"</t>
@@ -3615,21 +2906,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Acoplador</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Coupler</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>Acoplador</t>
-        </is>
-      </c>
       <c r="J54" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3647,12 +2923,12 @@
       </c>
       <c r="M54" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*300ST25-H   ROTOR P10 VL40 HCP12 ESTATOR 332-R - COM LUVAS 3.1/2" EU BOX NAS EXTREMIDADES TUBO DE EXTENSÃO 3-1/2" EU BOX - 6 FEET LUVA 3-1/2" EU BOX STOP PIN  - 3.1/2" EU PIN</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*300ST25-H   ROTOR P10 VL40 HCP12 ESTATOR 332-R - COM LUVAS 3.1/2" EU BOX NAS EXTREMIDADES TUBO DE EXTENSÃO 3-1/2" EU BOX - 6 FEET LUVA 3-1/2" EU BOX STOP PIN  - 3.1/2" EU PIN</t>
         </is>
       </c>
     </row>
@@ -3677,21 +2953,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J55" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3709,12 +2970,12 @@
       </c>
       <c r="M55" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*300ST25-H   ROTOR P9 VL40 HCP25 ESTATOR 286-R - COM LUVAS 3.1/2" EU BOX NAS EXTREMIDADES TUBO DE EXTENSÃO 3-1/2" EU BOX - 6 FEET LUVA 3-1/2" EU BOX STOP PIN  - 3.1/2" EU PIN</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*300ST25-H   ROTOR P9 VL40 HCP25 ESTATOR 286-R - COM LUVAS 3.1/2" EU BOX NAS EXTREMIDADES TUBO DE EXTENSÃO 3-1/2" EU BOX - 6 FEET LUVA 3-1/2" EU BOX STOP PIN  - 3.1/2" EU PIN</t>
         </is>
       </c>
     </row>
@@ -3739,21 +3000,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J56" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -3801,21 +3047,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="J57" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3863,21 +3094,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Motoredutor</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Gear Motor</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>Motorreductor</t>
-        </is>
-      </c>
       <c r="I58" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -3999,21 +3215,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I61" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -4036,12 +3237,12 @@
       </c>
       <c r="M61" t="inlineStr">
         <is>
+          <t>TE DE BOMBEIO COM VÁLVULA DE SEGURANÇA P/ HASTE 1-1/2"  MATERIAL 1020/1045/NBR01 CONEXÃO SUPERIOR: FLANGE 3.1/8" - 2000 PSI  CONEXÃO INFERIOR: FLANGE 7.1/16"- 3000 PSI C/ROSCA 4-1/2 EU BOX CONEXÃO LATERAL: ROSCA FEMEA 3"LP E 2"LP                                               (SUBS. PELO ITEM NDB4995495) RING JOINT + PARAFUSOS, PORCAS E ARRUELAS CONEXÕES FLANGEADAS CONF. NORMA API 6A TIPO 6B CONEXÕES ROSCADAS CONF. NORMA API 5B</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>TE DE BOMBEIO COM VÁLVULA DE SEGURANÇA P/ HASTE 1-1/2"  MATERIAL 1020/1045/NBR01 CONEXÃO SUPERIOR: FLANGE 3.1/8" - 2000 PSI  CONEXÃO INFERIOR: FLANGE 7.1/16"- 3000 PSI C/ROSCA 4-1/2 EU BOX CONEXÃO LATERAL: ROSCA FEMEA 3"LP E 2"LP                                               (SUBS. PELO ITEM NDB4995495) RING JOINT + PARAFUSOS, PORCAS E ARRUELAS CONEXÕES FLANGEADAS CONF. NORMA API 6A TIPO 6B CONEXÕES ROSCADAS CONF. NORMA API 5B</t>
         </is>
       </c>
     </row>
@@ -4066,21 +3267,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="J62" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -4098,12 +3284,12 @@
       </c>
       <c r="M62" t="inlineStr">
         <is>
+          <t>CONJ. EST/ROT/STOP PIN MOD. NTZ400*240ST50-H   ROTOR P10 1045 HCP25  ESTATOR 286 NU LUVA 4" NU BOX x 4" NU BOX LUVA ADAPTADORA 1" X 1-1/8"  STOP PIN 3.1/2" EU PIN</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>CONJ. EST/ROT/STOP PIN MOD. NTZ400*240ST50-H   ROTOR P10 1045 HCP25  ESTATOR 286 NU LUVA 4" NU BOX x 4" NU BOX LUVA ADAPTADORA 1" X 1-1/8"  STOP PIN 3.1/2" EU PIN</t>
         </is>
       </c>
     </row>
@@ -4128,21 +3314,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Quench</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Quench</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>Quench</t>
-        </is>
-      </c>
       <c r="J63" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -4190,21 +3361,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I64" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -4257,21 +3413,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="J65" t="inlineStr">
         <is>
           <t>special</t>
@@ -4319,21 +3460,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J66" t="inlineStr">
         <is>
           <t>special</t>
@@ -4381,21 +3507,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Anel Intermediário</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Intermediate Ring</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>Anillo intermedio</t>
-        </is>
-      </c>
       <c r="J67" t="inlineStr">
         <is>
           <t>150</t>
@@ -4443,21 +3554,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>Corpo Pcp</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Pcp housing</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>Cuerpo Pcp</t>
-        </is>
-      </c>
       <c r="J68" t="inlineStr">
         <is>
           <t>special</t>
@@ -4505,21 +3601,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Corpo Pcp</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Pcp housing</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Cuerpo Pcp</t>
-        </is>
-      </c>
       <c r="J69" t="inlineStr">
         <is>
           <t>special</t>
@@ -4567,21 +3648,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="J70" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4629,21 +3695,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="I71" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -4661,17 +3712,17 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
         <is>
+          <t>BOMBA PCP  TUBO: NTZ/DIAM. NOMINAL: 400/PRESSÃO: 090/GEOMETRIA: ST/VAZÃO 120/ SH: NÃO/PADDLE: NÃO/THT: NÃO/H: NÃO/LUVA ROT SH: NÃO/ANEL INOX SOLDA: NÃO/</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>BOMBA PCP  TUBO: NTZ/DIAM. NOMINAL: 400/PRESSÃO: 090/GEOMETRIA: ST/VAZÃO 120/ SH: NÃO/PADDLE: NÃO/THT: NÃO/H: NÃO/LUVA ROT SH: NÃO/ANEL INOX SOLDA: NÃO/</t>
         </is>
       </c>
     </row>
@@ -4696,21 +3747,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J72" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -4758,21 +3794,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J73" t="inlineStr">
         <is>
           <t>120</t>
@@ -4820,21 +3841,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J74" t="inlineStr">
         <is>
           <t>120</t>
@@ -4904,21 +3910,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4941,21 +3932,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J77" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -5003,21 +3979,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J78" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -5065,21 +4026,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>Adaptador</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Adapter</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>Adaptador</t>
-        </is>
-      </c>
       <c r="J79" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -5097,12 +4043,12 @@
       </c>
       <c r="M79" t="inlineStr">
         <is>
+          <t>BOMBA PCP MOD. - NTZ400*090ST120   ROTOR P5 1045 HCP25  ESTATOR 286 C/3.1/2" EU BOX STOP PIN - 3.1/2" EU PIN TUBO DE EXTENSÃO 3.1/2" EU PIN - 6 FEET</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>BOMBA PCP MOD. - NTZ400*090ST120   ROTOR P5 1045 HCP25  ESTATOR 286 C/3.1/2" EU BOX STOP PIN - 3.1/2" EU PIN TUBO DE EXTENSÃO 3.1/2" EU PIN - 6 FEET</t>
         </is>
       </c>
     </row>
@@ -5127,21 +4073,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>Display/Stand Com Rotor</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Display/Stand with Rotor</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Expositor/Soporte con Rotor</t>
-        </is>
-      </c>
       <c r="J80" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -5189,24 +4120,9 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -5253,7 +4169,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -5298,21 +4214,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Eixo Ligação</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Connecting Shaft</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Eje de enlace</t>
-        </is>
-      </c>
       <c r="J83" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -5360,21 +4261,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>Batente</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Stop</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Quicio</t>
-        </is>
-      </c>
       <c r="J84" t="inlineStr">
         <is>
           <t>120</t>
@@ -5422,21 +4308,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J85" t="inlineStr">
         <is>
           <t>120</t>
@@ -5484,21 +4355,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J86" t="inlineStr">
         <is>
           <t>180</t>
@@ -5593,21 +4449,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>Fuso Motor</t>
-        </is>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>Motor Spindle</t>
-        </is>
-      </c>
-      <c r="G88" t="inlineStr">
-        <is>
-          <t>Husillo del motor</t>
-        </is>
-      </c>
       <c r="J88" t="inlineStr">
         <is>
           <t>100</t>
@@ -5655,21 +4496,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>Fuso Motor</t>
-        </is>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>Motor Spindle</t>
-        </is>
-      </c>
-      <c r="G89" t="inlineStr">
-        <is>
-          <t>Husillo del motor</t>
-        </is>
-      </c>
       <c r="J89" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -5717,21 +4543,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J90" t="inlineStr">
         <is>
           <t>EU-M</t>
@@ -5779,21 +4590,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>Eixo Movido</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>Moved Shaft</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Accionado por eje</t>
-        </is>
-      </c>
       <c r="J91" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -5841,21 +4637,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>Eixo motor</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>Motor shaft</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Eje motor</t>
-        </is>
-      </c>
       <c r="J92" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -5903,21 +4684,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>Throat</t>
-        </is>
-      </c>
-      <c r="G93" t="inlineStr">
-        <is>
-          <t>Garganta</t>
-        </is>
-      </c>
       <c r="J93" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -5965,26 +4731,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>Porta selo</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>Mechanical seal housing</t>
-        </is>
-      </c>
-      <c r="G94" t="inlineStr">
-        <is>
-          <t>Caja del sello mecánico</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Aufnahmegehäuse</t>
-        </is>
-      </c>
       <c r="J94" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -6032,21 +4778,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G95" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="J95" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -6094,24 +4825,9 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>Suporte</t>
-        </is>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>Bracket</t>
-        </is>
-      </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>Apoyo</t>
-        </is>
-      </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -6126,12 +4842,12 @@
       </c>
       <c r="M96" t="inlineStr">
         <is>
+          <t>BOMBA PCP NETZSCH MODELO NTZ350*100DT40-SH   ROTOR P6 1045 HCP25 ESTATOR 286 EU CROSS OVER 3-1/2" EU X 2-7/8" EU BOX - SOLDADO TUBO DE EXTENSÃO 3-1/2" - 6 PÉS - SOLDADO STOP PIN - 2-7/8" EU PIN - SOLDADO</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>BOMBA PCP NETZSCH MODELO NTZ350*100DT40-SH   ROTOR P6 1045 HCP25 ESTATOR 286 EU CROSS OVER 3-1/2" EU X 2-7/8" EU BOX - SOLDADO TUBO DE EXTENSÃO 3-1/2" - 6 PÉS - SOLDADO STOP PIN - 2-7/8" EU PIN - SOLDADO</t>
         </is>
       </c>
     </row>
@@ -6156,21 +4872,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>Tampa Dianteira</t>
-        </is>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>Front Cover</t>
-        </is>
-      </c>
-      <c r="G97" t="inlineStr">
-        <is>
-          <t>Portada</t>
-        </is>
-      </c>
       <c r="J97" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -6218,21 +4919,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Conexão</t>
-        </is>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>Connection</t>
-        </is>
-      </c>
-      <c r="G98" t="inlineStr">
-        <is>
-          <t>Conexión</t>
-        </is>
-      </c>
       <c r="J98" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -6280,21 +4966,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>Base-e</t>
-        </is>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>Base plate</t>
-        </is>
-      </c>
-      <c r="G99" t="inlineStr">
-        <is>
-          <t>Base-e</t>
-        </is>
-      </c>
       <c r="J99" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -6342,21 +5013,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>Tubo De Imersão</t>
-        </is>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>Immersion Tube</t>
-        </is>
-      </c>
-      <c r="G100" t="inlineStr">
-        <is>
-          <t>Tubo de inmersión</t>
-        </is>
-      </c>
       <c r="J100" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -6426,21 +5082,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr">
-        <is>
-          <t>Kit Bomba</t>
-        </is>
-      </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>Pump Kit</t>
-        </is>
-      </c>
-      <c r="G102" t="inlineStr">
-        <is>
-          <t>Kit de bomba</t>
-        </is>
-      </c>
       <c r="J102" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -6488,21 +5129,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
-        <is>
-          <t>Acoplamento</t>
-        </is>
-      </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>Coupling</t>
-        </is>
-      </c>
-      <c r="G103" t="inlineStr">
-        <is>
-          <t>Acoplamiento</t>
-        </is>
-      </c>
       <c r="I103" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6510,7 +5136,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>25</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -6555,21 +5181,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G104" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I104" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6622,21 +5233,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
-        <is>
-          <t>Eixo Ligação</t>
-        </is>
-      </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>Connecting Shaft</t>
-        </is>
-      </c>
-      <c r="G105" t="inlineStr">
-        <is>
-          <t>Eje de enlace</t>
-        </is>
-      </c>
       <c r="I105" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6689,21 +5285,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G106" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I106" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6756,21 +5337,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G107" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I107" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6823,21 +5389,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G108" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I108" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6890,21 +5441,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G109" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I109" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6957,26 +5493,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr">
-        <is>
-          <t>Perfil</t>
-        </is>
-      </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>Section</t>
-        </is>
-      </c>
-      <c r="G110" t="inlineStr">
-        <is>
-          <t>Perfil</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t>Profil</t>
-        </is>
-      </c>
       <c r="I110" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -6999,12 +5515,12 @@
       </c>
       <c r="M110" t="inlineStr">
         <is>
+          <t>CABECOTE DE ACIONAMENTO PCP NDH030DH20-HB   C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI       ACESSÓRIOS: 01 - PLACA DE ARRASTE C/PROTEÇÃO 01 - JOGO DE POLIAS E CORREIAS PARA 250~300 RPM           01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 200L, 25 HP, 50 HZ, 380V, 6 POLOS SUPORTES 01 - RING JOINT R31</t>
+        </is>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N110" t="inlineStr">
-        <is>
-          <t>CABECOTE DE ACIONAMENTO PCP NDH030DH20-HB   C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI       ACESSÓRIOS: 01 - PLACA DE ARRASTE C/PROTEÇÃO 01 - JOGO DE POLIAS E CORREIAS PARA 250~300 RPM           01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 200L, 25 HP, 50 HZ, 380V, 6 POLOS SUPORTES 01 - RING JOINT R31</t>
         </is>
       </c>
     </row>
@@ -7081,21 +5597,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G112" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I112" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7103,7 +5604,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -7118,12 +5619,12 @@
       </c>
       <c r="M112" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ350*120ST16.4   ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N112" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ350*120ST16.4   ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7155,7 +5656,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -7170,12 +5671,12 @@
       </c>
       <c r="M113" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ350*120ST20  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N113" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ350*120ST20  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7207,7 +5708,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -7222,12 +5723,12 @@
       </c>
       <c r="M114" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ350*120ST25  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N114" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ350*120ST25  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS LUVA 3-1/2" NU BOX CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU BOX X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7274,12 +5775,12 @@
       </c>
       <c r="M115" t="inlineStr">
         <is>
+          <t>CABECOTE DE ACIONAMENTO PCP NDH030DH20-HB  C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI - RJ31       ACESSÓRIOS: 01 - PLACA DE ARRASTE 01 - POLIA MOVIDA A670           01 - POLIA MOTORA A170 01 - BELT SET 01 - PROTEÇÃO P/CORREIAS E POLIAS 01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 01 - SUPORTE  i=3,94</t>
+        </is>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N115" t="inlineStr">
-        <is>
-          <t>CABECOTE DE ACIONAMENTO PCP NDH030DH20-HB  C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI - RJ31       ACESSÓRIOS: 01 - PLACA DE ARRASTE 01 - POLIA MOVIDA A670           01 - POLIA MOTORA A170 01 - BELT SET 01 - PROTEÇÃO P/CORREIAS E POLIAS 01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 01 - SUPORTE  i=3,94</t>
         </is>
       </c>
     </row>
@@ -7311,7 +5812,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -7326,12 +5827,12 @@
       </c>
       <c r="M116" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*120ST78  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1-1/8" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N116" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*120ST78  ESTATOR 286 NU ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1-1/8" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7356,21 +5857,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
-        <is>
-          <t>Externo</t>
-        </is>
-      </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>Outside</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t>Außen</t>
-        </is>
-      </c>
       <c r="I117" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7393,12 +5879,12 @@
       </c>
       <c r="M117" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*150ST58  ESTATOR 286 NU BOX WELDED ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1-1/8" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N117" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*150ST58  ESTATOR 286 NU BOX WELDED ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1-1/8" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7423,21 +5909,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr">
-        <is>
-          <t>Parafuso</t>
-        </is>
-      </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>Screw</t>
-        </is>
-      </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>Tornillo</t>
-        </is>
-      </c>
       <c r="I118" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7460,12 +5931,12 @@
       </c>
       <c r="M118" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ400*120ST40  ESTATOR 286 NU BOX WELDED ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N118" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ400*120ST40  ESTATOR 286 NU BOX WELDED ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 1" - SH TUBO DE EXTENSÃO 3-1/2" NU - 6 PÉS CROSS OVER 3-1/2" NU BOX  X 2-7/8" NU BOX STOP PIN - 3-1/2" NU PIN X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7512,12 +5983,12 @@
       </c>
       <c r="M119" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ278*150ST10  ESTATOR 286 NU  ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 7/8" - SH LUVA 2-7/8" NU BOX STOP PIN - 2-7/8" NU BOX X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N119" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ278*150ST10  ESTATOR 286 NU  ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 7/8" - SH LUVA 2-7/8" NU BOX STOP PIN - 2-7/8" NU BOX X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7564,12 +6035,12 @@
       </c>
       <c r="M120" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ278*120ST10  ESTATOR 286 NU  ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 7/8" - SH LUVA 2-7/8" NU BOX STOP PIN - 2-7/8" NU BOX X  2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N120" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ278*120ST10  ESTATOR 286 NU  ROTOR P4 1045 HCP25 SUB-COUPLING 7/8" X 7/8" - SH LUVA 2-7/8" NU BOX STOP PIN - 2-7/8" NU BOX X  2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7616,12 +6087,12 @@
       </c>
       <c r="M121" t="inlineStr">
         <is>
+          <t>CABECOTE DE ACIONAMENTO PCP NDH040DH20-HB  C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI - RJ31       ACESSÓRIOS: 01 - PLACA DE ARRASTE 01 - POLIA MOVIDA A670           01 - POLIA MOTORA A170 01 - BELT SET 01 - PROTEÇÃO P/CORREIAS E POLIAS 01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 01 - SUPORT 01 - RING JOINT  i=3,94</t>
+        </is>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N121" t="inlineStr">
-        <is>
-          <t>CABECOTE DE ACIONAMENTO PCP NDH040DH20-HB  C/FREIO HIDRÁULICO  P/HASTE DE 1 1/4" C/FLANGE 3.1/8" - 2000 PSI - RJ31       ACESSÓRIOS: 01 - PLACA DE ARRASTE 01 - POLIA MOVIDA A670           01 - POLIA MOTORA A170 01 - BELT SET 01 - PROTEÇÃO P/CORREIAS E POLIAS 01 - BASE METÁLICA AJUSTÁVEL PARA MOTOR 01 - SUPORT 01 - RING JOINT  i=3,94</t>
         </is>
       </c>
     </row>
@@ -7720,12 +6191,12 @@
       </c>
       <c r="M123" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ350*100ST25   ROTOR Z2 1045 HCP25 SUB-COUPLING 1" X 7/8" - SH ESTATOR 286 EU TUBO DE EXTENSÃO 3-1/2" EU - 6 PÉS LUVA 3-1/2" EU BOX CROSS OVER 3-1/2" EU BOX  X 2-7/8" NU BOX  STOP PIN 2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N123" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ350*100ST25   ROTOR Z2 1045 HCP25 SUB-COUPLING 1" X 7/8" - SH ESTATOR 286 EU TUBO DE EXTENSÃO 3-1/2" EU - 6 PÉS LUVA 3-1/2" EU BOX CROSS OVER 3-1/2" EU BOX  X 2-7/8" NU BOX  STOP PIN 2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7750,21 +6221,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G124" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="I124" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7787,12 +6243,12 @@
       </c>
       <c r="M124" t="inlineStr">
         <is>
+          <t>BOMBA PCP - NTZ350*100DT40   ROTOR Z2 1045 HCP25 SUB-COUPLING 1" X 7/8" - SH ESTATOR 286 EU TUBO DE EXTENSÃO 3-1/2" EU - 6 PÉS LUVA 3-1/2" EU BOX CROSS OVER 3-1/2" EU BOX  X 2-7/8" NU BOX  STOP PIN 2-7/8" NU PIN</t>
+        </is>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N124" t="inlineStr">
-        <is>
-          <t>BOMBA PCP - NTZ350*100DT40   ROTOR Z2 1045 HCP25 SUB-COUPLING 1" X 7/8" - SH ESTATOR 286 EU TUBO DE EXTENSÃO 3-1/2" EU - 6 PÉS LUVA 3-1/2" EU BOX CROSS OVER 3-1/2" EU BOX  X 2-7/8" NU BOX  STOP PIN 2-7/8" NU PIN</t>
         </is>
       </c>
     </row>
@@ -7817,21 +6273,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr">
-        <is>
-          <t>Corpo De Desgaste</t>
-        </is>
-      </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>Wear housing</t>
-        </is>
-      </c>
-      <c r="G125" t="inlineStr">
-        <is>
-          <t>Cuerpo de desgaste</t>
-        </is>
-      </c>
       <c r="I125" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7844,12 +6285,12 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
@@ -7884,21 +6325,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G126" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I126" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7916,7 +6342,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M126" t="inlineStr">
@@ -7951,21 +6377,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F127" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G127" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I127" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -7983,7 +6394,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M127" t="inlineStr">
@@ -8018,21 +6429,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E128" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F128" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G128" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I128" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8050,7 +6446,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
@@ -8097,12 +6493,12 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -8149,12 +6545,12 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M130" t="inlineStr">
@@ -8201,12 +6597,12 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
@@ -8248,7 +6644,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
@@ -8258,7 +6654,7 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M132" t="inlineStr">
@@ -8305,12 +6701,12 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M133" t="inlineStr">
@@ -8362,7 +6758,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
@@ -8414,7 +6810,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
@@ -8466,7 +6862,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M136" t="inlineStr">
@@ -8518,7 +6914,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
@@ -8570,7 +6966,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M138" t="inlineStr">
@@ -8622,7 +7018,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M139" t="inlineStr">
@@ -8669,12 +7065,12 @@
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
@@ -8721,12 +7117,12 @@
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M141" t="inlineStr">
@@ -8761,26 +7157,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E142" t="inlineStr">
-        <is>
-          <t>Camisa</t>
-        </is>
-      </c>
-      <c r="F142" t="inlineStr">
-        <is>
-          <t>Shell</t>
-        </is>
-      </c>
-      <c r="G142" t="inlineStr">
-        <is>
-          <t>Camisa</t>
-        </is>
-      </c>
-      <c r="H142" t="inlineStr">
-        <is>
-          <t>Mantel</t>
-        </is>
-      </c>
       <c r="I142" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8798,7 +7174,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M142" t="inlineStr">
@@ -8850,7 +7226,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
@@ -8897,12 +7273,12 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M144" t="inlineStr">
@@ -8937,21 +7313,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E145" t="inlineStr">
-        <is>
-          <t>Polido</t>
-        </is>
-      </c>
-      <c r="F145" t="inlineStr">
-        <is>
-          <t>Polished</t>
-        </is>
-      </c>
-      <c r="H145" t="inlineStr">
-        <is>
-          <t>Poliert</t>
-        </is>
-      </c>
       <c r="I145" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8964,12 +7325,12 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
@@ -9016,12 +7377,12 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
@@ -9056,21 +7417,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Estator </t>
-        </is>
-      </c>
-      <c r="F147" t="inlineStr">
-        <is>
-          <t>Stator</t>
-        </is>
-      </c>
-      <c r="G147" t="inlineStr">
-        <is>
-          <t>Estator</t>
-        </is>
-      </c>
       <c r="I147" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9083,12 +7429,12 @@
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -9175,21 +7521,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E149" t="inlineStr">
-        <is>
-          <t>Corpo De Desgaste</t>
-        </is>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t>Wear housing</t>
-        </is>
-      </c>
-      <c r="G149" t="inlineStr">
-        <is>
-          <t>Cuerpo de desgaste</t>
-        </is>
-      </c>
       <c r="I149" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9207,7 +7538,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
@@ -9242,21 +7573,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E150" t="inlineStr">
-        <is>
-          <t>Mancal</t>
-        </is>
-      </c>
-      <c r="F150" t="inlineStr">
-        <is>
-          <t>Bearing</t>
-        </is>
-      </c>
-      <c r="G150" t="inlineStr">
-        <is>
-          <t>Cojinete</t>
-        </is>
-      </c>
       <c r="I150" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9274,7 +7590,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
@@ -9309,21 +7625,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E151" t="inlineStr">
-        <is>
-          <t>Corpo De Desgaste</t>
-        </is>
-      </c>
-      <c r="F151" t="inlineStr">
-        <is>
-          <t>Wear housing</t>
-        </is>
-      </c>
-      <c r="G151" t="inlineStr">
-        <is>
-          <t>Cuerpo de desgaste</t>
-        </is>
-      </c>
       <c r="I151" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9336,12 +7637,12 @@
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M151" t="inlineStr">
@@ -9383,7 +7684,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -9450,12 +7751,12 @@
       </c>
       <c r="M153" t="inlineStr">
         <is>
+          <t>TE DE BOMBEIO 3-1/8"-3000PSI X 7-1/16"-3000PSI    CONEXÃO SUPERIOR: FLANGE 3.1/8" - 3000 PSI  CONEXÃO INFERIOR: FLANGE 7.1/16"- 3000 PSI  CONEXÃO LATERAL: ROSCA FEMEA 2"LP E 3"LP COM PARAFUSOS, PORCAS E ARRUELAS CONEXÕES FLANGEADAS CONF. NORMA API 6A TIPO 6B CONEXÕES ROSCADAS CONF. NORMA API 5B</t>
+        </is>
+      </c>
+      <c r="N153" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N153" t="inlineStr">
-        <is>
-          <t>TE DE BOMBEIO 3-1/8"-3000PSI X 7-1/16"-3000PSI    CONEXÃO SUPERIOR: FLANGE 3.1/8" - 3000 PSI  CONEXÃO INFERIOR: FLANGE 7.1/16"- 3000 PSI  CONEXÃO LATERAL: ROSCA FEMEA 2"LP E 3"LP COM PARAFUSOS, PORCAS E ARRUELAS CONEXÕES FLANGEADAS CONF. NORMA API 6A TIPO 6B CONEXÕES ROSCADAS CONF. NORMA API 5B</t>
         </is>
       </c>
     </row>
@@ -9487,7 +7788,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -9532,21 +7833,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr">
-        <is>
-          <t>Pé Da Bomba</t>
-        </is>
-      </c>
-      <c r="F155" t="inlineStr">
-        <is>
-          <t>Pump Foot</t>
-        </is>
-      </c>
-      <c r="G155" t="inlineStr">
-        <is>
-          <t>Bomba de pie</t>
-        </is>
-      </c>
       <c r="I155" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -9554,7 +7840,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -9599,21 +7885,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E156" t="inlineStr">
-        <is>
-          <t>Bocal De Sucção</t>
-        </is>
-      </c>
-      <c r="F156" t="inlineStr">
-        <is>
-          <t>Suction Nozzle</t>
-        </is>
-      </c>
-      <c r="G156" t="inlineStr">
-        <is>
-          <t>Boquilla de aspiración</t>
-        </is>
-      </c>
       <c r="I156" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9631,7 +7902,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M156" t="inlineStr">
@@ -9678,12 +7949,12 @@
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>PCP</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -9740,12 +8011,12 @@
       </c>
       <c r="M158" t="inlineStr">
         <is>
+          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 100 GEOMETRIA: ST VAZÃO 14 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO BORRACHA EST: 237 ANEL INOX SOLDA: NÃO OBS: -/-</t>
+        </is>
+      </c>
+      <c r="N158" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N158" t="inlineStr">
-        <is>
-          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 100 GEOMETRIA: ST VAZÃO 14 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO BORRACHA EST: 237 ANEL INOX SOLDA: NÃO OBS: -/-</t>
         </is>
       </c>
     </row>
@@ -9836,7 +8107,7 @@
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>SAE4140</t>
+          <t>SAE1045</t>
         </is>
       </c>
       <c r="L161" t="inlineStr">
@@ -9846,12 +8117,12 @@
       </c>
       <c r="M161" t="inlineStr">
         <is>
+          <t>MODELO: SERVICE BOP HASTE: 1.1/4" CONEXÃO SUP: FLANGED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 3000 CON INT SUP: 3.1/2" NR CON INT SUP: EU API 5B CONEXÃO INF: FLANGED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 5000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 79 SAIDA PRODUÇÃO: 2" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE4140 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
+        </is>
+      </c>
+      <c r="N161" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N161" t="inlineStr">
-        <is>
-          <t>MODELO: SERVICE BOP HASTE: 1.1/4" CONEXÃO SUP: FLANGED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 3000 CON INT SUP: 3.1/2" NR CON INT SUP: EU API 5B CONEXÃO INF: FLANGED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 5000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 79 SAIDA PRODUÇÃO: 2" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE4140 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
         </is>
       </c>
     </row>
@@ -9888,7 +8159,7 @@
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>SAE4140</t>
+          <t>SAE1045</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
@@ -9898,12 +8169,12 @@
       </c>
       <c r="M162" t="inlineStr">
         <is>
+          <t>MODELO: SERVICE BOP HASTE: 1.1/4" CONEXÃO SUP: FLANGED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 3000 CON INT SUP: 3.1/2" NR CON INT SUP: EU API 5B CONEXÃO INF: FLANGED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 3000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 79 SAIDA PRODUÇÃO: 2" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE4140 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
+        </is>
+      </c>
+      <c r="N162" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N162" t="inlineStr">
-        <is>
-          <t>MODELO: SERVICE BOP HASTE: 1.1/4" CONEXÃO SUP: FLANGED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 3000 CON INT SUP: 3.1/2" NR CON INT SUP: EU API 5B CONEXÃO INF: FLANGED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 3000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 79 SAIDA PRODUÇÃO: 2" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE4140 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
         </is>
       </c>
     </row>
@@ -9945,17 +8216,17 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
         <is>
+          <t>TUBO: NTZ DIAM. NOMINAL: 400 PRESSÃO: 090 GEOMETRIA: ST VAZÃO 78 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO DIAM LUVA ROTOR: SH BORRACHA EST: 299 ANEL INOX SOLDA: NÃO OBS: -/-</t>
+        </is>
+      </c>
+      <c r="N163" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N163" t="inlineStr">
-        <is>
-          <t>TUBO: NTZ DIAM. NOMINAL: 400 PRESSÃO: 090 GEOMETRIA: ST VAZÃO 78 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO DIAM LUVA ROTOR: SH BORRACHA EST: 299 ANEL INOX SOLDA: NÃO OBS: -/-</t>
         </is>
       </c>
     </row>
@@ -10002,12 +8273,12 @@
       </c>
       <c r="M164" t="inlineStr">
         <is>
+          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 180 GEOMETRIA: ST VAZÃO 10 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO DIAM LUVA ROTOR: SH BORRACHA EST: 286 ANEL INOX SOLDA: NÃO OBS: -/-</t>
+        </is>
+      </c>
+      <c r="N164" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N164" t="inlineStr">
-        <is>
-          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 180 GEOMETRIA: ST VAZÃO 10 SH: NÃO PADDLE: NÃO THT: NÃO H: NÃO DIAM LUVA ROTOR: SH BORRACHA EST: 286 ANEL INOX SOLDA: NÃO OBS: -/-</t>
         </is>
       </c>
     </row>
@@ -10084,21 +8355,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E166" t="inlineStr">
-        <is>
-          <t>Medida</t>
-        </is>
-      </c>
-      <c r="F166" t="inlineStr">
-        <is>
-          <t>Dimension</t>
-        </is>
-      </c>
-      <c r="H166" t="inlineStr">
-        <is>
-          <t>Maß</t>
-        </is>
-      </c>
       <c r="I166" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -10106,7 +8362,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -10121,12 +8377,12 @@
       </c>
       <c r="M166" t="inlineStr">
         <is>
+          <t>MODELO: COMPOSITE BOP HASTE: 1.1/4" CONEXÃO SUP: STUDDED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 2000 CONEXÃO INF: ROSCA PIN TAM CONEXÃO INF: 2.7/8" NORMA CON SUP: EU API 5B  DIAM PASSAGEM: 50 SAIDA PRODUÇÃO: 3" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE1045 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
+        </is>
+      </c>
+      <c r="N166" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N166" t="inlineStr">
-        <is>
-          <t>MODELO: COMPOSITE BOP HASTE: 1.1/4" CONEXÃO SUP: STUDDED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 2000 CONEXÃO INF: ROSCA PIN TAM CONEXÃO INF: 2.7/8" NORMA CON SUP: EU API 5B  DIAM PASSAGEM: 50 SAIDA PRODUÇÃO: 3" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: SAE1045 MAT PISTOES: SAE1045 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
         </is>
       </c>
     </row>
@@ -10151,21 +8407,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F167" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G167" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="I167" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10218,21 +8459,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E168" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="F168" t="inlineStr">
-        <is>
-          <t>Flange</t>
-        </is>
-      </c>
-      <c r="G168" t="inlineStr">
-        <is>
-          <t>Reborde</t>
-        </is>
-      </c>
       <c r="I168" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10285,21 +8511,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E169" t="inlineStr">
-        <is>
-          <t>Bomba De Fusos</t>
-        </is>
-      </c>
-      <c r="F169" t="inlineStr">
-        <is>
-          <t>Spindle Pump</t>
-        </is>
-      </c>
-      <c r="G169" t="inlineStr">
-        <is>
-          <t>Bomba de husillo</t>
-        </is>
-      </c>
       <c r="I169" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10352,21 +8563,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E170" t="inlineStr">
-        <is>
-          <t>Polido</t>
-        </is>
-      </c>
-      <c r="F170" t="inlineStr">
-        <is>
-          <t>Polished</t>
-        </is>
-      </c>
-      <c r="H170" t="inlineStr">
-        <is>
-          <t>Poliert</t>
-        </is>
-      </c>
       <c r="I170" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10419,21 +8615,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E171" t="inlineStr">
-        <is>
-          <t>Corpo De Desgaste</t>
-        </is>
-      </c>
-      <c r="F171" t="inlineStr">
-        <is>
-          <t>Wear housing</t>
-        </is>
-      </c>
-      <c r="G171" t="inlineStr">
-        <is>
-          <t>Cuerpo de desgaste</t>
-        </is>
-      </c>
       <c r="I171" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10486,21 +8667,6 @@
           <t>NDB</t>
         </is>
       </c>
-      <c r="E172" t="inlineStr">
-        <is>
-          <t>Corpo De Desgaste</t>
-        </is>
-      </c>
-      <c r="F172" t="inlineStr">
-        <is>
-          <t>Wear housing</t>
-        </is>
-      </c>
-      <c r="G172" t="inlineStr">
-        <is>
-          <t>Cuerpo de desgaste</t>
-        </is>
-      </c>
       <c r="I172" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -10768,7 +8934,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -10976,7 +9142,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -10991,12 +9157,12 @@
       </c>
       <c r="M181" t="inlineStr">
         <is>
+          <t>MODELO: COMPOSITE BOP HASTE: 1.1/4" CONEXÃO SUP: STUDDED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 2000 CON INT SUP: 2.7/8" NR CON INT SUP: EU API 5B CONEXÃO INF: STUDDED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 2000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 70 SAIDA PRODUÇÃO: 3" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: GGG50 MAT PISTOES: SAE1045 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
+        </is>
+      </c>
+      <c r="N181" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N181" t="inlineStr">
-        <is>
-          <t>MODELO: COMPOSITE BOP HASTE: 1.1/4" CONEXÃO SUP: STUDDED TAM CONEXAO SUP: 3.1/8" NORMA CON SUP: API 6A CL PR CON SUP: 2000 CON INT SUP: 2.7/8" NR CON INT SUP: EU API 5B CONEXÃO INF: STUDDED TAM CONEXÃO INF: 3.1/8" NORMA CON SUP: API 6A CL PR CON INF: 2000 NR CON INT INF: EU API 5B  DIAM PASSAGEM: 70 SAIDA PRODUÇÃO: 3" NR SAIDA PROD: LP SAIDA AUXILIAR: 3" NR SAIDA AUX: LP MAT CO BOP: GGG50 MAT PISTOES: SAE1045 MAT VEDACAO: NBR RING JOINTS: SIM PORCAS E PARAFU: SIM</t>
         </is>
       </c>
     </row>
@@ -11038,17 +9204,17 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>4"</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="M182" t="inlineStr">
         <is>
+          <t>POT CABEÇOTE: 030 UNIDADE POT: Hp FORMA CONSTR: DH CARGA AXIAL 20 UN CARGA AXIAL: Lbs TIPO FREIO: HB TIPO VEDAÇÃO: GAXETAS POS VEDAÇÃO INFERIOR DIAM HASTE POL: 1.1/4" CONEXÃO INF: FLANGE TAM CONEXÃO: 7.1/16" CLASSE PRESSÃO: 3000 RING JOINT: SIM PRI/POR FL INF: SIM PROT POL E COR: SIM PROT CLAMP: SIM NORMA MOTOR: IEC TAM CARC MOTOR: 200M/L FREQ MOTOR: 50 QTDE POLOS: 6 FORNEC MOTOR: NÃO RPM CABEÇOTE: 240 DIAM POL MOV: 670 DIAM POL MOT: 170 BUCHA CÔNICA: SIM CORREIAS: STANDARD SUPORTE CABEÇ: SUPORTE MOTOR (1x) DES DIMENSIONAL: . OBSERVAÇÕES: - NOVA LANTERNA FUNDIDA</t>
+        </is>
+      </c>
+      <c r="N182" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N182" t="inlineStr">
-        <is>
-          <t>POT CABEÇOTE: 030 UNIDADE POT: Hp FORMA CONSTR: DH CARGA AXIAL 20 UN CARGA AXIAL: Lbs TIPO FREIO: HB TIPO VEDAÇÃO: GAXETAS POS VEDAÇÃO INFERIOR DIAM HASTE POL: 1.1/4" CONEXÃO INF: FLANGE TAM CONEXÃO: 7.1/16" CLASSE PRESSÃO: 3000 RING JOINT: SIM PRI/POR FL INF: SIM PROT POL E COR: SIM PROT CLAMP: SIM NORMA MOTOR: IEC TAM CARC MOTOR: 200M/L FREQ MOTOR: 50 QTDE POLOS: 6 FORNEC MOTOR: NÃO RPM CABEÇOTE: 240 DIAM POL MOV: 670 DIAM POL MOT: 170 BUCHA CÔNICA: SIM CORREIAS: STANDARD SUPORTE CABEÇ: SUPORTE MOTOR (1x) DES DIMENSIONAL: . OBSERVAÇÕES: - NOVA LANTERNA FUNDIDA</t>
         </is>
       </c>
     </row>
@@ -11095,12 +9261,12 @@
       </c>
       <c r="M183" t="inlineStr">
         <is>
+          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 120 GEOMETRIA: ST VAZÃO 7.0 SH: NÃO PADDLE: NÃO THT: NÃO ALTA PRESSÃO: NÃO TIPO PINO STOP: TIPO PINO CONEXAO INF. BO: 2.7/8"-EU (MACHO) P ROTOR: Z2 CAMADA DE CROMO: HCP25 MATERIAL ROTOR: 1045 ROSCA EST: EU-M BORRACHA EST: 286 ANEL INOX SOLDA: NÃO TESTE CFE: ESPECIAL (ESPECIFICADO PELO CLIENTE) MEIO DE TESTE: ÁGUA</t>
+        </is>
+      </c>
+      <c r="N183" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N183" t="inlineStr">
-        <is>
-          <t>TUBO: NTZ DIAM. NOMINAL: 278 PRESSÃO: 120 GEOMETRIA: ST VAZÃO 7.0 SH: NÃO PADDLE: NÃO THT: NÃO ALTA PRESSÃO: NÃO TIPO PINO STOP: TIPO PINO CONEXAO INF. BO: 2.7/8"-EU (MACHO) P ROTOR: Z2 CAMADA DE CROMO: HCP25 MATERIAL ROTOR: 1045 ROSCA EST: EU-M BORRACHA EST: 286 ANEL INOX SOLDA: NÃO TESTE CFE: ESPECIAL (ESPECIFICADO PELO CLIENTE) MEIO DE TESTE: ÁGUA</t>
         </is>
       </c>
     </row>
@@ -11147,12 +9313,12 @@
       </c>
       <c r="M184" t="inlineStr">
         <is>
+          <t>TUBO: NTZ DIAM. NOMINAL: 550 PRESSÃO: 150 GEOMETRIA: STM VAZÃO 140 SH: NÃO PADDLE: NÃO THT: NÃO ALTA PRESSÃO: NÃO TIPO PINO STOP: TIPO ESTRELA - COM RASGOS CONEXAO INF. BO: 5.1/2"-LTC (MACHO) CONEXAO SUP. BO: 4.1/2"-EU (FÊMEA) TUBO EXTENSÃO: 10FT CAMADA DE CROMO: S/CRM MATERIAL ROTOR: 4140 LUVA ADAP. ROT: 1" (FÊMEA) DIAM LUVA ROTOR: SH ROSCA EST: LTC-M BORRACHA EST: GGG50 ANEL INOX SOLDA: NÃO TESTE CFE: NDB147 (NETZSCH) MEIO DE TESTE: ÓLEO</t>
+        </is>
+      </c>
+      <c r="N184" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N184" t="inlineStr">
-        <is>
-          <t>TUBO: NTZ DIAM. NOMINAL: 550 PRESSÃO: 150 GEOMETRIA: STM VAZÃO 140 SH: NÃO PADDLE: NÃO THT: NÃO ALTA PRESSÃO: NÃO TIPO PINO STOP: TIPO ESTRELA - COM RASGOS CONEXAO INF. BO: 5.1/2"-LTC (MACHO) CONEXAO SUP. BO: 4.1/2"-EU (FÊMEA) TUBO EXTENSÃO: 10FT CAMADA DE CROMO: S/CRM MATERIAL ROTOR: 4140 LUVA ADAP. ROT: 1" (FÊMEA) DIAM LUVA ROTOR: SH ROSCA EST: LTC-M BORRACHA EST: GGG50 ANEL INOX SOLDA: NÃO TESTE CFE: NDB147 (NETZSCH) MEIO DE TESTE: ÓLEO</t>
         </is>
       </c>
     </row>
@@ -11199,12 +9365,12 @@
       </c>
       <c r="M185" t="inlineStr">
         <is>
+          <t>POT CABEÇOTE: 100 UNIDADE POT: Hp FORMA CONSTR: DH CARGA AXIAL 33 UN CARGA AXIAL: Lbs TIPO FREIO: MBD TIPO VEDAÇÃO: GAXETAS POS VEDAÇÃO INFERIOR DIAM HASTE POL: 1.1/2" CONEXÃO INF: FLANGE TAM CONEXÃO: 3.1/8" CLASSE PRESSÃO: 3000 RING JOINT: SIM PRI/POR FL INF: SIM PROT POL E COR: SIM PROT CLAMP: SIM NORMA MOTOR: IEC TAM CARC MOTOR: 280S/M FREQ MOTOR: 50 QTDE POLOS: 4 FORNEC MOTOR: NÃO ROTAÇÃO SAÍDA: 250 TORQUE SAÍDA: 3000 POT MOT INST: 100 HP DIAM POL MOV: 800 DIAM POL MOT: 138 BUCHA CÔNICA: NÃO CORREIAS: POWER BAND SUPORTE CABEÇ: SUPORTE MOTOR (1x) + SUPORTE BASE MOTORA (2x) OBSERVAÇÕES: 01 - POLIA MOTORA 150, I=5,33 (250 RPM)</t>
+        </is>
+      </c>
+      <c r="N185" t="inlineStr">
+        <is>
           <t>verificar internal comment</t>
-        </is>
-      </c>
-      <c r="N185" t="inlineStr">
-        <is>
-          <t>POT CABEÇOTE: 100 UNIDADE POT: Hp FORMA CONSTR: DH CARGA AXIAL 33 UN CARGA AXIAL: Lbs TIPO FREIO: MBD TIPO VEDAÇÃO: GAXETAS POS VEDAÇÃO INFERIOR DIAM HASTE POL: 1.1/2" CONEXÃO INF: FLANGE TAM CONEXÃO: 3.1/8" CLASSE PRESSÃO: 3000 RING JOINT: SIM PRI/POR FL INF: SIM PROT POL E COR: SIM PROT CLAMP: SIM NORMA MOTOR: IEC TAM CARC MOTOR: 280S/M FREQ MOTOR: 50 QTDE POLOS: 4 FORNEC MOTOR: NÃO ROTAÇÃO SAÍDA: 250 TORQUE SAÍDA: 3000 POT MOT INST: 100 HP DIAM POL MOV: 800 DIAM POL MOT: 138 BUCHA CÔNICA: NÃO CORREIAS: POWER BAND SUPORTE CABEÇ: SUPORTE MOTOR (1x) + SUPORTE BASE MOTORA (2x) OBSERVAÇÕES: 01 - POLIA MOTORA 150, I=5,33 (250 RPM)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance translation insertion logic with improved column name handling and fallback mechanisms
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -594,6 +594,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I3" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -646,6 +666,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -693,6 +733,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -740,6 +800,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -809,6 +889,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J8" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -856,6 +956,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J9" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -903,6 +1023,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -910,7 +1050,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>PIN</t>
+          <t>286</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -950,6 +1090,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -997,6 +1157,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J12" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1044,6 +1224,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1091,6 +1291,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J14" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1138,6 +1358,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J15" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1185,6 +1425,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J16" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1232,6 +1492,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J17" t="inlineStr">
         <is>
           <t>2.3/8"</t>
@@ -1279,9 +1559,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>4.1/2"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1326,9 +1626,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>4.1/2"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1373,6 +1693,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J20" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1420,6 +1760,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J21" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1467,6 +1827,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J22" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1514,6 +1894,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J23" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1561,6 +1961,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J24" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1608,6 +2028,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J25" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1655,6 +2095,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J26" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1702,6 +2162,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J27" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -1749,6 +2229,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J28" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1796,6 +2296,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J29" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1843,6 +2363,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1890,6 +2430,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J31" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -1937,6 +2497,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J32" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -1984,6 +2564,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2031,9 +2631,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Conexão</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Connection</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Conexión</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Verbindung</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>4.1/2"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2078,6 +2698,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J35" t="inlineStr">
         <is>
           <t>4.1/2"</t>
@@ -2085,7 +2725,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>V-630</t>
+          <t>ROTOR</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2125,9 +2765,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>4.1/2"</t>
+          <t>1.1/8"</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -2172,6 +2832,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J37" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -2219,6 +2899,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J38" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2266,6 +2966,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J39" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2313,6 +3033,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J40" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -2426,6 +3166,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J44" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2473,6 +3233,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J45" t="inlineStr">
         <is>
           <t>120</t>
@@ -2520,6 +3300,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I46" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -2572,6 +3372,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J47" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -2619,6 +3439,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J48" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -2666,6 +3506,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J49" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2730,7 +3590,7 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
@@ -2765,6 +3625,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J51" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2812,6 +3692,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J52" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -2859,6 +3759,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J53" t="inlineStr">
         <is>
           <t>2.3/8"</t>
@@ -2906,6 +3826,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J54" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -2953,6 +3893,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J55" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3000,6 +3960,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J56" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -3047,6 +4027,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J57" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3094,6 +4094,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I58" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -3146,6 +4166,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J59" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -3215,6 +4255,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>Válvula De Segurança</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Safety Valve</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Válvula de seguridad</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Sicherheitsventil</t>
+        </is>
+      </c>
       <c r="I61" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -3267,6 +4327,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>Luva Adaptadora</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Adapter Sleeve</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Manguito adaptador</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Adapterhülse</t>
+        </is>
+      </c>
       <c r="J62" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3314,6 +4394,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J63" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -3361,6 +4461,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I64" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -3413,6 +4533,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J65" t="inlineStr">
         <is>
           <t>special</t>
@@ -3460,6 +4600,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J66" t="inlineStr">
         <is>
           <t>special</t>
@@ -3507,6 +4667,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J67" t="inlineStr">
         <is>
           <t>150</t>
@@ -3554,6 +4734,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J68" t="inlineStr">
         <is>
           <t>special</t>
@@ -3566,7 +4766,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -3601,6 +4801,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J69" t="inlineStr">
         <is>
           <t>special</t>
@@ -3648,6 +4868,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J70" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -3712,7 +4952,7 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M71" t="inlineStr">
@@ -3747,6 +4987,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J72" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -3794,6 +5054,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J73" t="inlineStr">
         <is>
           <t>120</t>
@@ -3841,6 +5121,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J74" t="inlineStr">
         <is>
           <t>120</t>
@@ -3932,6 +5232,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J77" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -3979,6 +5299,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J78" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -4026,6 +5366,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J79" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -4073,6 +5433,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J80" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -4120,9 +5500,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>P5</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -4167,9 +5567,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>60</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -4214,6 +5634,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J83" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -4261,6 +5701,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J84" t="inlineStr">
         <is>
           <t>120</t>
@@ -4273,7 +5733,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>NTZ 400</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -4308,6 +5768,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J85" t="inlineStr">
         <is>
           <t>120</t>
@@ -4320,7 +5800,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>NTZ 400</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -4355,6 +5835,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J86" t="inlineStr">
         <is>
           <t>180</t>
@@ -4367,7 +5867,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>NTZ 278</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -4402,6 +5902,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J87" t="inlineStr">
         <is>
           <t>100</t>
@@ -4449,6 +5969,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J88" t="inlineStr">
         <is>
           <t>100</t>
@@ -4496,6 +6036,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J89" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -4543,6 +6103,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J90" t="inlineStr">
         <is>
           <t>EU-M</t>
@@ -4590,6 +6170,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J91" t="inlineStr">
         <is>
           <t>2.7/8"</t>
@@ -4637,6 +6237,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J92" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4684,6 +6304,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J93" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4731,6 +6371,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J94" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4778,6 +6438,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J95" t="inlineStr">
         <is>
           <t>1/2"</t>
@@ -4825,9 +6505,29 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -4872,6 +6572,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J97" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4919,6 +6639,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J98" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -4966,6 +6706,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J99" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -5013,6 +6773,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J100" t="inlineStr">
         <is>
           <t>3.1/2"</t>
@@ -5082,6 +6862,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="J102" t="inlineStr">
         <is>
           <t>7/8"</t>
@@ -5129,6 +6929,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I103" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5136,7 +6956,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -5181,6 +7001,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I104" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5233,6 +7073,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I105" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5285,6 +7145,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I106" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5337,6 +7217,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I107" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5389,6 +7289,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I108" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5441,6 +7361,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I109" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5493,6 +7433,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Placa De Arraste</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Drag Plate</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>Placa de arrastre</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t>Bremsplatte</t>
+        </is>
+      </c>
       <c r="I110" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -5505,7 +7465,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>EL</t>
+          <t>50</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -5545,6 +7505,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H111" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I111" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5597,6 +7577,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I112" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5604,7 +7604,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -5649,6 +7649,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H113" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I113" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5656,7 +7676,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -5701,6 +7721,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H114" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I114" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5708,7 +7748,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -5753,6 +7793,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Placa De Arraste</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Drag Plate</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>Placa de arrastre</t>
+        </is>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Bremsplatte</t>
+        </is>
+      </c>
       <c r="I115" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -5805,6 +7865,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H116" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I116" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5812,7 +7892,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>7/8"</t>
+          <t>1/2"</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -5857,6 +7937,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H117" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I117" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5909,6 +8009,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I118" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -5961,6 +8081,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I119" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6013,6 +8153,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I120" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6065,6 +8225,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Placa De Arraste</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Drag Plate</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>Placa de arrastre</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>Bremsplatte</t>
+        </is>
+      </c>
       <c r="I121" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -6117,6 +8297,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Estator </t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>Estator</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Stator</t>
+        </is>
+      </c>
       <c r="I122" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6169,6 +8369,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I123" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6221,6 +8441,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Tubo De Extensão</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Extension Tube</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Tubo de extensión</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>Verlängerungsrohr</t>
+        </is>
+      </c>
       <c r="I124" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -6290,7 +8530,7 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M125" t="inlineStr">
@@ -6342,7 +8582,7 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M126" t="inlineStr">
@@ -6394,7 +8634,7 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M127" t="inlineStr">
@@ -6446,7 +8686,7 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M128" t="inlineStr">
@@ -6498,7 +8738,7 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M129" t="inlineStr">
@@ -6550,7 +8790,7 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M130" t="inlineStr">
@@ -6602,7 +8842,7 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M131" t="inlineStr">
@@ -6644,7 +8884,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>65</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
@@ -6654,7 +8894,7 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M132" t="inlineStr">
@@ -6706,7 +8946,7 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M133" t="inlineStr">
@@ -6758,7 +8998,7 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M134" t="inlineStr">
@@ -6810,7 +9050,7 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M135" t="inlineStr">
@@ -6862,7 +9102,7 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M136" t="inlineStr">
@@ -6914,7 +9154,7 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M137" t="inlineStr">
@@ -6966,7 +9206,7 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M138" t="inlineStr">
@@ -7018,7 +9258,7 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M139" t="inlineStr">
@@ -7070,7 +9310,7 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M140" t="inlineStr">
@@ -7122,7 +9362,7 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M141" t="inlineStr">
@@ -7174,7 +9414,7 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M142" t="inlineStr">
@@ -7226,7 +9466,7 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M143" t="inlineStr">
@@ -7278,7 +9518,7 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M144" t="inlineStr">
@@ -7330,7 +9570,7 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M145" t="inlineStr">
@@ -7382,7 +9622,7 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M146" t="inlineStr">
@@ -7434,7 +9674,7 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M147" t="inlineStr">
@@ -7538,7 +9778,7 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M149" t="inlineStr">
@@ -7590,7 +9830,7 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M150" t="inlineStr">
@@ -7642,7 +9882,7 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M151" t="inlineStr">
@@ -7684,7 +9924,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -7729,6 +9969,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>Parafuso</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Screw</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Tornillo</t>
+        </is>
+      </c>
+      <c r="H153" t="inlineStr">
+        <is>
+          <t>Schraube</t>
+        </is>
+      </c>
       <c r="I153" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -7741,7 +10001,7 @@
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>EL</t>
+          <t>PA</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
@@ -7788,7 +10048,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -7840,7 +10100,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -7902,7 +10162,7 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M156" t="inlineStr">
@@ -7954,7 +10214,7 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>PCP</t>
         </is>
       </c>
       <c r="M157" t="inlineStr">
@@ -7989,6 +10249,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H158" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I158" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8095,6 +10375,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>Junta de anillo</t>
+        </is>
+      </c>
+      <c r="H161" t="inlineStr">
+        <is>
+          <t>Ringgelenk</t>
+        </is>
+      </c>
       <c r="I161" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -8107,7 +10407,7 @@
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>SAE1045</t>
+          <t>SAE4140</t>
         </is>
       </c>
       <c r="L161" t="inlineStr">
@@ -8147,6 +10447,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>Junta de anillo</t>
+        </is>
+      </c>
+      <c r="H162" t="inlineStr">
+        <is>
+          <t>Ringgelenk</t>
+        </is>
+      </c>
       <c r="I162" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -8159,7 +10479,7 @@
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>SAE1045</t>
+          <t>SAE4140</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
@@ -8199,6 +10519,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>Luva Rotor</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>Rotor Sleeve</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>Guante de rotor</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>Rotor-Handschuh</t>
+        </is>
+      </c>
       <c r="I163" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8216,7 +10556,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>299</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
@@ -8251,6 +10591,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>Luva Rotor</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>Rotor Sleeve</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>Guante de rotor</t>
+        </is>
+      </c>
+      <c r="H164" t="inlineStr">
+        <is>
+          <t>Rotor-Handschuh</t>
+        </is>
+      </c>
       <c r="I164" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8303,6 +10663,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H165" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I165" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8355,6 +10735,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>Junta de anillo</t>
+        </is>
+      </c>
+      <c r="H166" t="inlineStr">
+        <is>
+          <t>Ringgelenk</t>
+        </is>
+      </c>
       <c r="I166" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -8407,6 +10807,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H167" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I167" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8459,6 +10879,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H168" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I168" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8511,6 +10951,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H169" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I169" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8563,6 +11023,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H170" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I170" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8615,6 +11095,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H171" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I171" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8667,6 +11167,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I172" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8719,6 +11239,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H173" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I173" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8771,6 +11311,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H174" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I174" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8823,6 +11383,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H175" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I175" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8875,6 +11455,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H176" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I176" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8927,6 +11527,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H177" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I177" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -8934,7 +11554,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>40</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -8979,6 +11599,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H178" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I178" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9031,6 +11671,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H179" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I179" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9083,6 +11743,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>Borracha</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>Rubber</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>Caucho</t>
+        </is>
+      </c>
+      <c r="H180" t="inlineStr">
+        <is>
+          <t>Gummi</t>
+        </is>
+      </c>
       <c r="I180" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9135,6 +11815,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>Junta de anillo</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>Ringgelenk</t>
+        </is>
+      </c>
       <c r="I181" t="inlineStr">
         <is>
           <t>PCP-BOP</t>
@@ -9187,6 +11887,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>Ring Joint</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>Junta de anillo</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>Ringgelenk</t>
+        </is>
+      </c>
       <c r="I182" t="inlineStr">
         <is>
           <t>PCP-NDH</t>
@@ -9239,6 +11959,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>Pino Stop</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>Stop Pin</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>Pin de tope</t>
+        </is>
+      </c>
+      <c r="H183" t="inlineStr">
+        <is>
+          <t>Anschlagstift</t>
+        </is>
+      </c>
       <c r="I183" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9291,6 +12031,26 @@
           <t>NDB</t>
         </is>
       </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>Luva Rotor</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Rotor Sleeve</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>Guante de rotor</t>
+        </is>
+      </c>
+      <c r="H184" t="inlineStr">
+        <is>
+          <t>Rotor-Handschuh</t>
+        </is>
+      </c>
       <c r="I184" t="inlineStr">
         <is>
           <t>PCP-P</t>
@@ -9298,7 +12058,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>5.1/2"</t>
+          <t>4.1/2"</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -9341,6 +12101,26 @@
       <c r="D185" t="inlineStr">
         <is>
           <t>NDB</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>Suporte Base Motora</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Motor Base Bracket</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>Soporte de base de motor</t>
+        </is>
+      </c>
+      <c r="H185" t="inlineStr">
+        <is>
+          <t>Halterung für Motorsockel</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">

</xml_diff>

<commit_message>
Refactor README for clarity on main app runner location, remove unneeded dependencies from requirements, and clean up unused code in various modules.
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -1581,7 +1581,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>3.1/2"</t>
+          <t>2.7/8"</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>3.1/2"</t>
+          <t>2.7/8"</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>3.1/2"</t>
+          <t>2.7/8"</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>ROTOR</t>
+          <t>V-630</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -2787,7 +2787,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>1.1/8"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>3000 PSI</t>
+          <t>2000 PSI</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>SPECIAL</t>
+          <t>NETZSCH</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -5522,7 +5522,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>P5</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>06</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -5733,7 +5733,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>NTZ 400</t>
+          <t>NETZSCH</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -5800,7 +5800,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>NTZ 400</t>
+          <t>NETZSCH</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -6527,7 +6527,7 @@
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>P8</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -7465,7 +7465,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>EL</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -7604,7 +7604,7 @@
       </c>
       <c r="J112" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K112" t="inlineStr">
@@ -7676,7 +7676,7 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
@@ -7748,7 +7748,7 @@
       </c>
       <c r="J114" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K114" t="inlineStr">
@@ -7892,7 +7892,7 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>1/2"</t>
+          <t>7/8"</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
@@ -8884,7 +8884,7 @@
       </c>
       <c r="J132" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K132" t="inlineStr">
@@ -9144,7 +9144,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>70</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -9924,7 +9924,7 @@
       </c>
       <c r="J152" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K152" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>PA</t>
+          <t>EL</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
@@ -10048,7 +10048,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -10100,7 +10100,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>15</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -10402,7 +10402,7 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>1.1/4"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -10412,7 +10412,7 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>API 6A</t>
+          <t>API 5B</t>
         </is>
       </c>
       <c r="M161" t="inlineStr">
@@ -10474,7 +10474,7 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>1.1/4"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
@@ -10484,7 +10484,7 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>API 6A</t>
+          <t>API 5B</t>
         </is>
       </c>
       <c r="M162" t="inlineStr">
@@ -10546,7 +10546,7 @@
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>90</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -10556,7 +10556,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>299</t>
+          <t>NTZ</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>1.1/4"</t>
+          <t>2.7/8"</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -10772,7 +10772,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>API 6A</t>
+          <t>API 5B</t>
         </is>
       </c>
       <c r="M166" t="inlineStr">
@@ -11554,7 +11554,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -11842,7 +11842,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>1.1/4"</t>
+          <t>2.7/8"</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -11852,7 +11852,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>API 6A</t>
+          <t>API 5B</t>
         </is>
       </c>
       <c r="M181" t="inlineStr">
@@ -11924,7 +11924,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>NE</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="M182" t="inlineStr">
@@ -12058,7 +12058,7 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>4.1/2"</t>
+          <t>5.1/2"</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">

</xml_diff>

<commit_message>
Add execution report generation and enhance internal comment statistics
- Introduced a report generation feature that logs execution details in `logs/relatorio_execucao.json`.
- Enhanced the internal comment insertion logic to accurately count filled entries, considering empty and 'nan' values.
- Updated README to document the new report feature.
</commit_message>
<xml_diff>
--- a/planilhas/planilha_atualizada.xlsx
+++ b/planilhas/planilha_atualizada.xlsx
@@ -1581,7 +1581,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>3.1/2"</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -4282,7 +4282,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>2000 PSI</t>
+          <t>3000 PSI</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>SPECIAL</t>
         </is>
       </c>
       <c r="M68" t="inlineStr">
@@ -5522,7 +5522,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -5589,7 +5589,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -5733,7 +5733,7 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>NTZ 400</t>
         </is>
       </c>
       <c r="M84" t="inlineStr">
@@ -5800,7 +5800,7 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>NETZSCH</t>
+          <t>NTZ 400</t>
         </is>
       </c>
       <c r="M85" t="inlineStr">
@@ -5867,7 +5867,7 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>NTZ 278</t>
+          <t>NETZSCH</t>
         </is>
       </c>
       <c r="M86" t="inlineStr">
@@ -6956,7 +6956,7 @@
       </c>
       <c r="J103" t="inlineStr">
         <is>
-          <t>P8</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K103" t="inlineStr">
@@ -7465,7 +7465,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>EL</t>
+          <t>CI</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -8525,7 +8525,7 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="L125" t="inlineStr">
@@ -8577,7 +8577,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L126" t="inlineStr">
@@ -8629,7 +8629,7 @@
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L127" t="inlineStr">
@@ -8733,7 +8733,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L129" t="inlineStr">
@@ -8785,7 +8785,7 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L130" t="inlineStr">
@@ -8837,7 +8837,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L131" t="inlineStr">
@@ -8889,7 +8889,7 @@
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L133" t="inlineStr">
@@ -9097,7 +9097,7 @@
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L136" t="inlineStr">
@@ -9144,7 +9144,7 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>70</t>
+          <t>90</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
@@ -9201,7 +9201,7 @@
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L138" t="inlineStr">
@@ -9253,7 +9253,7 @@
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L139" t="inlineStr">
@@ -9305,7 +9305,7 @@
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L140" t="inlineStr">
@@ -9357,7 +9357,7 @@
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L141" t="inlineStr">
@@ -9513,7 +9513,7 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="L144" t="inlineStr">
@@ -9565,7 +9565,7 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L145" t="inlineStr">
@@ -9617,7 +9617,7 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L146" t="inlineStr">
@@ -9669,7 +9669,7 @@
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L147" t="inlineStr">
@@ -9877,7 +9877,7 @@
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>SS</t>
         </is>
       </c>
       <c r="L151" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>EL</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="L153" t="inlineStr">
@@ -10048,7 +10048,7 @@
       </c>
       <c r="J154" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>30</t>
         </is>
       </c>
       <c r="K154" t="inlineStr">
@@ -10100,7 +10100,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>20</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -10157,7 +10157,7 @@
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>SS</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L156" t="inlineStr">
@@ -10209,7 +10209,7 @@
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>St</t>
         </is>
       </c>
       <c r="L157" t="inlineStr">
@@ -10402,17 +10402,17 @@
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>3.1/2"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>SAE4140</t>
+          <t>SAE1045</t>
         </is>
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>API 5B</t>
+          <t>API 6A</t>
         </is>
       </c>
       <c r="M161" t="inlineStr">
@@ -10474,17 +10474,17 @@
       </c>
       <c r="J162" t="inlineStr">
         <is>
-          <t>3.1/2"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>SAE4140</t>
+          <t>SAE1045</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>API 5B</t>
+          <t>API 6A</t>
         </is>
       </c>
       <c r="M162" t="inlineStr">
@@ -10556,7 +10556,7 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>NTZ</t>
+          <t>299</t>
         </is>
       </c>
       <c r="M163" t="inlineStr">
@@ -10762,7 +10762,7 @@
       </c>
       <c r="J166" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K166" t="inlineStr">
@@ -10772,7 +10772,7 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>API 5B</t>
+          <t>API 6A</t>
         </is>
       </c>
       <c r="M166" t="inlineStr">
@@ -11554,7 +11554,7 @@
       </c>
       <c r="J177" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>27</t>
         </is>
       </c>
       <c r="K177" t="inlineStr">
@@ -11842,7 +11842,7 @@
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>2.7/8"</t>
+          <t>1.1/4"</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -11852,7 +11852,7 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>API 5B</t>
+          <t>API 6A</t>
         </is>
       </c>
       <c r="M181" t="inlineStr">
@@ -11924,7 +11924,7 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>NE</t>
         </is>
       </c>
       <c r="M182" t="inlineStr">
@@ -12058,12 +12058,12 @@
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>5.1/2"</t>
+          <t>4.1/2"</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>ROTOR</t>
+          <t>GGG50</t>
         </is>
       </c>
       <c r="L184" t="inlineStr">

</xml_diff>